<commit_message>
JsonToArray handling more complex cases
</commit_message>
<xml_diff>
--- a/JsonExcel/doc/JsonExcel-test.xlsx
+++ b/JsonExcel/doc/JsonExcel-test.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="P:\JsonExcel\JsonExcel\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28A157A5-9DC0-46D6-B2A6-2C158323E807}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{678E5B05-37B1-42C6-9244-ABFB9E2948E2}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18885" windowHeight="5910" xr2:uid="{90F70DC4-6E6D-491C-88DA-FF972DBF519E}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18885" windowHeight="5910" activeTab="1" xr2:uid="{90F70DC4-6E6D-491C-88DA-FF972DBF519E}"/>
   </bookViews>
   <sheets>
     <sheet name="Simple Json" sheetId="1" r:id="rId1"/>
+    <sheet name="complex" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="JSON">'Simple Json'!$M$2</definedName>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>bbb</t>
   </si>
@@ -56,18 +57,111 @@
   <si>
     <t>Vertical Orientation</t>
   </si>
+  <si>
+    <t>{"web-app": {
+  "servlet": [   
+    {
+      "servlet-name": "cofaxCDS",
+      "servlet-class": "org.cofax.cds.CDSServlet",
+      "init-param": {
+        "configGlossary:installationAt": "Philadelphia, PA",
+        "configGlossary:adminEmail": "ksm@pobox.com",
+        "configGlossary:poweredBy": "Cofax",
+        "configGlossary:poweredByIcon": "/images/cofax.gif",
+        "configGlossary:staticPath": "/content/static",
+        "templateProcessorClass": "org.cofax.WysiwygTemplate",
+        "templateLoaderClass": "org.cofax.FilesTemplateLoader",
+        "templatePath": "templates",
+        "templateOverridePath": "",
+        "defaultListTemplate": "listTemplate.htm",
+        "defaultFileTemplate": "articleTemplate.htm",
+        "useJSP": false,
+        "jspListTemplate": "listTemplate.jsp",
+        "jspFileTemplate": "articleTemplate.jsp",
+        "cachePackageTagsTrack": 200,
+        "cachePackageTagsStore": 200,
+        "cachePackageTagsRefresh": 60,
+        "cacheTemplatesTrack": 100,
+        "cacheTemplatesStore": 50,
+        "cacheTemplatesRefresh": 15,
+        "cachePagesTrack": 200,
+        "cachePagesStore": 100,
+        "cachePagesRefresh": 10,
+        "cachePagesDirtyRead": 10,
+        "searchEngineListTemplate": "forSearchEnginesList.htm",
+        "searchEngineFileTemplate": "forSearchEngines.htm",
+        "searchEngineRobotsDb": "WEB-INF/robots.db",
+        "useDataStore": true,
+        "dataStoreClass": "org.cofax.SqlDataStore",
+        "redirectionClass": "org.cofax.SqlRedirection",
+        "dataStoreName": "cofax",
+        "dataStoreDriver": "com.microsoft.jdbc.sqlserver.SQLServerDriver",
+        "dataStoreUrl": "jdbc:microsoft:sqlserver://LOCALHOST:1433;DatabaseName=goon",
+        "dataStoreUser": "sa",
+        "dataStorePassword": "dataStoreTestQuery",
+        "dataStoreTestQuery": "SET NOCOUNT ON;select test='test';",
+        "dataStoreLogFile": "/usr/local/tomcat/logs/datastore.log",
+        "dataStoreInitConns": 10,
+        "dataStoreMaxConns": 100,
+        "dataStoreConnUsageLimit": 100,
+        "dataStoreLogLevel": "debug",
+        "maxUrlLength": 500}},
+    {
+      "servlet-name": "cofaxEmail",
+      "servlet-class": "org.cofax.cds.EmailServlet",
+      "init-param": {
+      "mailHost": "mail1",
+      "mailHostOverride": "mail2"}},
+    {
+      "servlet-name": "cofaxAdmin",
+      "servlet-class": "org.cofax.cds.AdminServlet"},
+    {
+      "servlet-name": "fileServlet",
+      "servlet-class": "org.cofax.cds.FileServlet"},
+    {
+      "servlet-name": "cofaxTools",
+      "servlet-class": "org.cofax.cms.CofaxToolsServlet",
+      "init-param": {
+        "templatePath": "toolstemplates/",
+        "log": 1,
+        "logLocation": "/usr/local/tomcat/logs/CofaxTools.log",
+        "logMaxSize": "",
+        "dataLog": 1,
+        "dataLogLocation": "/usr/local/tomcat/logs/dataLog.log",
+        "dataLogMaxSize": "",
+        "removePageCache": "/content/admin/remove?cache=pages&amp;id=",
+        "removeTemplateCache": "/content/admin/remove?cache=templates&amp;id=",
+        "fileTransferFolder": "/usr/local/tomcat/webapps/content/fileTransferFolder",
+        "lookInContext": 1,
+        "adminGroupID": 4,
+        "betaServer": true}}],
+  "servlet-mapping": {
+    "cofaxCDS": "/",
+    "cofaxEmail": "/cofaxutil/aemail/*",
+    "cofaxAdmin": "/admin/*",
+    "fileServlet": "/static/*",
+    "cofaxTools": "/tools/*"},
+  "taglib": {
+    "taglib-uri": "cofax.tld",
+    "taglib-location": "/WEB-INF/tlds/cofax.tld"}}}</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial Unicode MS"/>
     </font>
   </fonts>
   <fills count="2">
@@ -90,9 +184,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -409,13 +510,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3DB9AC6D-111D-443E-9E75-E3C0D374BD0F}">
   <dimension ref="C1:M14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="N5" sqref="N5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="3:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="3:13">
       <c r="C1" t="s">
         <v>8</v>
       </c>
@@ -423,7 +524,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="3:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="3:13">
       <c r="L2" t="s">
         <v>6</v>
       </c>
@@ -432,7 +533,7 @@
         <v>{ 'aaaa': 123,'bbb': 456,3: 789}</v>
       </c>
     </row>
-    <row r="4" spans="3:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="3:13">
       <c r="C4" s="1" t="s">
         <v>1</v>
       </c>
@@ -443,7 +544,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="3:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="3:13">
       <c r="C5" t="str">
         <f t="array" ref="C5:E8">_xll.JsonToArray(JSON)</f>
         <v>aaaa</v>
@@ -469,7 +570,7 @@
         <v>{"aaaa":123.0,"bbb":456.0,"3":789.0}</v>
       </c>
     </row>
-    <row r="6" spans="3:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="3:13">
       <c r="C6" t="str">
         <v>bbb</v>
       </c>
@@ -489,7 +590,7 @@
         <v>789</v>
       </c>
     </row>
-    <row r="7" spans="3:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="3:13">
       <c r="C7" t="str">
         <v>3</v>
       </c>
@@ -509,7 +610,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="8" spans="3:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="3:13">
       <c r="C8" t="e">
         <v>#N/A</v>
       </c>
@@ -529,13 +630,13 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="11" spans="3:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="3:13">
       <c r="C11" s="1" t="s">
         <v>2</v>
       </c>
       <c r="G11" s="1"/>
     </row>
-    <row r="12" spans="3:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="3:13">
       <c r="C12" t="s">
         <v>0</v>
       </c>
@@ -544,7 +645,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="13" spans="3:13" x14ac:dyDescent="0.25">
+    <row r="13" spans="3:13">
       <c r="C13" t="s">
         <v>3</v>
       </c>
@@ -553,7 +654,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="14" spans="3:13" x14ac:dyDescent="0.25">
+    <row r="14" spans="3:13">
       <c r="C14">
         <v>3</v>
       </c>
@@ -565,4 +666,506 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{476E53B7-47D8-4C73-9AFD-D21323878C5A}">
+  <dimension ref="B1:E89"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3:E37"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="2" width="85.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:5">
+      <c r="B1" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="2:5">
+      <c r="B2" s="4"/>
+    </row>
+    <row r="3" spans="2:5">
+      <c r="B3" s="4"/>
+      <c r="D3" t="str">
+        <f t="array" ref="D3:E37">_xll.JsonToArray(B1)</f>
+        <v>web-app.servlet[0].servlet-name</v>
+      </c>
+      <c r="E3" t="str">
+        <v>cofaxCDS</v>
+      </c>
+    </row>
+    <row r="4" spans="2:5">
+      <c r="B4" s="4"/>
+      <c r="D4" t="str">
+        <v>web-app.servlet[0].servlet-class</v>
+      </c>
+      <c r="E4" t="str">
+        <v>org.cofax.cds.CDSServlet</v>
+      </c>
+    </row>
+    <row r="5" spans="2:5">
+      <c r="B5" s="4"/>
+      <c r="D5" t="str">
+        <v>web-app.servlet[0].init-param.configGlossary:installationAt</v>
+      </c>
+      <c r="E5" t="str">
+        <v>Philadelphia, PA</v>
+      </c>
+    </row>
+    <row r="6" spans="2:5">
+      <c r="B6" s="4"/>
+      <c r="D6" t="str">
+        <v>web-app.servlet[0].init-param.configGlossary:adminEmail</v>
+      </c>
+      <c r="E6" t="str">
+        <v>ksm@pobox.com</v>
+      </c>
+    </row>
+    <row r="7" spans="2:5">
+      <c r="B7" s="4"/>
+      <c r="D7" t="str">
+        <v>web-app.servlet[0].init-param.configGlossary:poweredBy</v>
+      </c>
+      <c r="E7" t="str">
+        <v>Cofax</v>
+      </c>
+    </row>
+    <row r="8" spans="2:5">
+      <c r="B8" s="4"/>
+      <c r="D8" t="str">
+        <v>web-app.servlet[0].init-param.configGlossary:poweredByIcon</v>
+      </c>
+      <c r="E8" t="str">
+        <v>/images/cofax.gif</v>
+      </c>
+    </row>
+    <row r="9" spans="2:5">
+      <c r="B9" s="4"/>
+      <c r="D9" t="str">
+        <v>web-app.servlet[0].init-param.configGlossary:staticPath</v>
+      </c>
+      <c r="E9" t="str">
+        <v>/content/static</v>
+      </c>
+    </row>
+    <row r="10" spans="2:5">
+      <c r="B10" s="4"/>
+      <c r="D10" t="str">
+        <v>web-app.servlet[0].init-param.templateProcessorClass</v>
+      </c>
+      <c r="E10" t="str">
+        <v>org.cofax.WysiwygTemplate</v>
+      </c>
+    </row>
+    <row r="11" spans="2:5">
+      <c r="B11" s="4"/>
+      <c r="D11" t="str">
+        <v>web-app.servlet[0].init-param.templateLoaderClass</v>
+      </c>
+      <c r="E11" t="str">
+        <v>org.cofax.FilesTemplateLoader</v>
+      </c>
+    </row>
+    <row r="12" spans="2:5">
+      <c r="B12" s="4"/>
+      <c r="D12" t="str">
+        <v>web-app.servlet[0].init-param.templatePath</v>
+      </c>
+      <c r="E12" t="str">
+        <v>templates</v>
+      </c>
+    </row>
+    <row r="13" spans="2:5">
+      <c r="B13" s="4"/>
+      <c r="D13" t="str">
+        <v>web-app.servlet[0].init-param.templateOverridePath</v>
+      </c>
+      <c r="E13" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="14" spans="2:5">
+      <c r="B14" s="4"/>
+      <c r="D14" t="str">
+        <v>web-app.servlet[0].init-param.defaultListTemplate</v>
+      </c>
+      <c r="E14" t="str">
+        <v>listTemplate.htm</v>
+      </c>
+    </row>
+    <row r="15" spans="2:5">
+      <c r="B15" s="4"/>
+      <c r="D15" t="str">
+        <v>web-app.servlet[0].init-param.defaultFileTemplate</v>
+      </c>
+      <c r="E15" t="str">
+        <v>articleTemplate.htm</v>
+      </c>
+    </row>
+    <row r="16" spans="2:5">
+      <c r="B16" s="4"/>
+      <c r="D16" t="str">
+        <v>web-app.servlet[0].init-param.useJSP</v>
+      </c>
+      <c r="E16" t="str">
+        <v>False</v>
+      </c>
+    </row>
+    <row r="17" spans="2:5">
+      <c r="B17" s="4"/>
+      <c r="D17" t="str">
+        <v>web-app.servlet[0].init-param.jspListTemplate</v>
+      </c>
+      <c r="E17" t="str">
+        <v>listTemplate.jsp</v>
+      </c>
+    </row>
+    <row r="18" spans="2:5">
+      <c r="B18" s="4"/>
+      <c r="D18" t="str">
+        <v>web-app.servlet[0].init-param.jspFileTemplate</v>
+      </c>
+      <c r="E18" t="str">
+        <v>articleTemplate.jsp</v>
+      </c>
+    </row>
+    <row r="19" spans="2:5">
+      <c r="B19" s="4"/>
+      <c r="D19" t="str">
+        <v>web-app.servlet[0].init-param.cachePackageTagsTrack</v>
+      </c>
+      <c r="E19" t="str">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="20" spans="2:5">
+      <c r="B20" s="4"/>
+      <c r="D20" t="str">
+        <v>web-app.servlet[0].init-param.cachePackageTagsStore</v>
+      </c>
+      <c r="E20" t="str">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="21" spans="2:5">
+      <c r="B21" s="4"/>
+      <c r="D21" t="str">
+        <v>web-app.servlet[0].init-param.cachePackageTagsRefresh</v>
+      </c>
+      <c r="E21" t="str">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="22" spans="2:5">
+      <c r="B22" s="4"/>
+      <c r="D22" t="str">
+        <v>web-app.servlet[0].init-param.cacheTemplatesTrack</v>
+      </c>
+      <c r="E22" t="str">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="23" spans="2:5">
+      <c r="B23" s="4"/>
+      <c r="D23" t="str">
+        <v>web-app.servlet[0].init-param.cacheTemplatesStore</v>
+      </c>
+      <c r="E23" t="str">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="24" spans="2:5">
+      <c r="B24" s="4"/>
+      <c r="D24" t="str">
+        <v>web-app.servlet[0].init-param.cacheTemplatesRefresh</v>
+      </c>
+      <c r="E24" t="str">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="25" spans="2:5">
+      <c r="B25" s="4"/>
+      <c r="D25" t="str">
+        <v>web-app.servlet[0].init-param.cachePagesTrack</v>
+      </c>
+      <c r="E25" t="str">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="26" spans="2:5">
+      <c r="B26" s="4"/>
+      <c r="D26" t="str">
+        <v>web-app.servlet[0].init-param.cachePagesStore</v>
+      </c>
+      <c r="E26" t="str">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="27" spans="2:5">
+      <c r="B27" s="4"/>
+      <c r="D27" t="str">
+        <v>web-app.servlet[0].init-param.cachePagesRefresh</v>
+      </c>
+      <c r="E27" t="str">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="28" spans="2:5">
+      <c r="B28" s="4"/>
+      <c r="D28" t="str">
+        <v>web-app.servlet[0].init-param.cachePagesDirtyRead</v>
+      </c>
+      <c r="E28" t="str">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="29" spans="2:5">
+      <c r="B29" s="4"/>
+      <c r="D29" t="str">
+        <v>web-app.servlet[0].init-param.searchEngineListTemplate</v>
+      </c>
+      <c r="E29" t="str">
+        <v>forSearchEnginesList.htm</v>
+      </c>
+    </row>
+    <row r="30" spans="2:5">
+      <c r="B30" s="4"/>
+      <c r="D30" t="str">
+        <v>web-app.servlet[0].init-param.searchEngineFileTemplate</v>
+      </c>
+      <c r="E30" t="str">
+        <v>forSearchEngines.htm</v>
+      </c>
+    </row>
+    <row r="31" spans="2:5">
+      <c r="B31" s="4"/>
+      <c r="D31" t="str">
+        <v>web-app.servlet[0].init-param.searchEngineRobotsDb</v>
+      </c>
+      <c r="E31" t="str">
+        <v>WEB-INF/robots.db</v>
+      </c>
+    </row>
+    <row r="32" spans="2:5">
+      <c r="B32" s="4"/>
+      <c r="D32" t="str">
+        <v>web-app.servlet[0].init-param.useDataStore</v>
+      </c>
+      <c r="E32" t="str">
+        <v>True</v>
+      </c>
+    </row>
+    <row r="33" spans="2:5">
+      <c r="B33" s="4"/>
+      <c r="D33" t="str">
+        <v>web-app.servlet[0].init-param.dataStoreClass</v>
+      </c>
+      <c r="E33" t="str">
+        <v>org.cofax.SqlDataStore</v>
+      </c>
+    </row>
+    <row r="34" spans="2:5">
+      <c r="B34" s="4"/>
+      <c r="D34" t="str">
+        <v>web-app.servlet[0].init-param.redirectionClass</v>
+      </c>
+      <c r="E34" t="str">
+        <v>org.cofax.SqlRedirection</v>
+      </c>
+    </row>
+    <row r="35" spans="2:5">
+      <c r="B35" s="4"/>
+      <c r="D35" t="str">
+        <v>web-app.servlet[0].init-param.dataStoreName</v>
+      </c>
+      <c r="E35" t="str">
+        <v>cofax</v>
+      </c>
+    </row>
+    <row r="36" spans="2:5">
+      <c r="B36" s="4"/>
+      <c r="D36" t="str">
+        <v>web-app.servlet[0].init-param.dataStoreDriver</v>
+      </c>
+      <c r="E36" t="str">
+        <v>com.microsoft.jdbc.sqlserver.SQLServerDriver</v>
+      </c>
+    </row>
+    <row r="37" spans="2:5">
+      <c r="B37" s="4"/>
+      <c r="D37" t="str">
+        <v>web-app.servlet[0].init-param.dataStoreUrl</v>
+      </c>
+      <c r="E37" t="str">
+        <v>jdbc:microsoft:sqlserver://LOCALHOST:1433;DatabaseName=goon</v>
+      </c>
+    </row>
+    <row r="38" spans="2:5">
+      <c r="B38" s="4"/>
+    </row>
+    <row r="39" spans="2:5">
+      <c r="B39" s="2"/>
+    </row>
+    <row r="40" spans="2:5">
+      <c r="B40" s="2"/>
+    </row>
+    <row r="41" spans="2:5">
+      <c r="B41" s="2"/>
+    </row>
+    <row r="42" spans="2:5">
+      <c r="B42" s="2"/>
+    </row>
+    <row r="43" spans="2:5">
+      <c r="B43" s="2"/>
+    </row>
+    <row r="44" spans="2:5">
+      <c r="B44" s="2"/>
+    </row>
+    <row r="45" spans="2:5">
+      <c r="B45" s="2"/>
+    </row>
+    <row r="46" spans="2:5">
+      <c r="B46" s="2"/>
+    </row>
+    <row r="47" spans="2:5">
+      <c r="B47" s="2"/>
+    </row>
+    <row r="48" spans="2:5">
+      <c r="B48" s="2"/>
+    </row>
+    <row r="49" spans="2:2">
+      <c r="B49" s="2"/>
+    </row>
+    <row r="50" spans="2:2">
+      <c r="B50" s="2"/>
+    </row>
+    <row r="51" spans="2:2">
+      <c r="B51" s="2"/>
+    </row>
+    <row r="52" spans="2:2">
+      <c r="B52" s="2"/>
+    </row>
+    <row r="53" spans="2:2">
+      <c r="B53" s="2"/>
+    </row>
+    <row r="54" spans="2:2">
+      <c r="B54" s="2"/>
+    </row>
+    <row r="55" spans="2:2">
+      <c r="B55" s="2"/>
+    </row>
+    <row r="56" spans="2:2">
+      <c r="B56" s="2"/>
+    </row>
+    <row r="57" spans="2:2">
+      <c r="B57" s="2"/>
+    </row>
+    <row r="58" spans="2:2">
+      <c r="B58" s="2"/>
+    </row>
+    <row r="59" spans="2:2">
+      <c r="B59" s="2"/>
+    </row>
+    <row r="60" spans="2:2">
+      <c r="B60" s="2"/>
+    </row>
+    <row r="61" spans="2:2">
+      <c r="B61" s="2"/>
+    </row>
+    <row r="62" spans="2:2">
+      <c r="B62" s="2"/>
+    </row>
+    <row r="63" spans="2:2">
+      <c r="B63" s="2"/>
+    </row>
+    <row r="64" spans="2:2">
+      <c r="B64" s="2"/>
+    </row>
+    <row r="65" spans="2:2">
+      <c r="B65" s="2"/>
+    </row>
+    <row r="66" spans="2:2">
+      <c r="B66" s="2"/>
+    </row>
+    <row r="67" spans="2:2">
+      <c r="B67" s="2"/>
+    </row>
+    <row r="68" spans="2:2">
+      <c r="B68" s="2"/>
+    </row>
+    <row r="69" spans="2:2">
+      <c r="B69" s="2"/>
+    </row>
+    <row r="70" spans="2:2">
+      <c r="B70" s="2"/>
+    </row>
+    <row r="71" spans="2:2">
+      <c r="B71" s="2"/>
+    </row>
+    <row r="72" spans="2:2">
+      <c r="B72" s="2"/>
+    </row>
+    <row r="73" spans="2:2">
+      <c r="B73" s="2"/>
+    </row>
+    <row r="74" spans="2:2">
+      <c r="B74" s="2"/>
+    </row>
+    <row r="75" spans="2:2">
+      <c r="B75" s="2"/>
+    </row>
+    <row r="76" spans="2:2">
+      <c r="B76" s="2"/>
+    </row>
+    <row r="77" spans="2:2">
+      <c r="B77" s="2"/>
+    </row>
+    <row r="78" spans="2:2">
+      <c r="B78" s="2"/>
+    </row>
+    <row r="79" spans="2:2">
+      <c r="B79" s="2"/>
+    </row>
+    <row r="80" spans="2:2">
+      <c r="B80" s="2"/>
+    </row>
+    <row r="81" spans="2:2">
+      <c r="B81" s="2"/>
+    </row>
+    <row r="82" spans="2:2">
+      <c r="B82" s="2"/>
+    </row>
+    <row r="83" spans="2:2">
+      <c r="B83" s="2"/>
+    </row>
+    <row r="84" spans="2:2">
+      <c r="B84" s="2"/>
+    </row>
+    <row r="85" spans="2:2">
+      <c r="B85" s="2"/>
+    </row>
+    <row r="86" spans="2:2">
+      <c r="B86" s="2"/>
+    </row>
+    <row r="87" spans="2:2">
+      <c r="B87" s="2"/>
+    </row>
+    <row r="88" spans="2:2">
+      <c r="B88" s="2"/>
+    </row>
+    <row r="89" spans="2:2">
+      <c r="B89" s="2"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B1:B38"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
convert to natives types
</commit_message>
<xml_diff>
--- a/JsonExcel/doc/JsonExcel-test.xlsx
+++ b/JsonExcel/doc/JsonExcel-test.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="P:\OpenSource\JsonExcel\JsonExcel\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D042300-4DF9-41F4-A81C-83307EF0FCE5}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FADF5517-D98D-44FD-8217-BDDA2BA921CF}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18885" windowHeight="5910" activeTab="1" xr2:uid="{90F70DC4-6E6D-491C-88DA-FF972DBF519E}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18885" windowHeight="5910" activeTab="2" xr2:uid="{90F70DC4-6E6D-491C-88DA-FF972DBF519E}"/>
   </bookViews>
   <sheets>
     <sheet name="Simple Json" sheetId="1" r:id="rId1"/>
     <sheet name="complex" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="JSON">'Simple Json'!$M$2</definedName>
@@ -29,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>bbb</t>
   </si>
@@ -145,11 +146,17 @@
     "taglib-uri": "cofax.tld",
     "taglib-location": "/WEB-INF/tlds/cofax.tld"}}}</t>
   </si>
+  <si>
+    <t>{"Model":"SMA","TargetTime":"2018-07-09T21:29:00Z","Data":{"2018-07-09T19:56:00Z":6711.49300000,"2018-07-09T19:57:00Z":6711.92000000,"2018-07-09T19:58:00Z":6712.53200000,"2018-07-09T19:59:00Z":6712.43100000,"2018-07-09T20:00:00Z":6711.93400000,"2018-07-09T20:01:00Z":6712.13100000,"2018-07-09T20:02:00Z":6711.98100000,"2018-07-09T20:03:00Z":6711.78100000,"2018-07-09T20:04:00Z":6711.58600000,"2018-07-09T20:05:00Z":6711.13900000,"2018-07-09T20:06:00Z":6710.86200000,"2018-07-09T20:07:00Z":6710.37000000,"2018-07-09T20:08:00Z":6709.85000000,"2018-07-09T20:09:00Z":6709.28700000,"2018-07-09T20:10:00Z":6709.27600000,"2018-07-09T20:11:00Z":6708.48100000,"2018-07-09T20:12:00Z":6707.57700000,"2018-07-09T20:13:00Z":6706.42600000,"2018-07-09T20:14:00Z":6705.26200000,"2018-07-09T20:15:00Z":6704.55500000,"2018-07-09T20:16:00Z":6703.43500000,"2018-07-09T20:17:00Z":6702.49900000,"2018-07-09T20:18:00Z":6701.40600000,"2018-07-09T20:19:00Z":6700.76400000,"2018-07-09T20:20:00Z":6700.17200000,"2018-07-09T20:21:00Z":6700.06800000,"2018-07-09T20:22:00Z":6700.36900000,"2018-07-09T20:23:00Z":6701.09100000,"2018-07-09T20:24:00Z":6701.53800000,"2018-07-09T20:25:00Z":6701.73800000,"2018-07-09T20:26:00Z":6702.11900000,"2018-07-09T20:27:00Z":6702.61900000,"2018-07-09T20:28:00Z":6703.01400000,"2018-07-09T20:29:00Z":6703.00000000,"2018-07-09T20:30:00Z":6702.89900000,"2018-07-09T20:31:00Z":6702.82200000,"2018-07-09T20:32:00Z":6703.14600000,"2018-07-09T20:33:00Z":6702.99600000,"2018-07-09T20:34:00Z":6703.11900000,"2018-07-09T20:35:00Z":6703.50100000,"2018-07-09T20:36:00Z":6703.49700000,"2018-07-09T20:37:00Z":6703.83100000,"2018-07-09T20:38:00Z":6703.92700000,"2018-07-09T20:39:00Z":6704.30700000,"2018-07-09T20:40:00Z":6704.57100000,"2018-07-09T20:41:00Z":6705.04800000,"2018-07-09T20:42:00Z":6704.33200000,"2018-07-09T20:43:00Z":6703.92000000,"2018-07-09T20:44:00Z":6703.68500000,"2018-07-09T20:45:00Z":6703.19000000,"2018-07-09T20:46:00Z":6703.34500000,"2018-07-09T20:47:00Z":6703.20800000,"2018-07-09T20:48:00Z":6703.21800000,"2018-07-09T20:49:00Z":6703.05700000,"2018-07-09T20:50:00Z":6702.83600000,"2018-07-09T20:51:00Z":6702.37900000,"2018-07-09T20:52:00Z":6702.36800000,"2018-07-09T20:53:00Z":6702.28100000,"2018-07-09T20:54:00Z":6702.01700000,"2018-07-09T20:55:00Z":6701.85100000,"2018-07-09T20:56:00Z":6701.26000000,"2018-07-09T20:57:00Z":6700.68400000,"2018-07-09T20:58:00Z":6699.99900000,"2018-07-09T20:59:00Z":6699.60000000,"2018-07-09T21:00:00Z":6699.08700000,"2018-07-09T21:01:00Z":6698.74500000,"2018-07-09T21:02:00Z":6698.44900000,"2018-07-09T21:03:00Z":6698.29100000,"2018-07-09T21:04:00Z":6698.13300000,"2018-07-09T21:05:00Z":6697.73800000,"2018-07-09T21:06:00Z":6697.31900000,"2018-07-09T21:07:00Z":6697.16100000,"2018-07-09T21:08:00Z":6697.44500000,"2018-07-09T21:09:00Z":6697.44400000,"2018-07-09T21:10:00Z":6697.62000000,"2018-07-09T21:11:00Z":6697.61900000,"2018-07-09T21:12:00Z":6697.64200000,"2018-07-09T21:13:00Z":6697.60400000,"2018-07-09T21:14:00Z":6697.56500000,"2018-07-09T21:15:00Z":6698.03900000,"2018-07-09T21:16:00Z":6698.22900000,"2018-07-09T21:17:00Z":6698.15800000,"2018-07-09T21:18:00Z":6697.99500000,"2018-07-09T21:19:00Z":6698.07700000,"2018-07-09T21:20:00Z":6698.17400000,"2018-07-09T21:21:00Z":6698.57400000,"2018-07-09T21:22:00Z":6699.39700000,"2018-07-09T21:23:00Z":6700.54900000,"2018-07-09T21:24:00Z":6701.63300000,"2018-07-09T21:25:00Z":6702.44100000,"2018-07-09T21:26:00Z":6703.55400000,"2018-07-09T21:27:00Z":6704.66700000,"2018-07-09T21:28:00Z":6705.63800000,"2018-07-09T21:29:00Z":6706.43000000},"Inputs":{"PERIOD":10},"ModelStartTime":1531157418480.0,"ModelEndTime":1531157418480.0,"Interval":"OneMinute","Symbol":"BTCUSDT","Source":"BINANCE_KLINE.BTCUSDT.OneMinute"}</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="166" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
+  </numFmts>
   <fonts count="2">
     <font>
       <sz val="11"/>
@@ -184,7 +191,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -194,6 +201,7 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -209,6 +217,1162 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$C$7:$C$100</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="94"/>
+                <c:pt idx="0">
+                  <c:v>6711.4930000000004</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6711.92</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6712.5320000000002</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6712.4309999999996</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6711.9340000000002</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6712.1310000000003</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6711.9809999999998</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>6711.7809999999999</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>6711.5860000000002</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>6711.1390000000001</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>6710.8620000000001</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>6710.37</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>6709.85</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>6709.2870000000003</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>6709.2759999999998</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>6708.4809999999998</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>6707.5770000000002</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>6706.4260000000004</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>6705.2619999999997</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>6704.5550000000003</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>6703.4350000000004</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>6702.4989999999998</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>6701.4059999999999</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>6700.7640000000001</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>6700.1719999999996</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>6700.0680000000002</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>6700.3689999999997</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>6701.0910000000003</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>6701.5379999999996</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>6701.7380000000003</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>6702.1189999999997</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>6702.6189999999997</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>6703.0140000000001</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>6703</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>6702.8990000000003</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>6702.8220000000001</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>6703.1459999999997</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>6702.9960000000001</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>6703.1189999999997</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>6703.5010000000002</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>6703.4970000000003</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>6703.8310000000001</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>6703.9269999999997</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>6704.3069999999998</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>6704.5709999999999</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>6705.0479999999998</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>6704.3320000000003</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>6703.92</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>6703.6850000000004</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>6703.19</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>6703.3450000000003</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>6703.2079999999996</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>6703.2179999999998</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>6703.0569999999998</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>6702.8360000000002</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>6702.3789999999999</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>6702.3680000000004</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>6702.2809999999999</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>6702.0169999999998</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>6701.8509999999997</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>6701.26</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>6700.6840000000002</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>6699.9989999999998</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>6699.6</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>6699.0870000000004</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>6698.7449999999999</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>6698.4489999999996</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>6698.2910000000002</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>6698.1329999999998</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>6697.7380000000003</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>6697.3190000000004</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>6697.1610000000001</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>6697.4449999999997</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>6697.4440000000004</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>6697.62</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>6697.6189999999997</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>6697.6419999999998</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>6697.6040000000003</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>6697.5649999999996</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>6698.0389999999998</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>6698.2290000000003</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>6698.1580000000004</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>6697.9949999999999</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>6698.0770000000002</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>6698.174</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>6698.5739999999996</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>6699.3969999999999</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>6700.549</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>6701.6329999999998</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>6702.4409999999998</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>6703.5540000000001</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>6704.6670000000004</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>6705.6379999999999</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>6706.43</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-B36D-47CC-A124-6DF096C23507}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="470088656"/>
+        <c:axId val="470088328"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="470088656"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="470088328"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="470088328"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="470088656"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>533400</xdr:colOff>
+      <xdr:row>84</xdr:row>
+      <xdr:rowOff>23812</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
+      <xdr:row>98</xdr:row>
+      <xdr:rowOff>100012</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{569DF9AE-9BBB-4D55-9847-8505E1A947CC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -672,8 +1836,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{476E53B7-47D8-4C73-9AFD-D21323878C5A}">
   <dimension ref="A1:E89"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1721,4 +2885,1919 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{54B4FA4A-253A-4DC7-B007-BD642767BFAD}">
+  <dimension ref="A1:D161"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="B81" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7:C100"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="2" width="16.5703125" customWidth="1"/>
+    <col min="3" max="3" width="11.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" t="str">
+        <f t="array" ref="A5:B161">_xll.JsonToArray($A$1)</f>
+        <v>Model</v>
+      </c>
+      <c r="B5" t="str">
+        <v>SMA</v>
+      </c>
+      <c r="C5" t="str">
+        <f>_xll.JsonLookup($A$1,A5)</f>
+        <v>SMA</v>
+      </c>
+      <c r="D5" t="e">
+        <f>_xll.JsonLookup(A1, "Data")</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" t="str">
+        <v>TargetTime</v>
+      </c>
+      <c r="B6" t="str">
+        <v>7/9/2018 9:29:00 PM</v>
+      </c>
+      <c r="C6" s="5">
+        <f>_xll.JsonLookup($A$1,A6)</f>
+        <v>43290.895138888889</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" t="str">
+        <v>Data.2018-07-09T19:56:00Z</v>
+      </c>
+      <c r="B7" t="str">
+        <v>6711.493</v>
+      </c>
+      <c r="C7">
+        <f>_xll.JsonLookup($A$1,A7)</f>
+        <v>6711.4930000000004</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" t="str">
+        <v>Data.2018-07-09T19:57:00Z</v>
+      </c>
+      <c r="B8" t="str">
+        <v>6711.92</v>
+      </c>
+      <c r="C8">
+        <f>_xll.JsonLookup($A$1,A8)</f>
+        <v>6711.92</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" t="str">
+        <v>Data.2018-07-09T19:58:00Z</v>
+      </c>
+      <c r="B9" t="str">
+        <v>6712.532</v>
+      </c>
+      <c r="C9">
+        <f>_xll.JsonLookup($A$1,A9)</f>
+        <v>6712.5320000000002</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" t="str">
+        <v>Data.2018-07-09T19:59:00Z</v>
+      </c>
+      <c r="B10" t="str">
+        <v>6712.431</v>
+      </c>
+      <c r="C10">
+        <f>_xll.JsonLookup($A$1,A10)</f>
+        <v>6712.4309999999996</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" t="str">
+        <v>Data.2018-07-09T20:00:00Z</v>
+      </c>
+      <c r="B11" t="str">
+        <v>6711.934</v>
+      </c>
+      <c r="C11">
+        <f>_xll.JsonLookup($A$1,A11)</f>
+        <v>6711.9340000000002</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" t="str">
+        <v>Data.2018-07-09T20:01:00Z</v>
+      </c>
+      <c r="B12" t="str">
+        <v>6712.131</v>
+      </c>
+      <c r="C12">
+        <f>_xll.JsonLookup($A$1,A12)</f>
+        <v>6712.1310000000003</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" t="str">
+        <v>Data.2018-07-09T20:02:00Z</v>
+      </c>
+      <c r="B13" t="str">
+        <v>6711.981</v>
+      </c>
+      <c r="C13">
+        <f>_xll.JsonLookup($A$1,A13)</f>
+        <v>6711.9809999999998</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" t="str">
+        <v>Data.2018-07-09T20:03:00Z</v>
+      </c>
+      <c r="B14" t="str">
+        <v>6711.781</v>
+      </c>
+      <c r="C14">
+        <f>_xll.JsonLookup($A$1,A14)</f>
+        <v>6711.7809999999999</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15" t="str">
+        <v>Data.2018-07-09T20:04:00Z</v>
+      </c>
+      <c r="B15" t="str">
+        <v>6711.586</v>
+      </c>
+      <c r="C15">
+        <f>_xll.JsonLookup($A$1,A15)</f>
+        <v>6711.5860000000002</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="A16" t="str">
+        <v>Data.2018-07-09T20:05:00Z</v>
+      </c>
+      <c r="B16" t="str">
+        <v>6711.139</v>
+      </c>
+      <c r="C16">
+        <f>_xll.JsonLookup($A$1,A16)</f>
+        <v>6711.1390000000001</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" t="str">
+        <v>Data.2018-07-09T20:06:00Z</v>
+      </c>
+      <c r="B17" t="str">
+        <v>6710.862</v>
+      </c>
+      <c r="C17">
+        <f>_xll.JsonLookup($A$1,A17)</f>
+        <v>6710.8620000000001</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18" t="str">
+        <v>Data.2018-07-09T20:07:00Z</v>
+      </c>
+      <c r="B18" t="str">
+        <v>6710.37</v>
+      </c>
+      <c r="C18">
+        <f>_xll.JsonLookup($A$1,A18)</f>
+        <v>6710.37</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19" t="str">
+        <v>Data.2018-07-09T20:08:00Z</v>
+      </c>
+      <c r="B19" t="str">
+        <v>6709.85</v>
+      </c>
+      <c r="C19">
+        <f>_xll.JsonLookup($A$1,A19)</f>
+        <v>6709.85</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20" t="str">
+        <v>Data.2018-07-09T20:09:00Z</v>
+      </c>
+      <c r="B20" t="str">
+        <v>6709.287</v>
+      </c>
+      <c r="C20">
+        <f>_xll.JsonLookup($A$1,A20)</f>
+        <v>6709.2870000000003</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
+      <c r="A21" t="str">
+        <v>Data.2018-07-09T20:10:00Z</v>
+      </c>
+      <c r="B21" t="str">
+        <v>6709.276</v>
+      </c>
+      <c r="C21">
+        <f>_xll.JsonLookup($A$1,A21)</f>
+        <v>6709.2759999999998</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3">
+      <c r="A22" t="str">
+        <v>Data.2018-07-09T20:11:00Z</v>
+      </c>
+      <c r="B22" t="str">
+        <v>6708.481</v>
+      </c>
+      <c r="C22">
+        <f>_xll.JsonLookup($A$1,A22)</f>
+        <v>6708.4809999999998</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3">
+      <c r="A23" t="str">
+        <v>Data.2018-07-09T20:12:00Z</v>
+      </c>
+      <c r="B23" t="str">
+        <v>6707.577</v>
+      </c>
+      <c r="C23">
+        <f>_xll.JsonLookup($A$1,A23)</f>
+        <v>6707.5770000000002</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3">
+      <c r="A24" t="str">
+        <v>Data.2018-07-09T20:13:00Z</v>
+      </c>
+      <c r="B24" t="str">
+        <v>6706.426</v>
+      </c>
+      <c r="C24">
+        <f>_xll.JsonLookup($A$1,A24)</f>
+        <v>6706.4260000000004</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3">
+      <c r="A25" t="str">
+        <v>Data.2018-07-09T20:14:00Z</v>
+      </c>
+      <c r="B25" t="str">
+        <v>6705.262</v>
+      </c>
+      <c r="C25">
+        <f>_xll.JsonLookup($A$1,A25)</f>
+        <v>6705.2619999999997</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3">
+      <c r="A26" t="str">
+        <v>Data.2018-07-09T20:15:00Z</v>
+      </c>
+      <c r="B26" t="str">
+        <v>6704.555</v>
+      </c>
+      <c r="C26">
+        <f>_xll.JsonLookup($A$1,A26)</f>
+        <v>6704.5550000000003</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3">
+      <c r="A27" t="str">
+        <v>Data.2018-07-09T20:16:00Z</v>
+      </c>
+      <c r="B27" t="str">
+        <v>6703.435</v>
+      </c>
+      <c r="C27">
+        <f>_xll.JsonLookup($A$1,A27)</f>
+        <v>6703.4350000000004</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3">
+      <c r="A28" t="str">
+        <v>Data.2018-07-09T20:17:00Z</v>
+      </c>
+      <c r="B28" t="str">
+        <v>6702.499</v>
+      </c>
+      <c r="C28">
+        <f>_xll.JsonLookup($A$1,A28)</f>
+        <v>6702.4989999999998</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3">
+      <c r="A29" t="str">
+        <v>Data.2018-07-09T20:18:00Z</v>
+      </c>
+      <c r="B29" t="str">
+        <v>6701.406</v>
+      </c>
+      <c r="C29">
+        <f>_xll.JsonLookup($A$1,A29)</f>
+        <v>6701.4059999999999</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3">
+      <c r="A30" t="str">
+        <v>Data.2018-07-09T20:19:00Z</v>
+      </c>
+      <c r="B30" t="str">
+        <v>6700.764</v>
+      </c>
+      <c r="C30">
+        <f>_xll.JsonLookup($A$1,A30)</f>
+        <v>6700.7640000000001</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3">
+      <c r="A31" t="str">
+        <v>Data.2018-07-09T20:20:00Z</v>
+      </c>
+      <c r="B31" t="str">
+        <v>6700.172</v>
+      </c>
+      <c r="C31">
+        <f>_xll.JsonLookup($A$1,A31)</f>
+        <v>6700.1719999999996</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3">
+      <c r="A32" t="str">
+        <v>Data.2018-07-09T20:21:00Z</v>
+      </c>
+      <c r="B32" t="str">
+        <v>6700.068</v>
+      </c>
+      <c r="C32">
+        <f>_xll.JsonLookup($A$1,A32)</f>
+        <v>6700.0680000000002</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3">
+      <c r="A33" t="str">
+        <v>Data.2018-07-09T20:22:00Z</v>
+      </c>
+      <c r="B33" t="str">
+        <v>6700.369</v>
+      </c>
+      <c r="C33">
+        <f>_xll.JsonLookup($A$1,A33)</f>
+        <v>6700.3689999999997</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3">
+      <c r="A34" t="str">
+        <v>Data.2018-07-09T20:23:00Z</v>
+      </c>
+      <c r="B34" t="str">
+        <v>6701.091</v>
+      </c>
+      <c r="C34">
+        <f>_xll.JsonLookup($A$1,A34)</f>
+        <v>6701.0910000000003</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3">
+      <c r="A35" t="str">
+        <v>Data.2018-07-09T20:24:00Z</v>
+      </c>
+      <c r="B35" t="str">
+        <v>6701.538</v>
+      </c>
+      <c r="C35">
+        <f>_xll.JsonLookup($A$1,A35)</f>
+        <v>6701.5379999999996</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3">
+      <c r="A36" t="str">
+        <v>Data.2018-07-09T20:25:00Z</v>
+      </c>
+      <c r="B36" t="str">
+        <v>6701.738</v>
+      </c>
+      <c r="C36">
+        <f>_xll.JsonLookup($A$1,A36)</f>
+        <v>6701.7380000000003</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3">
+      <c r="A37" t="str">
+        <v>Data.2018-07-09T20:26:00Z</v>
+      </c>
+      <c r="B37" t="str">
+        <v>6702.119</v>
+      </c>
+      <c r="C37">
+        <f>_xll.JsonLookup($A$1,A37)</f>
+        <v>6702.1189999999997</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3">
+      <c r="A38" t="str">
+        <v>Data.2018-07-09T20:27:00Z</v>
+      </c>
+      <c r="B38" t="str">
+        <v>6702.619</v>
+      </c>
+      <c r="C38">
+        <f>_xll.JsonLookup($A$1,A38)</f>
+        <v>6702.6189999999997</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3">
+      <c r="A39" t="str">
+        <v>Data.2018-07-09T20:28:00Z</v>
+      </c>
+      <c r="B39" t="str">
+        <v>6703.014</v>
+      </c>
+      <c r="C39">
+        <f>_xll.JsonLookup($A$1,A39)</f>
+        <v>6703.0140000000001</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3">
+      <c r="A40" t="str">
+        <v>Data.2018-07-09T20:29:00Z</v>
+      </c>
+      <c r="B40" t="str">
+        <v>6703</v>
+      </c>
+      <c r="C40">
+        <f>_xll.JsonLookup($A$1,A40)</f>
+        <v>6703</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3">
+      <c r="A41" t="str">
+        <v>Data.2018-07-09T20:30:00Z</v>
+      </c>
+      <c r="B41" t="str">
+        <v>6702.899</v>
+      </c>
+      <c r="C41">
+        <f>_xll.JsonLookup($A$1,A41)</f>
+        <v>6702.8990000000003</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3">
+      <c r="A42" t="str">
+        <v>Data.2018-07-09T20:31:00Z</v>
+      </c>
+      <c r="B42" t="str">
+        <v>6702.822</v>
+      </c>
+      <c r="C42">
+        <f>_xll.JsonLookup($A$1,A42)</f>
+        <v>6702.8220000000001</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3">
+      <c r="A43" t="str">
+        <v>Data.2018-07-09T20:32:00Z</v>
+      </c>
+      <c r="B43" t="str">
+        <v>6703.146</v>
+      </c>
+      <c r="C43">
+        <f>_xll.JsonLookup($A$1,A43)</f>
+        <v>6703.1459999999997</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3">
+      <c r="A44" t="str">
+        <v>Data.2018-07-09T20:33:00Z</v>
+      </c>
+      <c r="B44" t="str">
+        <v>6702.996</v>
+      </c>
+      <c r="C44">
+        <f>_xll.JsonLookup($A$1,A44)</f>
+        <v>6702.9960000000001</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3">
+      <c r="A45" t="str">
+        <v>Data.2018-07-09T20:34:00Z</v>
+      </c>
+      <c r="B45" t="str">
+        <v>6703.119</v>
+      </c>
+      <c r="C45">
+        <f>_xll.JsonLookup($A$1,A45)</f>
+        <v>6703.1189999999997</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3">
+      <c r="A46" t="str">
+        <v>Data.2018-07-09T20:35:00Z</v>
+      </c>
+      <c r="B46" t="str">
+        <v>6703.501</v>
+      </c>
+      <c r="C46">
+        <f>_xll.JsonLookup($A$1,A46)</f>
+        <v>6703.5010000000002</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3">
+      <c r="A47" t="str">
+        <v>Data.2018-07-09T20:36:00Z</v>
+      </c>
+      <c r="B47" t="str">
+        <v>6703.497</v>
+      </c>
+      <c r="C47">
+        <f>_xll.JsonLookup($A$1,A47)</f>
+        <v>6703.4970000000003</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3">
+      <c r="A48" t="str">
+        <v>Data.2018-07-09T20:37:00Z</v>
+      </c>
+      <c r="B48" t="str">
+        <v>6703.831</v>
+      </c>
+      <c r="C48">
+        <f>_xll.JsonLookup($A$1,A48)</f>
+        <v>6703.8310000000001</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3">
+      <c r="A49" t="str">
+        <v>Data.2018-07-09T20:38:00Z</v>
+      </c>
+      <c r="B49" t="str">
+        <v>6703.927</v>
+      </c>
+      <c r="C49">
+        <f>_xll.JsonLookup($A$1,A49)</f>
+        <v>6703.9269999999997</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3">
+      <c r="A50" t="str">
+        <v>Data.2018-07-09T20:39:00Z</v>
+      </c>
+      <c r="B50" t="str">
+        <v>6704.307</v>
+      </c>
+      <c r="C50">
+        <f>_xll.JsonLookup($A$1,A50)</f>
+        <v>6704.3069999999998</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3">
+      <c r="A51" t="str">
+        <v>Data.2018-07-09T20:40:00Z</v>
+      </c>
+      <c r="B51" t="str">
+        <v>6704.571</v>
+      </c>
+      <c r="C51">
+        <f>_xll.JsonLookup($A$1,A51)</f>
+        <v>6704.5709999999999</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3">
+      <c r="A52" t="str">
+        <v>Data.2018-07-09T20:41:00Z</v>
+      </c>
+      <c r="B52" t="str">
+        <v>6705.048</v>
+      </c>
+      <c r="C52">
+        <f>_xll.JsonLookup($A$1,A52)</f>
+        <v>6705.0479999999998</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3">
+      <c r="A53" t="str">
+        <v>Data.2018-07-09T20:42:00Z</v>
+      </c>
+      <c r="B53" t="str">
+        <v>6704.332</v>
+      </c>
+      <c r="C53">
+        <f>_xll.JsonLookup($A$1,A53)</f>
+        <v>6704.3320000000003</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3">
+      <c r="A54" t="str">
+        <v>Data.2018-07-09T20:43:00Z</v>
+      </c>
+      <c r="B54" t="str">
+        <v>6703.92</v>
+      </c>
+      <c r="C54">
+        <f>_xll.JsonLookup($A$1,A54)</f>
+        <v>6703.92</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3">
+      <c r="A55" t="str">
+        <v>Data.2018-07-09T20:44:00Z</v>
+      </c>
+      <c r="B55" t="str">
+        <v>6703.685</v>
+      </c>
+      <c r="C55">
+        <f>_xll.JsonLookup($A$1,A55)</f>
+        <v>6703.6850000000004</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3">
+      <c r="A56" t="str">
+        <v>Data.2018-07-09T20:45:00Z</v>
+      </c>
+      <c r="B56" t="str">
+        <v>6703.19</v>
+      </c>
+      <c r="C56">
+        <f>_xll.JsonLookup($A$1,A56)</f>
+        <v>6703.19</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3">
+      <c r="A57" t="str">
+        <v>Data.2018-07-09T20:46:00Z</v>
+      </c>
+      <c r="B57" t="str">
+        <v>6703.345</v>
+      </c>
+      <c r="C57">
+        <f>_xll.JsonLookup($A$1,A57)</f>
+        <v>6703.3450000000003</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3">
+      <c r="A58" t="str">
+        <v>Data.2018-07-09T20:47:00Z</v>
+      </c>
+      <c r="B58" t="str">
+        <v>6703.208</v>
+      </c>
+      <c r="C58">
+        <f>_xll.JsonLookup($A$1,A58)</f>
+        <v>6703.2079999999996</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3">
+      <c r="A59" t="str">
+        <v>Data.2018-07-09T20:48:00Z</v>
+      </c>
+      <c r="B59" t="str">
+        <v>6703.218</v>
+      </c>
+      <c r="C59">
+        <f>_xll.JsonLookup($A$1,A59)</f>
+        <v>6703.2179999999998</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3">
+      <c r="A60" t="str">
+        <v>Data.2018-07-09T20:49:00Z</v>
+      </c>
+      <c r="B60" t="str">
+        <v>6703.057</v>
+      </c>
+      <c r="C60">
+        <f>_xll.JsonLookup($A$1,A60)</f>
+        <v>6703.0569999999998</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3">
+      <c r="A61" t="str">
+        <v>Data.2018-07-09T20:50:00Z</v>
+      </c>
+      <c r="B61" t="str">
+        <v>6702.836</v>
+      </c>
+      <c r="C61">
+        <f>_xll.JsonLookup($A$1,A61)</f>
+        <v>6702.8360000000002</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3">
+      <c r="A62" t="str">
+        <v>Data.2018-07-09T20:51:00Z</v>
+      </c>
+      <c r="B62" t="str">
+        <v>6702.379</v>
+      </c>
+      <c r="C62">
+        <f>_xll.JsonLookup($A$1,A62)</f>
+        <v>6702.3789999999999</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3">
+      <c r="A63" t="str">
+        <v>Data.2018-07-09T20:52:00Z</v>
+      </c>
+      <c r="B63" t="str">
+        <v>6702.368</v>
+      </c>
+      <c r="C63">
+        <f>_xll.JsonLookup($A$1,A63)</f>
+        <v>6702.3680000000004</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3">
+      <c r="A64" t="str">
+        <v>Data.2018-07-09T20:53:00Z</v>
+      </c>
+      <c r="B64" t="str">
+        <v>6702.281</v>
+      </c>
+      <c r="C64">
+        <f>_xll.JsonLookup($A$1,A64)</f>
+        <v>6702.2809999999999</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3">
+      <c r="A65" t="str">
+        <v>Data.2018-07-09T20:54:00Z</v>
+      </c>
+      <c r="B65" t="str">
+        <v>6702.017</v>
+      </c>
+      <c r="C65">
+        <f>_xll.JsonLookup($A$1,A65)</f>
+        <v>6702.0169999999998</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3">
+      <c r="A66" t="str">
+        <v>Data.2018-07-09T20:55:00Z</v>
+      </c>
+      <c r="B66" t="str">
+        <v>6701.851</v>
+      </c>
+      <c r="C66">
+        <f>_xll.JsonLookup($A$1,A66)</f>
+        <v>6701.8509999999997</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3">
+      <c r="A67" t="str">
+        <v>Data.2018-07-09T20:56:00Z</v>
+      </c>
+      <c r="B67" t="str">
+        <v>6701.26</v>
+      </c>
+      <c r="C67">
+        <f>_xll.JsonLookup($A$1,A67)</f>
+        <v>6701.26</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3">
+      <c r="A68" t="str">
+        <v>Data.2018-07-09T20:57:00Z</v>
+      </c>
+      <c r="B68" t="str">
+        <v>6700.684</v>
+      </c>
+      <c r="C68">
+        <f>_xll.JsonLookup($A$1,A68)</f>
+        <v>6700.6840000000002</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3">
+      <c r="A69" t="str">
+        <v>Data.2018-07-09T20:58:00Z</v>
+      </c>
+      <c r="B69" t="str">
+        <v>6699.999</v>
+      </c>
+      <c r="C69">
+        <f>_xll.JsonLookup($A$1,A69)</f>
+        <v>6699.9989999999998</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3">
+      <c r="A70" t="str">
+        <v>Data.2018-07-09T20:59:00Z</v>
+      </c>
+      <c r="B70" t="str">
+        <v>6699.6</v>
+      </c>
+      <c r="C70">
+        <f>_xll.JsonLookup($A$1,A70)</f>
+        <v>6699.6</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3">
+      <c r="A71" t="str">
+        <v>Data.2018-07-09T21:00:00Z</v>
+      </c>
+      <c r="B71" t="str">
+        <v>6699.087</v>
+      </c>
+      <c r="C71">
+        <f>_xll.JsonLookup($A$1,A71)</f>
+        <v>6699.0870000000004</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3">
+      <c r="A72" t="str">
+        <v>Data.2018-07-09T21:01:00Z</v>
+      </c>
+      <c r="B72" t="str">
+        <v>6698.745</v>
+      </c>
+      <c r="C72">
+        <f>_xll.JsonLookup($A$1,A72)</f>
+        <v>6698.7449999999999</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3">
+      <c r="A73" t="str">
+        <v>Data.2018-07-09T21:02:00Z</v>
+      </c>
+      <c r="B73" t="str">
+        <v>6698.449</v>
+      </c>
+      <c r="C73">
+        <f>_xll.JsonLookup($A$1,A73)</f>
+        <v>6698.4489999999996</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3">
+      <c r="A74" t="str">
+        <v>Data.2018-07-09T21:03:00Z</v>
+      </c>
+      <c r="B74" t="str">
+        <v>6698.291</v>
+      </c>
+      <c r="C74">
+        <f>_xll.JsonLookup($A$1,A74)</f>
+        <v>6698.2910000000002</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3">
+      <c r="A75" t="str">
+        <v>Data.2018-07-09T21:04:00Z</v>
+      </c>
+      <c r="B75" t="str">
+        <v>6698.133</v>
+      </c>
+      <c r="C75">
+        <f>_xll.JsonLookup($A$1,A75)</f>
+        <v>6698.1329999999998</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3">
+      <c r="A76" t="str">
+        <v>Data.2018-07-09T21:05:00Z</v>
+      </c>
+      <c r="B76" t="str">
+        <v>6697.738</v>
+      </c>
+      <c r="C76">
+        <f>_xll.JsonLookup($A$1,A76)</f>
+        <v>6697.7380000000003</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3">
+      <c r="A77" t="str">
+        <v>Data.2018-07-09T21:06:00Z</v>
+      </c>
+      <c r="B77" t="str">
+        <v>6697.319</v>
+      </c>
+      <c r="C77">
+        <f>_xll.JsonLookup($A$1,A77)</f>
+        <v>6697.3190000000004</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3">
+      <c r="A78" t="str">
+        <v>Data.2018-07-09T21:07:00Z</v>
+      </c>
+      <c r="B78" t="str">
+        <v>6697.161</v>
+      </c>
+      <c r="C78">
+        <f>_xll.JsonLookup($A$1,A78)</f>
+        <v>6697.1610000000001</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3">
+      <c r="A79" t="str">
+        <v>Data.2018-07-09T21:08:00Z</v>
+      </c>
+      <c r="B79" t="str">
+        <v>6697.445</v>
+      </c>
+      <c r="C79">
+        <f>_xll.JsonLookup($A$1,A79)</f>
+        <v>6697.4449999999997</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3">
+      <c r="A80" t="str">
+        <v>Data.2018-07-09T21:09:00Z</v>
+      </c>
+      <c r="B80" t="str">
+        <v>6697.444</v>
+      </c>
+      <c r="C80">
+        <f>_xll.JsonLookup($A$1,A80)</f>
+        <v>6697.4440000000004</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3">
+      <c r="A81" t="str">
+        <v>Data.2018-07-09T21:10:00Z</v>
+      </c>
+      <c r="B81" t="str">
+        <v>6697.62</v>
+      </c>
+      <c r="C81">
+        <f>_xll.JsonLookup($A$1,A81)</f>
+        <v>6697.62</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3">
+      <c r="A82" t="str">
+        <v>Data.2018-07-09T21:11:00Z</v>
+      </c>
+      <c r="B82" t="str">
+        <v>6697.619</v>
+      </c>
+      <c r="C82">
+        <f>_xll.JsonLookup($A$1,A82)</f>
+        <v>6697.6189999999997</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3">
+      <c r="A83" t="str">
+        <v>Data.2018-07-09T21:12:00Z</v>
+      </c>
+      <c r="B83" t="str">
+        <v>6697.642</v>
+      </c>
+      <c r="C83">
+        <f>_xll.JsonLookup($A$1,A83)</f>
+        <v>6697.6419999999998</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3">
+      <c r="A84" t="str">
+        <v>Data.2018-07-09T21:13:00Z</v>
+      </c>
+      <c r="B84" t="str">
+        <v>6697.604</v>
+      </c>
+      <c r="C84">
+        <f>_xll.JsonLookup($A$1,A84)</f>
+        <v>6697.6040000000003</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3">
+      <c r="A85" t="str">
+        <v>Data.2018-07-09T21:14:00Z</v>
+      </c>
+      <c r="B85" t="str">
+        <v>6697.565</v>
+      </c>
+      <c r="C85">
+        <f>_xll.JsonLookup($A$1,A85)</f>
+        <v>6697.5649999999996</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3">
+      <c r="A86" t="str">
+        <v>Data.2018-07-09T21:15:00Z</v>
+      </c>
+      <c r="B86" t="str">
+        <v>6698.039</v>
+      </c>
+      <c r="C86">
+        <f>_xll.JsonLookup($A$1,A86)</f>
+        <v>6698.0389999999998</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3">
+      <c r="A87" t="str">
+        <v>Data.2018-07-09T21:16:00Z</v>
+      </c>
+      <c r="B87" t="str">
+        <v>6698.229</v>
+      </c>
+      <c r="C87">
+        <f>_xll.JsonLookup($A$1,A87)</f>
+        <v>6698.2290000000003</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3">
+      <c r="A88" t="str">
+        <v>Data.2018-07-09T21:17:00Z</v>
+      </c>
+      <c r="B88" t="str">
+        <v>6698.158</v>
+      </c>
+      <c r="C88">
+        <f>_xll.JsonLookup($A$1,A88)</f>
+        <v>6698.1580000000004</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3">
+      <c r="A89" t="str">
+        <v>Data.2018-07-09T21:18:00Z</v>
+      </c>
+      <c r="B89" t="str">
+        <v>6697.995</v>
+      </c>
+      <c r="C89">
+        <f>_xll.JsonLookup($A$1,A89)</f>
+        <v>6697.9949999999999</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3">
+      <c r="A90" t="str">
+        <v>Data.2018-07-09T21:19:00Z</v>
+      </c>
+      <c r="B90" t="str">
+        <v>6698.077</v>
+      </c>
+      <c r="C90">
+        <f>_xll.JsonLookup($A$1,A90)</f>
+        <v>6698.0770000000002</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3">
+      <c r="A91" t="str">
+        <v>Data.2018-07-09T21:20:00Z</v>
+      </c>
+      <c r="B91" t="str">
+        <v>6698.174</v>
+      </c>
+      <c r="C91">
+        <f>_xll.JsonLookup($A$1,A91)</f>
+        <v>6698.174</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3">
+      <c r="A92" t="str">
+        <v>Data.2018-07-09T21:21:00Z</v>
+      </c>
+      <c r="B92" t="str">
+        <v>6698.574</v>
+      </c>
+      <c r="C92">
+        <f>_xll.JsonLookup($A$1,A92)</f>
+        <v>6698.5739999999996</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3">
+      <c r="A93" t="str">
+        <v>Data.2018-07-09T21:22:00Z</v>
+      </c>
+      <c r="B93" t="str">
+        <v>6699.397</v>
+      </c>
+      <c r="C93">
+        <f>_xll.JsonLookup($A$1,A93)</f>
+        <v>6699.3969999999999</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3">
+      <c r="A94" t="str">
+        <v>Data.2018-07-09T21:23:00Z</v>
+      </c>
+      <c r="B94" t="str">
+        <v>6700.549</v>
+      </c>
+      <c r="C94">
+        <f>_xll.JsonLookup($A$1,A94)</f>
+        <v>6700.549</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3">
+      <c r="A95" t="str">
+        <v>Data.2018-07-09T21:24:00Z</v>
+      </c>
+      <c r="B95" t="str">
+        <v>6701.633</v>
+      </c>
+      <c r="C95">
+        <f>_xll.JsonLookup($A$1,A95)</f>
+        <v>6701.6329999999998</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3">
+      <c r="A96" t="str">
+        <v>Data.2018-07-09T21:25:00Z</v>
+      </c>
+      <c r="B96" t="str">
+        <v>6702.441</v>
+      </c>
+      <c r="C96">
+        <f>_xll.JsonLookup($A$1,A96)</f>
+        <v>6702.4409999999998</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3">
+      <c r="A97" t="str">
+        <v>Data.2018-07-09T21:26:00Z</v>
+      </c>
+      <c r="B97" t="str">
+        <v>6703.554</v>
+      </c>
+      <c r="C97">
+        <f>_xll.JsonLookup($A$1,A97)</f>
+        <v>6703.5540000000001</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3">
+      <c r="A98" t="str">
+        <v>Data.2018-07-09T21:27:00Z</v>
+      </c>
+      <c r="B98" t="str">
+        <v>6704.667</v>
+      </c>
+      <c r="C98">
+        <f>_xll.JsonLookup($A$1,A98)</f>
+        <v>6704.6670000000004</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3">
+      <c r="A99" t="str">
+        <v>Data.2018-07-09T21:28:00Z</v>
+      </c>
+      <c r="B99" t="str">
+        <v>6705.638</v>
+      </c>
+      <c r="C99">
+        <f>_xll.JsonLookup($A$1,A99)</f>
+        <v>6705.6379999999999</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3">
+      <c r="A100" t="str">
+        <v>Data.2018-07-09T21:29:00Z</v>
+      </c>
+      <c r="B100" t="str">
+        <v>6706.43</v>
+      </c>
+      <c r="C100">
+        <f>_xll.JsonLookup($A$1,A100)</f>
+        <v>6706.43</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3">
+      <c r="A101" t="str">
+        <v>Inputs.PERIOD</v>
+      </c>
+      <c r="B101" t="str">
+        <v>10</v>
+      </c>
+      <c r="C101">
+        <f>_xll.JsonLookup($A$1,A101)</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3">
+      <c r="A102" t="str">
+        <v>ModelStartTime</v>
+      </c>
+      <c r="B102" t="str">
+        <v>1531157418480</v>
+      </c>
+      <c r="C102">
+        <f>_xll.JsonLookup($A$1,A102)</f>
+        <v>1531157418480</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3">
+      <c r="A103" t="str">
+        <v>ModelEndTime</v>
+      </c>
+      <c r="B103" t="str">
+        <v>1531157418480</v>
+      </c>
+      <c r="C103">
+        <f>_xll.JsonLookup($A$1,A103)</f>
+        <v>1531157418480</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3">
+      <c r="A104" t="str">
+        <v>Interval</v>
+      </c>
+      <c r="B104" t="str">
+        <v>OneMinute</v>
+      </c>
+      <c r="C104" t="str">
+        <f>_xll.JsonLookup($A$1,A104)</f>
+        <v>OneMinute</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3">
+      <c r="A105" t="str">
+        <v>Symbol</v>
+      </c>
+      <c r="B105" t="str">
+        <v>BTCUSDT</v>
+      </c>
+      <c r="C105" t="str">
+        <f>_xll.JsonLookup($A$1,A105)</f>
+        <v>BTCUSDT</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3">
+      <c r="A106" t="str">
+        <v>Source</v>
+      </c>
+      <c r="B106" t="str">
+        <v>BINANCE_KLINE.BTCUSDT.OneMinute</v>
+      </c>
+      <c r="C106" t="str">
+        <f>_xll.JsonLookup($A$1,A106)</f>
+        <v>BINANCE_KLINE.BTCUSDT.OneMinute</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3">
+      <c r="A107" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="B107" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="C107" t="e">
+        <f>_xll.JsonLookup($A$1,A107)</f>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="108" spans="1:3">
+      <c r="A108" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="B108" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="C108" t="e">
+        <f>_xll.JsonLookup($A$1,A108)</f>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3">
+      <c r="A109" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="B109" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="C109" t="e">
+        <f>_xll.JsonLookup($A$1,A109)</f>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="110" spans="1:3">
+      <c r="A110" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="B110" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="C110" t="e">
+        <f>_xll.JsonLookup($A$1,A110)</f>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="111" spans="1:3">
+      <c r="A111" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="B111" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="C111" t="e">
+        <f>_xll.JsonLookup($A$1,A111)</f>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="112" spans="1:3">
+      <c r="A112" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="B112" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="C112" t="e">
+        <f>_xll.JsonLookup($A$1,A112)</f>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="113" spans="1:3">
+      <c r="A113" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="B113" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="C113" t="e">
+        <f>_xll.JsonLookup($A$1,A113)</f>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="114" spans="1:3">
+      <c r="A114" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="B114" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="C114" t="e">
+        <f>_xll.JsonLookup($A$1,A114)</f>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="115" spans="1:3">
+      <c r="A115" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="B115" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="C115" t="e">
+        <f>_xll.JsonLookup($A$1,A115)</f>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="116" spans="1:3">
+      <c r="A116" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="B116" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="C116" t="e">
+        <f>_xll.JsonLookup($A$1,A116)</f>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="117" spans="1:3">
+      <c r="A117" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="B117" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="C117" t="e">
+        <f>_xll.JsonLookup($A$1,A117)</f>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="118" spans="1:3">
+      <c r="A118" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="B118" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="C118" t="e">
+        <f>_xll.JsonLookup($A$1,A118)</f>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="119" spans="1:3">
+      <c r="A119" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="B119" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="C119" t="e">
+        <f>_xll.JsonLookup($A$1,A119)</f>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="120" spans="1:3">
+      <c r="A120" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="B120" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="C120" t="e">
+        <f>_xll.JsonLookup($A$1,A120)</f>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="121" spans="1:3">
+      <c r="A121" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="B121" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="C121" t="e">
+        <f>_xll.JsonLookup($A$1,A121)</f>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="122" spans="1:3">
+      <c r="A122" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="B122" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="C122" t="e">
+        <f>_xll.JsonLookup($A$1,A122)</f>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="123" spans="1:3">
+      <c r="A123" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="B123" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="C123" t="e">
+        <f>_xll.JsonLookup($A$1,A123)</f>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="124" spans="1:3">
+      <c r="A124" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="B124" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="C124" t="e">
+        <f>_xll.JsonLookup($A$1,A124)</f>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="125" spans="1:3">
+      <c r="A125" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="B125" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="C125" t="e">
+        <f>_xll.JsonLookup($A$1,A125)</f>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="126" spans="1:3">
+      <c r="A126" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="B126" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="C126" t="e">
+        <f>_xll.JsonLookup($A$1,A126)</f>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="127" spans="1:3">
+      <c r="A127" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="B127" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="C127" t="e">
+        <f>_xll.JsonLookup($A$1,A127)</f>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="128" spans="1:3">
+      <c r="A128" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="B128" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="C128" t="e">
+        <f>_xll.JsonLookup($A$1,A128)</f>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="129" spans="1:3">
+      <c r="A129" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="B129" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="C129" t="e">
+        <f>_xll.JsonLookup($A$1,A129)</f>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="130" spans="1:3">
+      <c r="A130" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="B130" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="C130" t="e">
+        <f>_xll.JsonLookup($A$1,A130)</f>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="131" spans="1:3">
+      <c r="A131" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="B131" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="C131" t="e">
+        <f>_xll.JsonLookup($A$1,A131)</f>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="132" spans="1:3">
+      <c r="A132" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="B132" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="C132" t="e">
+        <f>_xll.JsonLookup($A$1,A132)</f>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="133" spans="1:3">
+      <c r="A133" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="B133" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="C133" t="e">
+        <f>_xll.JsonLookup($A$1,A133)</f>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="134" spans="1:3">
+      <c r="A134" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="B134" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="C134" t="e">
+        <f>_xll.JsonLookup($A$1,A134)</f>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="135" spans="1:3">
+      <c r="A135" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="B135" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="C135" t="e">
+        <f>_xll.JsonLookup($A$1,A135)</f>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="136" spans="1:3">
+      <c r="A136" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="B136" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="C136" t="e">
+        <f>_xll.JsonLookup($A$1,A136)</f>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="137" spans="1:3">
+      <c r="A137" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="B137" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="C137" t="e">
+        <f>_xll.JsonLookup($A$1,A137)</f>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="138" spans="1:3">
+      <c r="A138" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="B138" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="C138" t="e">
+        <f>_xll.JsonLookup($A$1,A138)</f>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="139" spans="1:3">
+      <c r="A139" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="B139" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="C139" t="e">
+        <f>_xll.JsonLookup($A$1,A139)</f>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="140" spans="1:3">
+      <c r="A140" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="B140" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="C140" t="e">
+        <f>_xll.JsonLookup($A$1,A140)</f>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="141" spans="1:3">
+      <c r="A141" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="B141" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="C141" t="e">
+        <f>_xll.JsonLookup($A$1,A141)</f>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="142" spans="1:3">
+      <c r="A142" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="B142" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="C142" t="e">
+        <f>_xll.JsonLookup($A$1,A142)</f>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="143" spans="1:3">
+      <c r="A143" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="B143" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="C143" t="e">
+        <f>_xll.JsonLookup($A$1,A143)</f>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="144" spans="1:3">
+      <c r="A144" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="B144" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="C144" t="e">
+        <f>_xll.JsonLookup($A$1,A144)</f>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="145" spans="1:3">
+      <c r="A145" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="B145" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="C145" t="e">
+        <f>_xll.JsonLookup($A$1,A145)</f>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="146" spans="1:3">
+      <c r="A146" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="B146" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="C146" t="e">
+        <f>_xll.JsonLookup($A$1,A146)</f>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="147" spans="1:3">
+      <c r="A147" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="B147" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="C147" t="e">
+        <f>_xll.JsonLookup($A$1,A147)</f>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="148" spans="1:3">
+      <c r="A148" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="B148" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="C148" t="e">
+        <f>_xll.JsonLookup($A$1,A148)</f>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="149" spans="1:3">
+      <c r="A149" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="B149" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="C149" t="e">
+        <f>_xll.JsonLookup($A$1,A149)</f>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="150" spans="1:3">
+      <c r="A150" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="B150" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="C150" t="e">
+        <f>_xll.JsonLookup($A$1,A150)</f>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="151" spans="1:3">
+      <c r="A151" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="B151" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="C151" t="e">
+        <f>_xll.JsonLookup($A$1,A151)</f>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="152" spans="1:3">
+      <c r="A152" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="B152" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="C152" t="e">
+        <f>_xll.JsonLookup($A$1,A152)</f>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="153" spans="1:3">
+      <c r="A153" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="B153" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="C153" t="e">
+        <f>_xll.JsonLookup($A$1,A153)</f>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="154" spans="1:3">
+      <c r="A154" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="B154" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="C154" t="e">
+        <f>_xll.JsonLookup($A$1,A154)</f>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="155" spans="1:3">
+      <c r="A155" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="B155" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="C155" t="e">
+        <f>_xll.JsonLookup($A$1,A155)</f>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="156" spans="1:3">
+      <c r="A156" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="B156" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="C156" t="e">
+        <f>_xll.JsonLookup($A$1,A156)</f>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="157" spans="1:3">
+      <c r="A157" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="B157" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="C157" t="e">
+        <f>_xll.JsonLookup($A$1,A157)</f>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="158" spans="1:3">
+      <c r="A158" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="B158" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="C158" t="e">
+        <f>_xll.JsonLookup($A$1,A158)</f>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="159" spans="1:3">
+      <c r="A159" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="B159" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="C159" t="e">
+        <f>_xll.JsonLookup($A$1,A159)</f>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="160" spans="1:3">
+      <c r="A160" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="B160" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="C160" t="e">
+        <f>_xll.JsonLookup($A$1,A160)</f>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="161" spans="1:3">
+      <c r="A161" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="B161" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="C161" t="e">
+        <f>_xll.JsonLookup($A$1,A161)</f>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Arrays, convert to native type
</commit_message>
<xml_diff>
--- a/JsonExcel/doc/JsonExcel-test.xlsx
+++ b/JsonExcel/doc/JsonExcel-test.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="P:\OpenSource\JsonExcel\JsonExcel\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FADF5517-D98D-44FD-8217-BDDA2BA921CF}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FFEB442-95C2-4421-AE08-4D2B2C2752BB}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="18885" windowHeight="5910" activeTab="2" xr2:uid="{90F70DC4-6E6D-491C-88DA-FF972DBF519E}"/>
   </bookViews>
@@ -155,7 +155,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
+    <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
   </numFmts>
   <fonts count="2">
     <font>
@@ -197,11 +197,11 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1849,7 +1849,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="4" t="s">
         <v>9</v>
       </c>
       <c r="C1" t="str">
@@ -1865,7 +1865,7 @@
       </c>
     </row>
     <row r="2" spans="1:5">
-      <c r="A2" s="4"/>
+      <c r="A2" s="5"/>
       <c r="C2" t="str">
         <v>web-app.servlet[0].servlet-class</v>
       </c>
@@ -1878,7 +1878,7 @@
       </c>
     </row>
     <row r="3" spans="1:5">
-      <c r="A3" s="4"/>
+      <c r="A3" s="5"/>
       <c r="C3" t="str">
         <v>web-app.servlet[0].init-param.configGlossary:installationAt</v>
       </c>
@@ -1891,7 +1891,7 @@
       </c>
     </row>
     <row r="4" spans="1:5">
-      <c r="A4" s="4"/>
+      <c r="A4" s="5"/>
       <c r="C4" t="str">
         <v>web-app.servlet[0].init-param.configGlossary:adminEmail</v>
       </c>
@@ -1904,7 +1904,7 @@
       </c>
     </row>
     <row r="5" spans="1:5">
-      <c r="A5" s="4"/>
+      <c r="A5" s="5"/>
       <c r="C5" t="str">
         <v>web-app.servlet[0].init-param.configGlossary:poweredBy</v>
       </c>
@@ -1917,7 +1917,7 @@
       </c>
     </row>
     <row r="6" spans="1:5">
-      <c r="A6" s="4"/>
+      <c r="A6" s="5"/>
       <c r="C6" t="str">
         <v>web-app.servlet[0].init-param.configGlossary:poweredByIcon</v>
       </c>
@@ -1930,7 +1930,7 @@
       </c>
     </row>
     <row r="7" spans="1:5">
-      <c r="A7" s="4"/>
+      <c r="A7" s="5"/>
       <c r="C7" t="str">
         <v>web-app.servlet[0].init-param.configGlossary:staticPath</v>
       </c>
@@ -1943,7 +1943,7 @@
       </c>
     </row>
     <row r="8" spans="1:5">
-      <c r="A8" s="4"/>
+      <c r="A8" s="5"/>
       <c r="C8" t="str">
         <v>web-app.servlet[0].init-param.templateProcessorClass</v>
       </c>
@@ -1956,7 +1956,7 @@
       </c>
     </row>
     <row r="9" spans="1:5">
-      <c r="A9" s="4"/>
+      <c r="A9" s="5"/>
       <c r="C9" t="str">
         <v>web-app.servlet[0].init-param.templateLoaderClass</v>
       </c>
@@ -1969,7 +1969,7 @@
       </c>
     </row>
     <row r="10" spans="1:5">
-      <c r="A10" s="4"/>
+      <c r="A10" s="5"/>
       <c r="C10" t="str">
         <v>web-app.servlet[0].init-param.templatePath</v>
       </c>
@@ -1982,7 +1982,7 @@
       </c>
     </row>
     <row r="11" spans="1:5">
-      <c r="A11" s="4"/>
+      <c r="A11" s="5"/>
       <c r="C11" t="str">
         <v>web-app.servlet[0].init-param.templateOverridePath</v>
       </c>
@@ -1995,7 +1995,7 @@
       </c>
     </row>
     <row r="12" spans="1:5">
-      <c r="A12" s="4"/>
+      <c r="A12" s="5"/>
       <c r="C12" t="str">
         <v>web-app.servlet[0].init-param.defaultListTemplate</v>
       </c>
@@ -2008,7 +2008,7 @@
       </c>
     </row>
     <row r="13" spans="1:5">
-      <c r="A13" s="4"/>
+      <c r="A13" s="5"/>
       <c r="C13" t="str">
         <v>web-app.servlet[0].init-param.defaultFileTemplate</v>
       </c>
@@ -2021,7 +2021,7 @@
       </c>
     </row>
     <row r="14" spans="1:5">
-      <c r="A14" s="4"/>
+      <c r="A14" s="5"/>
       <c r="C14" t="str">
         <v>web-app.servlet[0].init-param.useJSP</v>
       </c>
@@ -2034,7 +2034,7 @@
       </c>
     </row>
     <row r="15" spans="1:5">
-      <c r="A15" s="4"/>
+      <c r="A15" s="5"/>
       <c r="C15" t="str">
         <v>web-app.servlet[0].init-param.jspListTemplate</v>
       </c>
@@ -2047,7 +2047,7 @@
       </c>
     </row>
     <row r="16" spans="1:5">
-      <c r="A16" s="4"/>
+      <c r="A16" s="5"/>
       <c r="C16" t="str">
         <v>web-app.servlet[0].init-param.jspFileTemplate</v>
       </c>
@@ -2060,7 +2060,7 @@
       </c>
     </row>
     <row r="17" spans="1:5">
-      <c r="A17" s="4"/>
+      <c r="A17" s="5"/>
       <c r="C17" t="str">
         <v>web-app.servlet[0].init-param.cachePackageTagsTrack</v>
       </c>
@@ -2073,7 +2073,7 @@
       </c>
     </row>
     <row r="18" spans="1:5">
-      <c r="A18" s="4"/>
+      <c r="A18" s="5"/>
       <c r="C18" t="str">
         <v>web-app.servlet[0].init-param.cachePackageTagsStore</v>
       </c>
@@ -2086,7 +2086,7 @@
       </c>
     </row>
     <row r="19" spans="1:5">
-      <c r="A19" s="4"/>
+      <c r="A19" s="5"/>
       <c r="C19" t="str">
         <v>web-app.servlet[0].init-param.cachePackageTagsRefresh</v>
       </c>
@@ -2099,7 +2099,7 @@
       </c>
     </row>
     <row r="20" spans="1:5">
-      <c r="A20" s="4"/>
+      <c r="A20" s="5"/>
       <c r="C20" t="str">
         <v>web-app.servlet[0].init-param.cacheTemplatesTrack</v>
       </c>
@@ -2112,7 +2112,7 @@
       </c>
     </row>
     <row r="21" spans="1:5">
-      <c r="A21" s="4"/>
+      <c r="A21" s="5"/>
       <c r="C21" t="str">
         <v>web-app.servlet[0].init-param.cacheTemplatesStore</v>
       </c>
@@ -2125,7 +2125,7 @@
       </c>
     </row>
     <row r="22" spans="1:5">
-      <c r="A22" s="4"/>
+      <c r="A22" s="5"/>
       <c r="C22" t="str">
         <v>web-app.servlet[0].init-param.cacheTemplatesRefresh</v>
       </c>
@@ -2138,7 +2138,7 @@
       </c>
     </row>
     <row r="23" spans="1:5">
-      <c r="A23" s="4"/>
+      <c r="A23" s="5"/>
       <c r="C23" t="str">
         <v>web-app.servlet[0].init-param.cachePagesTrack</v>
       </c>
@@ -2151,7 +2151,7 @@
       </c>
     </row>
     <row r="24" spans="1:5">
-      <c r="A24" s="4"/>
+      <c r="A24" s="5"/>
       <c r="C24" t="str">
         <v>web-app.servlet[0].init-param.cachePagesStore</v>
       </c>
@@ -2164,7 +2164,7 @@
       </c>
     </row>
     <row r="25" spans="1:5">
-      <c r="A25" s="4"/>
+      <c r="A25" s="5"/>
       <c r="C25" t="str">
         <v>web-app.servlet[0].init-param.cachePagesRefresh</v>
       </c>
@@ -2177,7 +2177,7 @@
       </c>
     </row>
     <row r="26" spans="1:5">
-      <c r="A26" s="4"/>
+      <c r="A26" s="5"/>
       <c r="C26" t="str">
         <v>web-app.servlet[0].init-param.cachePagesDirtyRead</v>
       </c>
@@ -2190,7 +2190,7 @@
       </c>
     </row>
     <row r="27" spans="1:5">
-      <c r="A27" s="4"/>
+      <c r="A27" s="5"/>
       <c r="C27" t="str">
         <v>web-app.servlet[0].init-param.searchEngineListTemplate</v>
       </c>
@@ -2203,7 +2203,7 @@
       </c>
     </row>
     <row r="28" spans="1:5">
-      <c r="A28" s="4"/>
+      <c r="A28" s="5"/>
       <c r="C28" t="str">
         <v>web-app.servlet[0].init-param.searchEngineFileTemplate</v>
       </c>
@@ -2216,7 +2216,7 @@
       </c>
     </row>
     <row r="29" spans="1:5">
-      <c r="A29" s="4"/>
+      <c r="A29" s="5"/>
       <c r="C29" t="str">
         <v>web-app.servlet[0].init-param.searchEngineRobotsDb</v>
       </c>
@@ -2229,7 +2229,7 @@
       </c>
     </row>
     <row r="30" spans="1:5">
-      <c r="A30" s="4"/>
+      <c r="A30" s="5"/>
       <c r="C30" t="str">
         <v>web-app.servlet[0].init-param.useDataStore</v>
       </c>
@@ -2242,7 +2242,7 @@
       </c>
     </row>
     <row r="31" spans="1:5">
-      <c r="A31" s="4"/>
+      <c r="A31" s="5"/>
       <c r="C31" t="str">
         <v>web-app.servlet[0].init-param.dataStoreClass</v>
       </c>
@@ -2255,7 +2255,7 @@
       </c>
     </row>
     <row r="32" spans="1:5">
-      <c r="A32" s="4"/>
+      <c r="A32" s="5"/>
       <c r="C32" t="str">
         <v>web-app.servlet[0].init-param.redirectionClass</v>
       </c>
@@ -2268,7 +2268,7 @@
       </c>
     </row>
     <row r="33" spans="1:5">
-      <c r="A33" s="4"/>
+      <c r="A33" s="5"/>
       <c r="C33" t="str">
         <v>web-app.servlet[0].init-param.dataStoreName</v>
       </c>
@@ -2281,7 +2281,7 @@
       </c>
     </row>
     <row r="34" spans="1:5">
-      <c r="A34" s="4"/>
+      <c r="A34" s="5"/>
       <c r="C34" t="str">
         <v>web-app.servlet[0].init-param.dataStoreDriver</v>
       </c>
@@ -2294,7 +2294,7 @@
       </c>
     </row>
     <row r="35" spans="1:5">
-      <c r="A35" s="4"/>
+      <c r="A35" s="5"/>
       <c r="C35" t="str">
         <v>web-app.servlet[0].init-param.dataStoreUrl</v>
       </c>
@@ -2307,7 +2307,7 @@
       </c>
     </row>
     <row r="36" spans="1:5">
-      <c r="A36" s="4"/>
+      <c r="A36" s="5"/>
       <c r="C36" t="str">
         <v>web-app.servlet[0].init-param.dataStoreUser</v>
       </c>
@@ -2320,7 +2320,7 @@
       </c>
     </row>
     <row r="37" spans="1:5">
-      <c r="A37" s="4"/>
+      <c r="A37" s="5"/>
       <c r="C37" t="str">
         <v>web-app.servlet[0].init-param.dataStorePassword</v>
       </c>
@@ -2333,7 +2333,7 @@
       </c>
     </row>
     <row r="38" spans="1:5">
-      <c r="A38" s="4"/>
+      <c r="A38" s="5"/>
       <c r="C38" t="str">
         <v>web-app.servlet[0].init-param.dataStoreTestQuery</v>
       </c>
@@ -2891,8 +2891,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{54B4FA4A-253A-4DC7-B007-BD642767BFAD}">
   <dimension ref="A1:D161"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B81" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7:C100"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2927,10 +2927,10 @@
       <c r="A6" t="str">
         <v>TargetTime</v>
       </c>
-      <c r="B6" t="str">
-        <v>7/9/2018 9:29:00 PM</v>
-      </c>
-      <c r="C6" s="5">
+      <c r="B6">
+        <v>43290.895138888889</v>
+      </c>
+      <c r="C6" s="3">
         <f>_xll.JsonLookup($A$1,A6)</f>
         <v>43290.895138888889</v>
       </c>
@@ -2939,8 +2939,8 @@
       <c r="A7" t="str">
         <v>Data.2018-07-09T19:56:00Z</v>
       </c>
-      <c r="B7" t="str">
-        <v>6711.493</v>
+      <c r="B7">
+        <v>6711.4930000000004</v>
       </c>
       <c r="C7">
         <f>_xll.JsonLookup($A$1,A7)</f>
@@ -2951,7 +2951,7 @@
       <c r="A8" t="str">
         <v>Data.2018-07-09T19:57:00Z</v>
       </c>
-      <c r="B8" t="str">
+      <c r="B8">
         <v>6711.92</v>
       </c>
       <c r="C8">
@@ -2963,8 +2963,8 @@
       <c r="A9" t="str">
         <v>Data.2018-07-09T19:58:00Z</v>
       </c>
-      <c r="B9" t="str">
-        <v>6712.532</v>
+      <c r="B9">
+        <v>6712.5320000000002</v>
       </c>
       <c r="C9">
         <f>_xll.JsonLookup($A$1,A9)</f>
@@ -2975,8 +2975,8 @@
       <c r="A10" t="str">
         <v>Data.2018-07-09T19:59:00Z</v>
       </c>
-      <c r="B10" t="str">
-        <v>6712.431</v>
+      <c r="B10">
+        <v>6712.4309999999996</v>
       </c>
       <c r="C10">
         <f>_xll.JsonLookup($A$1,A10)</f>
@@ -2987,8 +2987,8 @@
       <c r="A11" t="str">
         <v>Data.2018-07-09T20:00:00Z</v>
       </c>
-      <c r="B11" t="str">
-        <v>6711.934</v>
+      <c r="B11">
+        <v>6711.9340000000002</v>
       </c>
       <c r="C11">
         <f>_xll.JsonLookup($A$1,A11)</f>
@@ -2999,8 +2999,8 @@
       <c r="A12" t="str">
         <v>Data.2018-07-09T20:01:00Z</v>
       </c>
-      <c r="B12" t="str">
-        <v>6712.131</v>
+      <c r="B12">
+        <v>6712.1310000000003</v>
       </c>
       <c r="C12">
         <f>_xll.JsonLookup($A$1,A12)</f>
@@ -3011,8 +3011,8 @@
       <c r="A13" t="str">
         <v>Data.2018-07-09T20:02:00Z</v>
       </c>
-      <c r="B13" t="str">
-        <v>6711.981</v>
+      <c r="B13">
+        <v>6711.9809999999998</v>
       </c>
       <c r="C13">
         <f>_xll.JsonLookup($A$1,A13)</f>
@@ -3023,8 +3023,8 @@
       <c r="A14" t="str">
         <v>Data.2018-07-09T20:03:00Z</v>
       </c>
-      <c r="B14" t="str">
-        <v>6711.781</v>
+      <c r="B14">
+        <v>6711.7809999999999</v>
       </c>
       <c r="C14">
         <f>_xll.JsonLookup($A$1,A14)</f>
@@ -3035,8 +3035,8 @@
       <c r="A15" t="str">
         <v>Data.2018-07-09T20:04:00Z</v>
       </c>
-      <c r="B15" t="str">
-        <v>6711.586</v>
+      <c r="B15">
+        <v>6711.5860000000002</v>
       </c>
       <c r="C15">
         <f>_xll.JsonLookup($A$1,A15)</f>
@@ -3047,8 +3047,8 @@
       <c r="A16" t="str">
         <v>Data.2018-07-09T20:05:00Z</v>
       </c>
-      <c r="B16" t="str">
-        <v>6711.139</v>
+      <c r="B16">
+        <v>6711.1390000000001</v>
       </c>
       <c r="C16">
         <f>_xll.JsonLookup($A$1,A16)</f>
@@ -3059,8 +3059,8 @@
       <c r="A17" t="str">
         <v>Data.2018-07-09T20:06:00Z</v>
       </c>
-      <c r="B17" t="str">
-        <v>6710.862</v>
+      <c r="B17">
+        <v>6710.8620000000001</v>
       </c>
       <c r="C17">
         <f>_xll.JsonLookup($A$1,A17)</f>
@@ -3071,7 +3071,7 @@
       <c r="A18" t="str">
         <v>Data.2018-07-09T20:07:00Z</v>
       </c>
-      <c r="B18" t="str">
+      <c r="B18">
         <v>6710.37</v>
       </c>
       <c r="C18">
@@ -3083,7 +3083,7 @@
       <c r="A19" t="str">
         <v>Data.2018-07-09T20:08:00Z</v>
       </c>
-      <c r="B19" t="str">
+      <c r="B19">
         <v>6709.85</v>
       </c>
       <c r="C19">
@@ -3095,8 +3095,8 @@
       <c r="A20" t="str">
         <v>Data.2018-07-09T20:09:00Z</v>
       </c>
-      <c r="B20" t="str">
-        <v>6709.287</v>
+      <c r="B20">
+        <v>6709.2870000000003</v>
       </c>
       <c r="C20">
         <f>_xll.JsonLookup($A$1,A20)</f>
@@ -3107,8 +3107,8 @@
       <c r="A21" t="str">
         <v>Data.2018-07-09T20:10:00Z</v>
       </c>
-      <c r="B21" t="str">
-        <v>6709.276</v>
+      <c r="B21">
+        <v>6709.2759999999998</v>
       </c>
       <c r="C21">
         <f>_xll.JsonLookup($A$1,A21)</f>
@@ -3119,8 +3119,8 @@
       <c r="A22" t="str">
         <v>Data.2018-07-09T20:11:00Z</v>
       </c>
-      <c r="B22" t="str">
-        <v>6708.481</v>
+      <c r="B22">
+        <v>6708.4809999999998</v>
       </c>
       <c r="C22">
         <f>_xll.JsonLookup($A$1,A22)</f>
@@ -3131,8 +3131,8 @@
       <c r="A23" t="str">
         <v>Data.2018-07-09T20:12:00Z</v>
       </c>
-      <c r="B23" t="str">
-        <v>6707.577</v>
+      <c r="B23">
+        <v>6707.5770000000002</v>
       </c>
       <c r="C23">
         <f>_xll.JsonLookup($A$1,A23)</f>
@@ -3143,8 +3143,8 @@
       <c r="A24" t="str">
         <v>Data.2018-07-09T20:13:00Z</v>
       </c>
-      <c r="B24" t="str">
-        <v>6706.426</v>
+      <c r="B24">
+        <v>6706.4260000000004</v>
       </c>
       <c r="C24">
         <f>_xll.JsonLookup($A$1,A24)</f>
@@ -3155,8 +3155,8 @@
       <c r="A25" t="str">
         <v>Data.2018-07-09T20:14:00Z</v>
       </c>
-      <c r="B25" t="str">
-        <v>6705.262</v>
+      <c r="B25">
+        <v>6705.2619999999997</v>
       </c>
       <c r="C25">
         <f>_xll.JsonLookup($A$1,A25)</f>
@@ -3167,8 +3167,8 @@
       <c r="A26" t="str">
         <v>Data.2018-07-09T20:15:00Z</v>
       </c>
-      <c r="B26" t="str">
-        <v>6704.555</v>
+      <c r="B26">
+        <v>6704.5550000000003</v>
       </c>
       <c r="C26">
         <f>_xll.JsonLookup($A$1,A26)</f>
@@ -3179,8 +3179,8 @@
       <c r="A27" t="str">
         <v>Data.2018-07-09T20:16:00Z</v>
       </c>
-      <c r="B27" t="str">
-        <v>6703.435</v>
+      <c r="B27">
+        <v>6703.4350000000004</v>
       </c>
       <c r="C27">
         <f>_xll.JsonLookup($A$1,A27)</f>
@@ -3191,8 +3191,8 @@
       <c r="A28" t="str">
         <v>Data.2018-07-09T20:17:00Z</v>
       </c>
-      <c r="B28" t="str">
-        <v>6702.499</v>
+      <c r="B28">
+        <v>6702.4989999999998</v>
       </c>
       <c r="C28">
         <f>_xll.JsonLookup($A$1,A28)</f>
@@ -3203,8 +3203,8 @@
       <c r="A29" t="str">
         <v>Data.2018-07-09T20:18:00Z</v>
       </c>
-      <c r="B29" t="str">
-        <v>6701.406</v>
+      <c r="B29">
+        <v>6701.4059999999999</v>
       </c>
       <c r="C29">
         <f>_xll.JsonLookup($A$1,A29)</f>
@@ -3215,8 +3215,8 @@
       <c r="A30" t="str">
         <v>Data.2018-07-09T20:19:00Z</v>
       </c>
-      <c r="B30" t="str">
-        <v>6700.764</v>
+      <c r="B30">
+        <v>6700.7640000000001</v>
       </c>
       <c r="C30">
         <f>_xll.JsonLookup($A$1,A30)</f>
@@ -3227,8 +3227,8 @@
       <c r="A31" t="str">
         <v>Data.2018-07-09T20:20:00Z</v>
       </c>
-      <c r="B31" t="str">
-        <v>6700.172</v>
+      <c r="B31">
+        <v>6700.1719999999996</v>
       </c>
       <c r="C31">
         <f>_xll.JsonLookup($A$1,A31)</f>
@@ -3239,8 +3239,8 @@
       <c r="A32" t="str">
         <v>Data.2018-07-09T20:21:00Z</v>
       </c>
-      <c r="B32" t="str">
-        <v>6700.068</v>
+      <c r="B32">
+        <v>6700.0680000000002</v>
       </c>
       <c r="C32">
         <f>_xll.JsonLookup($A$1,A32)</f>
@@ -3251,8 +3251,8 @@
       <c r="A33" t="str">
         <v>Data.2018-07-09T20:22:00Z</v>
       </c>
-      <c r="B33" t="str">
-        <v>6700.369</v>
+      <c r="B33">
+        <v>6700.3689999999997</v>
       </c>
       <c r="C33">
         <f>_xll.JsonLookup($A$1,A33)</f>
@@ -3263,8 +3263,8 @@
       <c r="A34" t="str">
         <v>Data.2018-07-09T20:23:00Z</v>
       </c>
-      <c r="B34" t="str">
-        <v>6701.091</v>
+      <c r="B34">
+        <v>6701.0910000000003</v>
       </c>
       <c r="C34">
         <f>_xll.JsonLookup($A$1,A34)</f>
@@ -3275,8 +3275,8 @@
       <c r="A35" t="str">
         <v>Data.2018-07-09T20:24:00Z</v>
       </c>
-      <c r="B35" t="str">
-        <v>6701.538</v>
+      <c r="B35">
+        <v>6701.5379999999996</v>
       </c>
       <c r="C35">
         <f>_xll.JsonLookup($A$1,A35)</f>
@@ -3287,8 +3287,8 @@
       <c r="A36" t="str">
         <v>Data.2018-07-09T20:25:00Z</v>
       </c>
-      <c r="B36" t="str">
-        <v>6701.738</v>
+      <c r="B36">
+        <v>6701.7380000000003</v>
       </c>
       <c r="C36">
         <f>_xll.JsonLookup($A$1,A36)</f>
@@ -3299,8 +3299,8 @@
       <c r="A37" t="str">
         <v>Data.2018-07-09T20:26:00Z</v>
       </c>
-      <c r="B37" t="str">
-        <v>6702.119</v>
+      <c r="B37">
+        <v>6702.1189999999997</v>
       </c>
       <c r="C37">
         <f>_xll.JsonLookup($A$1,A37)</f>
@@ -3311,8 +3311,8 @@
       <c r="A38" t="str">
         <v>Data.2018-07-09T20:27:00Z</v>
       </c>
-      <c r="B38" t="str">
-        <v>6702.619</v>
+      <c r="B38">
+        <v>6702.6189999999997</v>
       </c>
       <c r="C38">
         <f>_xll.JsonLookup($A$1,A38)</f>
@@ -3323,8 +3323,8 @@
       <c r="A39" t="str">
         <v>Data.2018-07-09T20:28:00Z</v>
       </c>
-      <c r="B39" t="str">
-        <v>6703.014</v>
+      <c r="B39">
+        <v>6703.0140000000001</v>
       </c>
       <c r="C39">
         <f>_xll.JsonLookup($A$1,A39)</f>
@@ -3335,7 +3335,7 @@
       <c r="A40" t="str">
         <v>Data.2018-07-09T20:29:00Z</v>
       </c>
-      <c r="B40" t="str">
+      <c r="B40">
         <v>6703</v>
       </c>
       <c r="C40">
@@ -3347,8 +3347,8 @@
       <c r="A41" t="str">
         <v>Data.2018-07-09T20:30:00Z</v>
       </c>
-      <c r="B41" t="str">
-        <v>6702.899</v>
+      <c r="B41">
+        <v>6702.8990000000003</v>
       </c>
       <c r="C41">
         <f>_xll.JsonLookup($A$1,A41)</f>
@@ -3359,8 +3359,8 @@
       <c r="A42" t="str">
         <v>Data.2018-07-09T20:31:00Z</v>
       </c>
-      <c r="B42" t="str">
-        <v>6702.822</v>
+      <c r="B42">
+        <v>6702.8220000000001</v>
       </c>
       <c r="C42">
         <f>_xll.JsonLookup($A$1,A42)</f>
@@ -3371,8 +3371,8 @@
       <c r="A43" t="str">
         <v>Data.2018-07-09T20:32:00Z</v>
       </c>
-      <c r="B43" t="str">
-        <v>6703.146</v>
+      <c r="B43">
+        <v>6703.1459999999997</v>
       </c>
       <c r="C43">
         <f>_xll.JsonLookup($A$1,A43)</f>
@@ -3383,8 +3383,8 @@
       <c r="A44" t="str">
         <v>Data.2018-07-09T20:33:00Z</v>
       </c>
-      <c r="B44" t="str">
-        <v>6702.996</v>
+      <c r="B44">
+        <v>6702.9960000000001</v>
       </c>
       <c r="C44">
         <f>_xll.JsonLookup($A$1,A44)</f>
@@ -3395,8 +3395,8 @@
       <c r="A45" t="str">
         <v>Data.2018-07-09T20:34:00Z</v>
       </c>
-      <c r="B45" t="str">
-        <v>6703.119</v>
+      <c r="B45">
+        <v>6703.1189999999997</v>
       </c>
       <c r="C45">
         <f>_xll.JsonLookup($A$1,A45)</f>
@@ -3407,8 +3407,8 @@
       <c r="A46" t="str">
         <v>Data.2018-07-09T20:35:00Z</v>
       </c>
-      <c r="B46" t="str">
-        <v>6703.501</v>
+      <c r="B46">
+        <v>6703.5010000000002</v>
       </c>
       <c r="C46">
         <f>_xll.JsonLookup($A$1,A46)</f>
@@ -3419,8 +3419,8 @@
       <c r="A47" t="str">
         <v>Data.2018-07-09T20:36:00Z</v>
       </c>
-      <c r="B47" t="str">
-        <v>6703.497</v>
+      <c r="B47">
+        <v>6703.4970000000003</v>
       </c>
       <c r="C47">
         <f>_xll.JsonLookup($A$1,A47)</f>
@@ -3431,8 +3431,8 @@
       <c r="A48" t="str">
         <v>Data.2018-07-09T20:37:00Z</v>
       </c>
-      <c r="B48" t="str">
-        <v>6703.831</v>
+      <c r="B48">
+        <v>6703.8310000000001</v>
       </c>
       <c r="C48">
         <f>_xll.JsonLookup($A$1,A48)</f>
@@ -3443,8 +3443,8 @@
       <c r="A49" t="str">
         <v>Data.2018-07-09T20:38:00Z</v>
       </c>
-      <c r="B49" t="str">
-        <v>6703.927</v>
+      <c r="B49">
+        <v>6703.9269999999997</v>
       </c>
       <c r="C49">
         <f>_xll.JsonLookup($A$1,A49)</f>
@@ -3455,8 +3455,8 @@
       <c r="A50" t="str">
         <v>Data.2018-07-09T20:39:00Z</v>
       </c>
-      <c r="B50" t="str">
-        <v>6704.307</v>
+      <c r="B50">
+        <v>6704.3069999999998</v>
       </c>
       <c r="C50">
         <f>_xll.JsonLookup($A$1,A50)</f>
@@ -3467,8 +3467,8 @@
       <c r="A51" t="str">
         <v>Data.2018-07-09T20:40:00Z</v>
       </c>
-      <c r="B51" t="str">
-        <v>6704.571</v>
+      <c r="B51">
+        <v>6704.5709999999999</v>
       </c>
       <c r="C51">
         <f>_xll.JsonLookup($A$1,A51)</f>
@@ -3479,8 +3479,8 @@
       <c r="A52" t="str">
         <v>Data.2018-07-09T20:41:00Z</v>
       </c>
-      <c r="B52" t="str">
-        <v>6705.048</v>
+      <c r="B52">
+        <v>6705.0479999999998</v>
       </c>
       <c r="C52">
         <f>_xll.JsonLookup($A$1,A52)</f>
@@ -3491,8 +3491,8 @@
       <c r="A53" t="str">
         <v>Data.2018-07-09T20:42:00Z</v>
       </c>
-      <c r="B53" t="str">
-        <v>6704.332</v>
+      <c r="B53">
+        <v>6704.3320000000003</v>
       </c>
       <c r="C53">
         <f>_xll.JsonLookup($A$1,A53)</f>
@@ -3503,7 +3503,7 @@
       <c r="A54" t="str">
         <v>Data.2018-07-09T20:43:00Z</v>
       </c>
-      <c r="B54" t="str">
+      <c r="B54">
         <v>6703.92</v>
       </c>
       <c r="C54">
@@ -3515,8 +3515,8 @@
       <c r="A55" t="str">
         <v>Data.2018-07-09T20:44:00Z</v>
       </c>
-      <c r="B55" t="str">
-        <v>6703.685</v>
+      <c r="B55">
+        <v>6703.6850000000004</v>
       </c>
       <c r="C55">
         <f>_xll.JsonLookup($A$1,A55)</f>
@@ -3527,7 +3527,7 @@
       <c r="A56" t="str">
         <v>Data.2018-07-09T20:45:00Z</v>
       </c>
-      <c r="B56" t="str">
+      <c r="B56">
         <v>6703.19</v>
       </c>
       <c r="C56">
@@ -3539,8 +3539,8 @@
       <c r="A57" t="str">
         <v>Data.2018-07-09T20:46:00Z</v>
       </c>
-      <c r="B57" t="str">
-        <v>6703.345</v>
+      <c r="B57">
+        <v>6703.3450000000003</v>
       </c>
       <c r="C57">
         <f>_xll.JsonLookup($A$1,A57)</f>
@@ -3551,8 +3551,8 @@
       <c r="A58" t="str">
         <v>Data.2018-07-09T20:47:00Z</v>
       </c>
-      <c r="B58" t="str">
-        <v>6703.208</v>
+      <c r="B58">
+        <v>6703.2079999999996</v>
       </c>
       <c r="C58">
         <f>_xll.JsonLookup($A$1,A58)</f>
@@ -3563,8 +3563,8 @@
       <c r="A59" t="str">
         <v>Data.2018-07-09T20:48:00Z</v>
       </c>
-      <c r="B59" t="str">
-        <v>6703.218</v>
+      <c r="B59">
+        <v>6703.2179999999998</v>
       </c>
       <c r="C59">
         <f>_xll.JsonLookup($A$1,A59)</f>
@@ -3575,8 +3575,8 @@
       <c r="A60" t="str">
         <v>Data.2018-07-09T20:49:00Z</v>
       </c>
-      <c r="B60" t="str">
-        <v>6703.057</v>
+      <c r="B60">
+        <v>6703.0569999999998</v>
       </c>
       <c r="C60">
         <f>_xll.JsonLookup($A$1,A60)</f>
@@ -3587,8 +3587,8 @@
       <c r="A61" t="str">
         <v>Data.2018-07-09T20:50:00Z</v>
       </c>
-      <c r="B61" t="str">
-        <v>6702.836</v>
+      <c r="B61">
+        <v>6702.8360000000002</v>
       </c>
       <c r="C61">
         <f>_xll.JsonLookup($A$1,A61)</f>
@@ -3599,8 +3599,8 @@
       <c r="A62" t="str">
         <v>Data.2018-07-09T20:51:00Z</v>
       </c>
-      <c r="B62" t="str">
-        <v>6702.379</v>
+      <c r="B62">
+        <v>6702.3789999999999</v>
       </c>
       <c r="C62">
         <f>_xll.JsonLookup($A$1,A62)</f>
@@ -3611,8 +3611,8 @@
       <c r="A63" t="str">
         <v>Data.2018-07-09T20:52:00Z</v>
       </c>
-      <c r="B63" t="str">
-        <v>6702.368</v>
+      <c r="B63">
+        <v>6702.3680000000004</v>
       </c>
       <c r="C63">
         <f>_xll.JsonLookup($A$1,A63)</f>
@@ -3623,8 +3623,8 @@
       <c r="A64" t="str">
         <v>Data.2018-07-09T20:53:00Z</v>
       </c>
-      <c r="B64" t="str">
-        <v>6702.281</v>
+      <c r="B64">
+        <v>6702.2809999999999</v>
       </c>
       <c r="C64">
         <f>_xll.JsonLookup($A$1,A64)</f>
@@ -3635,8 +3635,8 @@
       <c r="A65" t="str">
         <v>Data.2018-07-09T20:54:00Z</v>
       </c>
-      <c r="B65" t="str">
-        <v>6702.017</v>
+      <c r="B65">
+        <v>6702.0169999999998</v>
       </c>
       <c r="C65">
         <f>_xll.JsonLookup($A$1,A65)</f>
@@ -3647,8 +3647,8 @@
       <c r="A66" t="str">
         <v>Data.2018-07-09T20:55:00Z</v>
       </c>
-      <c r="B66" t="str">
-        <v>6701.851</v>
+      <c r="B66">
+        <v>6701.8509999999997</v>
       </c>
       <c r="C66">
         <f>_xll.JsonLookup($A$1,A66)</f>
@@ -3659,7 +3659,7 @@
       <c r="A67" t="str">
         <v>Data.2018-07-09T20:56:00Z</v>
       </c>
-      <c r="B67" t="str">
+      <c r="B67">
         <v>6701.26</v>
       </c>
       <c r="C67">
@@ -3671,8 +3671,8 @@
       <c r="A68" t="str">
         <v>Data.2018-07-09T20:57:00Z</v>
       </c>
-      <c r="B68" t="str">
-        <v>6700.684</v>
+      <c r="B68">
+        <v>6700.6840000000002</v>
       </c>
       <c r="C68">
         <f>_xll.JsonLookup($A$1,A68)</f>
@@ -3683,8 +3683,8 @@
       <c r="A69" t="str">
         <v>Data.2018-07-09T20:58:00Z</v>
       </c>
-      <c r="B69" t="str">
-        <v>6699.999</v>
+      <c r="B69">
+        <v>6699.9989999999998</v>
       </c>
       <c r="C69">
         <f>_xll.JsonLookup($A$1,A69)</f>
@@ -3695,7 +3695,7 @@
       <c r="A70" t="str">
         <v>Data.2018-07-09T20:59:00Z</v>
       </c>
-      <c r="B70" t="str">
+      <c r="B70">
         <v>6699.6</v>
       </c>
       <c r="C70">
@@ -3707,8 +3707,8 @@
       <c r="A71" t="str">
         <v>Data.2018-07-09T21:00:00Z</v>
       </c>
-      <c r="B71" t="str">
-        <v>6699.087</v>
+      <c r="B71">
+        <v>6699.0870000000004</v>
       </c>
       <c r="C71">
         <f>_xll.JsonLookup($A$1,A71)</f>
@@ -3719,8 +3719,8 @@
       <c r="A72" t="str">
         <v>Data.2018-07-09T21:01:00Z</v>
       </c>
-      <c r="B72" t="str">
-        <v>6698.745</v>
+      <c r="B72">
+        <v>6698.7449999999999</v>
       </c>
       <c r="C72">
         <f>_xll.JsonLookup($A$1,A72)</f>
@@ -3731,8 +3731,8 @@
       <c r="A73" t="str">
         <v>Data.2018-07-09T21:02:00Z</v>
       </c>
-      <c r="B73" t="str">
-        <v>6698.449</v>
+      <c r="B73">
+        <v>6698.4489999999996</v>
       </c>
       <c r="C73">
         <f>_xll.JsonLookup($A$1,A73)</f>
@@ -3743,8 +3743,8 @@
       <c r="A74" t="str">
         <v>Data.2018-07-09T21:03:00Z</v>
       </c>
-      <c r="B74" t="str">
-        <v>6698.291</v>
+      <c r="B74">
+        <v>6698.2910000000002</v>
       </c>
       <c r="C74">
         <f>_xll.JsonLookup($A$1,A74)</f>
@@ -3755,8 +3755,8 @@
       <c r="A75" t="str">
         <v>Data.2018-07-09T21:04:00Z</v>
       </c>
-      <c r="B75" t="str">
-        <v>6698.133</v>
+      <c r="B75">
+        <v>6698.1329999999998</v>
       </c>
       <c r="C75">
         <f>_xll.JsonLookup($A$1,A75)</f>
@@ -3767,8 +3767,8 @@
       <c r="A76" t="str">
         <v>Data.2018-07-09T21:05:00Z</v>
       </c>
-      <c r="B76" t="str">
-        <v>6697.738</v>
+      <c r="B76">
+        <v>6697.7380000000003</v>
       </c>
       <c r="C76">
         <f>_xll.JsonLookup($A$1,A76)</f>
@@ -3779,8 +3779,8 @@
       <c r="A77" t="str">
         <v>Data.2018-07-09T21:06:00Z</v>
       </c>
-      <c r="B77" t="str">
-        <v>6697.319</v>
+      <c r="B77">
+        <v>6697.3190000000004</v>
       </c>
       <c r="C77">
         <f>_xll.JsonLookup($A$1,A77)</f>
@@ -3791,8 +3791,8 @@
       <c r="A78" t="str">
         <v>Data.2018-07-09T21:07:00Z</v>
       </c>
-      <c r="B78" t="str">
-        <v>6697.161</v>
+      <c r="B78">
+        <v>6697.1610000000001</v>
       </c>
       <c r="C78">
         <f>_xll.JsonLookup($A$1,A78)</f>
@@ -3803,8 +3803,8 @@
       <c r="A79" t="str">
         <v>Data.2018-07-09T21:08:00Z</v>
       </c>
-      <c r="B79" t="str">
-        <v>6697.445</v>
+      <c r="B79">
+        <v>6697.4449999999997</v>
       </c>
       <c r="C79">
         <f>_xll.JsonLookup($A$1,A79)</f>
@@ -3815,8 +3815,8 @@
       <c r="A80" t="str">
         <v>Data.2018-07-09T21:09:00Z</v>
       </c>
-      <c r="B80" t="str">
-        <v>6697.444</v>
+      <c r="B80">
+        <v>6697.4440000000004</v>
       </c>
       <c r="C80">
         <f>_xll.JsonLookup($A$1,A80)</f>
@@ -3827,7 +3827,7 @@
       <c r="A81" t="str">
         <v>Data.2018-07-09T21:10:00Z</v>
       </c>
-      <c r="B81" t="str">
+      <c r="B81">
         <v>6697.62</v>
       </c>
       <c r="C81">
@@ -3839,8 +3839,8 @@
       <c r="A82" t="str">
         <v>Data.2018-07-09T21:11:00Z</v>
       </c>
-      <c r="B82" t="str">
-        <v>6697.619</v>
+      <c r="B82">
+        <v>6697.6189999999997</v>
       </c>
       <c r="C82">
         <f>_xll.JsonLookup($A$1,A82)</f>
@@ -3851,8 +3851,8 @@
       <c r="A83" t="str">
         <v>Data.2018-07-09T21:12:00Z</v>
       </c>
-      <c r="B83" t="str">
-        <v>6697.642</v>
+      <c r="B83">
+        <v>6697.6419999999998</v>
       </c>
       <c r="C83">
         <f>_xll.JsonLookup($A$1,A83)</f>
@@ -3863,8 +3863,8 @@
       <c r="A84" t="str">
         <v>Data.2018-07-09T21:13:00Z</v>
       </c>
-      <c r="B84" t="str">
-        <v>6697.604</v>
+      <c r="B84">
+        <v>6697.6040000000003</v>
       </c>
       <c r="C84">
         <f>_xll.JsonLookup($A$1,A84)</f>
@@ -3875,8 +3875,8 @@
       <c r="A85" t="str">
         <v>Data.2018-07-09T21:14:00Z</v>
       </c>
-      <c r="B85" t="str">
-        <v>6697.565</v>
+      <c r="B85">
+        <v>6697.5649999999996</v>
       </c>
       <c r="C85">
         <f>_xll.JsonLookup($A$1,A85)</f>
@@ -3887,8 +3887,8 @@
       <c r="A86" t="str">
         <v>Data.2018-07-09T21:15:00Z</v>
       </c>
-      <c r="B86" t="str">
-        <v>6698.039</v>
+      <c r="B86">
+        <v>6698.0389999999998</v>
       </c>
       <c r="C86">
         <f>_xll.JsonLookup($A$1,A86)</f>
@@ -3899,8 +3899,8 @@
       <c r="A87" t="str">
         <v>Data.2018-07-09T21:16:00Z</v>
       </c>
-      <c r="B87" t="str">
-        <v>6698.229</v>
+      <c r="B87">
+        <v>6698.2290000000003</v>
       </c>
       <c r="C87">
         <f>_xll.JsonLookup($A$1,A87)</f>
@@ -3911,8 +3911,8 @@
       <c r="A88" t="str">
         <v>Data.2018-07-09T21:17:00Z</v>
       </c>
-      <c r="B88" t="str">
-        <v>6698.158</v>
+      <c r="B88">
+        <v>6698.1580000000004</v>
       </c>
       <c r="C88">
         <f>_xll.JsonLookup($A$1,A88)</f>
@@ -3923,8 +3923,8 @@
       <c r="A89" t="str">
         <v>Data.2018-07-09T21:18:00Z</v>
       </c>
-      <c r="B89" t="str">
-        <v>6697.995</v>
+      <c r="B89">
+        <v>6697.9949999999999</v>
       </c>
       <c r="C89">
         <f>_xll.JsonLookup($A$1,A89)</f>
@@ -3935,8 +3935,8 @@
       <c r="A90" t="str">
         <v>Data.2018-07-09T21:19:00Z</v>
       </c>
-      <c r="B90" t="str">
-        <v>6698.077</v>
+      <c r="B90">
+        <v>6698.0770000000002</v>
       </c>
       <c r="C90">
         <f>_xll.JsonLookup($A$1,A90)</f>
@@ -3947,7 +3947,7 @@
       <c r="A91" t="str">
         <v>Data.2018-07-09T21:20:00Z</v>
       </c>
-      <c r="B91" t="str">
+      <c r="B91">
         <v>6698.174</v>
       </c>
       <c r="C91">
@@ -3959,8 +3959,8 @@
       <c r="A92" t="str">
         <v>Data.2018-07-09T21:21:00Z</v>
       </c>
-      <c r="B92" t="str">
-        <v>6698.574</v>
+      <c r="B92">
+        <v>6698.5739999999996</v>
       </c>
       <c r="C92">
         <f>_xll.JsonLookup($A$1,A92)</f>
@@ -3971,8 +3971,8 @@
       <c r="A93" t="str">
         <v>Data.2018-07-09T21:22:00Z</v>
       </c>
-      <c r="B93" t="str">
-        <v>6699.397</v>
+      <c r="B93">
+        <v>6699.3969999999999</v>
       </c>
       <c r="C93">
         <f>_xll.JsonLookup($A$1,A93)</f>
@@ -3983,7 +3983,7 @@
       <c r="A94" t="str">
         <v>Data.2018-07-09T21:23:00Z</v>
       </c>
-      <c r="B94" t="str">
+      <c r="B94">
         <v>6700.549</v>
       </c>
       <c r="C94">
@@ -3995,8 +3995,8 @@
       <c r="A95" t="str">
         <v>Data.2018-07-09T21:24:00Z</v>
       </c>
-      <c r="B95" t="str">
-        <v>6701.633</v>
+      <c r="B95">
+        <v>6701.6329999999998</v>
       </c>
       <c r="C95">
         <f>_xll.JsonLookup($A$1,A95)</f>
@@ -4007,8 +4007,8 @@
       <c r="A96" t="str">
         <v>Data.2018-07-09T21:25:00Z</v>
       </c>
-      <c r="B96" t="str">
-        <v>6702.441</v>
+      <c r="B96">
+        <v>6702.4409999999998</v>
       </c>
       <c r="C96">
         <f>_xll.JsonLookup($A$1,A96)</f>
@@ -4019,8 +4019,8 @@
       <c r="A97" t="str">
         <v>Data.2018-07-09T21:26:00Z</v>
       </c>
-      <c r="B97" t="str">
-        <v>6703.554</v>
+      <c r="B97">
+        <v>6703.5540000000001</v>
       </c>
       <c r="C97">
         <f>_xll.JsonLookup($A$1,A97)</f>
@@ -4031,8 +4031,8 @@
       <c r="A98" t="str">
         <v>Data.2018-07-09T21:27:00Z</v>
       </c>
-      <c r="B98" t="str">
-        <v>6704.667</v>
+      <c r="B98">
+        <v>6704.6670000000004</v>
       </c>
       <c r="C98">
         <f>_xll.JsonLookup($A$1,A98)</f>
@@ -4043,8 +4043,8 @@
       <c r="A99" t="str">
         <v>Data.2018-07-09T21:28:00Z</v>
       </c>
-      <c r="B99" t="str">
-        <v>6705.638</v>
+      <c r="B99">
+        <v>6705.6379999999999</v>
       </c>
       <c r="C99">
         <f>_xll.JsonLookup($A$1,A99)</f>
@@ -4055,7 +4055,7 @@
       <c r="A100" t="str">
         <v>Data.2018-07-09T21:29:00Z</v>
       </c>
-      <c r="B100" t="str">
+      <c r="B100">
         <v>6706.43</v>
       </c>
       <c r="C100">
@@ -4067,7 +4067,7 @@
       <c r="A101" t="str">
         <v>Inputs.PERIOD</v>
       </c>
-      <c r="B101" t="str">
+      <c r="B101">
         <v>10</v>
       </c>
       <c r="C101">
@@ -4079,7 +4079,7 @@
       <c r="A102" t="str">
         <v>ModelStartTime</v>
       </c>
-      <c r="B102" t="str">
+      <c r="B102">
         <v>1531157418480</v>
       </c>
       <c r="C102">
@@ -4091,7 +4091,7 @@
       <c r="A103" t="str">
         <v>ModelEndTime</v>
       </c>
-      <c r="B103" t="str">
+      <c r="B103">
         <v>1531157418480</v>
       </c>
       <c r="C103">

</xml_diff>

<commit_message>
better handling of children
</commit_message>
<xml_diff>
--- a/JsonExcel/doc/JsonExcel-test.xlsx
+++ b/JsonExcel/doc/JsonExcel-test.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="P:\OpenSource\JsonExcel\JsonExcel\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FFEB442-95C2-4421-AE08-4D2B2C2752BB}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F9810D7-CEA4-4DCE-87D9-2CEFCCAD4C6B}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="18885" windowHeight="5910" activeTab="2" xr2:uid="{90F70DC4-6E6D-491C-88DA-FF972DBF519E}"/>
   </bookViews>
   <sheets>
     <sheet name="Simple Json" sheetId="1" r:id="rId1"/>
     <sheet name="complex" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet1" sheetId="3" r:id="rId3"/>
+    <sheet name="Timeseries" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="JSON">'Simple Json'!$M$2</definedName>
@@ -147,7 +147,7 @@
     "taglib-location": "/WEB-INF/tlds/cofax.tld"}}}</t>
   </si>
   <si>
-    <t>{"Model":"SMA","TargetTime":"2018-07-09T21:29:00Z","Data":{"2018-07-09T19:56:00Z":6711.49300000,"2018-07-09T19:57:00Z":6711.92000000,"2018-07-09T19:58:00Z":6712.53200000,"2018-07-09T19:59:00Z":6712.43100000,"2018-07-09T20:00:00Z":6711.93400000,"2018-07-09T20:01:00Z":6712.13100000,"2018-07-09T20:02:00Z":6711.98100000,"2018-07-09T20:03:00Z":6711.78100000,"2018-07-09T20:04:00Z":6711.58600000,"2018-07-09T20:05:00Z":6711.13900000,"2018-07-09T20:06:00Z":6710.86200000,"2018-07-09T20:07:00Z":6710.37000000,"2018-07-09T20:08:00Z":6709.85000000,"2018-07-09T20:09:00Z":6709.28700000,"2018-07-09T20:10:00Z":6709.27600000,"2018-07-09T20:11:00Z":6708.48100000,"2018-07-09T20:12:00Z":6707.57700000,"2018-07-09T20:13:00Z":6706.42600000,"2018-07-09T20:14:00Z":6705.26200000,"2018-07-09T20:15:00Z":6704.55500000,"2018-07-09T20:16:00Z":6703.43500000,"2018-07-09T20:17:00Z":6702.49900000,"2018-07-09T20:18:00Z":6701.40600000,"2018-07-09T20:19:00Z":6700.76400000,"2018-07-09T20:20:00Z":6700.17200000,"2018-07-09T20:21:00Z":6700.06800000,"2018-07-09T20:22:00Z":6700.36900000,"2018-07-09T20:23:00Z":6701.09100000,"2018-07-09T20:24:00Z":6701.53800000,"2018-07-09T20:25:00Z":6701.73800000,"2018-07-09T20:26:00Z":6702.11900000,"2018-07-09T20:27:00Z":6702.61900000,"2018-07-09T20:28:00Z":6703.01400000,"2018-07-09T20:29:00Z":6703.00000000,"2018-07-09T20:30:00Z":6702.89900000,"2018-07-09T20:31:00Z":6702.82200000,"2018-07-09T20:32:00Z":6703.14600000,"2018-07-09T20:33:00Z":6702.99600000,"2018-07-09T20:34:00Z":6703.11900000,"2018-07-09T20:35:00Z":6703.50100000,"2018-07-09T20:36:00Z":6703.49700000,"2018-07-09T20:37:00Z":6703.83100000,"2018-07-09T20:38:00Z":6703.92700000,"2018-07-09T20:39:00Z":6704.30700000,"2018-07-09T20:40:00Z":6704.57100000,"2018-07-09T20:41:00Z":6705.04800000,"2018-07-09T20:42:00Z":6704.33200000,"2018-07-09T20:43:00Z":6703.92000000,"2018-07-09T20:44:00Z":6703.68500000,"2018-07-09T20:45:00Z":6703.19000000,"2018-07-09T20:46:00Z":6703.34500000,"2018-07-09T20:47:00Z":6703.20800000,"2018-07-09T20:48:00Z":6703.21800000,"2018-07-09T20:49:00Z":6703.05700000,"2018-07-09T20:50:00Z":6702.83600000,"2018-07-09T20:51:00Z":6702.37900000,"2018-07-09T20:52:00Z":6702.36800000,"2018-07-09T20:53:00Z":6702.28100000,"2018-07-09T20:54:00Z":6702.01700000,"2018-07-09T20:55:00Z":6701.85100000,"2018-07-09T20:56:00Z":6701.26000000,"2018-07-09T20:57:00Z":6700.68400000,"2018-07-09T20:58:00Z":6699.99900000,"2018-07-09T20:59:00Z":6699.60000000,"2018-07-09T21:00:00Z":6699.08700000,"2018-07-09T21:01:00Z":6698.74500000,"2018-07-09T21:02:00Z":6698.44900000,"2018-07-09T21:03:00Z":6698.29100000,"2018-07-09T21:04:00Z":6698.13300000,"2018-07-09T21:05:00Z":6697.73800000,"2018-07-09T21:06:00Z":6697.31900000,"2018-07-09T21:07:00Z":6697.16100000,"2018-07-09T21:08:00Z":6697.44500000,"2018-07-09T21:09:00Z":6697.44400000,"2018-07-09T21:10:00Z":6697.62000000,"2018-07-09T21:11:00Z":6697.61900000,"2018-07-09T21:12:00Z":6697.64200000,"2018-07-09T21:13:00Z":6697.60400000,"2018-07-09T21:14:00Z":6697.56500000,"2018-07-09T21:15:00Z":6698.03900000,"2018-07-09T21:16:00Z":6698.22900000,"2018-07-09T21:17:00Z":6698.15800000,"2018-07-09T21:18:00Z":6697.99500000,"2018-07-09T21:19:00Z":6698.07700000,"2018-07-09T21:20:00Z":6698.17400000,"2018-07-09T21:21:00Z":6698.57400000,"2018-07-09T21:22:00Z":6699.39700000,"2018-07-09T21:23:00Z":6700.54900000,"2018-07-09T21:24:00Z":6701.63300000,"2018-07-09T21:25:00Z":6702.44100000,"2018-07-09T21:26:00Z":6703.55400000,"2018-07-09T21:27:00Z":6704.66700000,"2018-07-09T21:28:00Z":6705.63800000,"2018-07-09T21:29:00Z":6706.43000000},"Inputs":{"PERIOD":10},"ModelStartTime":1531157418480.0,"ModelEndTime":1531157418480.0,"Interval":"OneMinute","Symbol":"BTCUSDT","Source":"BINANCE_KLINE.BTCUSDT.OneMinute"}</t>
+    <t>{"Model":"SMA", "Test": {"k":"v", "k2":"v2"},"TargetTime":"2018-07-09T21:29:00Z","Data":{"2018-07-09T19:56:00Z":6711.49300000,"2018-07-09T19:57:00Z":6711.92000000,"2018-07-09T19:58:00Z":6712.53200000,"2018-07-09T19:59:00Z":6712.43100000,"2018-07-09T20:00:00Z":6711.93400000,"2018-07-09T20:01:00Z":6712.13100000,"2018-07-09T20:02:00Z":6711.98100000,"2018-07-09T20:03:00Z":6711.78100000,"2018-07-09T20:04:00Z":6711.58600000,"2018-07-09T20:05:00Z":6711.13900000,"2018-07-09T20:06:00Z":6710.86200000,"2018-07-09T20:07:00Z":6710.37000000,"2018-07-09T20:08:00Z":6709.85000000,"2018-07-09T20:09:00Z":6709.28700000,"2018-07-09T20:10:00Z":6709.27600000,"2018-07-09T20:11:00Z":6708.48100000,"2018-07-09T20:12:00Z":6707.57700000,"2018-07-09T20:13:00Z":6706.42600000,"2018-07-09T20:14:00Z":6705.26200000,"2018-07-09T20:15:00Z":6704.55500000,"2018-07-09T20:16:00Z":6703.43500000,"2018-07-09T20:17:00Z":6702.49900000,"2018-07-09T20:18:00Z":6701.40600000,"2018-07-09T20:19:00Z":6700.76400000,"2018-07-09T20:20:00Z":6700.17200000,"2018-07-09T20:21:00Z":6700.06800000,"2018-07-09T20:22:00Z":6700.36900000,"2018-07-09T20:23:00Z":6701.09100000,"2018-07-09T20:24:00Z":6701.53800000,"2018-07-09T20:25:00Z":6701.73800000,"2018-07-09T20:26:00Z":6702.11900000,"2018-07-09T20:27:00Z":6702.61900000,"2018-07-09T20:28:00Z":6703.01400000,"2018-07-09T20:29:00Z":6703.00000000,"2018-07-09T20:30:00Z":6702.89900000,"2018-07-09T20:31:00Z":6702.82200000,"2018-07-09T20:32:00Z":6703.14600000,"2018-07-09T20:33:00Z":6702.99600000,"2018-07-09T20:34:00Z":6703.11900000,"2018-07-09T20:35:00Z":6703.50100000,"2018-07-09T20:36:00Z":6703.49700000,"2018-07-09T20:37:00Z":6703.83100000,"2018-07-09T20:38:00Z":6703.92700000,"2018-07-09T20:39:00Z":6704.30700000,"2018-07-09T20:40:00Z":6704.57100000,"2018-07-09T20:41:00Z":6705.04800000,"2018-07-09T20:42:00Z":6704.33200000,"2018-07-09T20:43:00Z":6703.92000000,"2018-07-09T20:44:00Z":6703.68500000,"2018-07-09T20:45:00Z":6703.19000000,"2018-07-09T20:46:00Z":6703.34500000,"2018-07-09T20:47:00Z":6703.20800000,"2018-07-09T20:48:00Z":6703.21800000,"2018-07-09T20:49:00Z":6703.05700000,"2018-07-09T20:50:00Z":6702.83600000,"2018-07-09T20:51:00Z":6702.37900000,"2018-07-09T20:52:00Z":6702.36800000,"2018-07-09T20:53:00Z":6702.28100000,"2018-07-09T20:54:00Z":6702.01700000,"2018-07-09T20:55:00Z":6701.85100000,"2018-07-09T20:56:00Z":6701.26000000,"2018-07-09T20:57:00Z":6700.68400000,"2018-07-09T20:58:00Z":6699.99900000,"2018-07-09T20:59:00Z":6699.60000000,"2018-07-09T21:00:00Z":6699.08700000,"2018-07-09T21:01:00Z":6698.74500000,"2018-07-09T21:02:00Z":6698.44900000,"2018-07-09T21:03:00Z":6698.29100000,"2018-07-09T21:04:00Z":6698.13300000,"2018-07-09T21:05:00Z":6697.73800000,"2018-07-09T21:06:00Z":6697.31900000,"2018-07-09T21:07:00Z":6697.16100000,"2018-07-09T21:08:00Z":6697.44500000,"2018-07-09T21:09:00Z":6697.44400000,"2018-07-09T21:10:00Z":6697.62000000,"2018-07-09T21:11:00Z":6697.61900000,"2018-07-09T21:12:00Z":6697.64200000,"2018-07-09T21:13:00Z":6697.60400000,"2018-07-09T21:14:00Z":6697.56500000,"2018-07-09T21:15:00Z":6698.03900000,"2018-07-09T21:16:00Z":6698.22900000,"2018-07-09T21:17:00Z":6698.15800000,"2018-07-09T21:18:00Z":6697.99500000,"2018-07-09T21:19:00Z":6698.07700000,"2018-07-09T21:20:00Z":6698.17400000,"2018-07-09T21:21:00Z":6698.57400000,"2018-07-09T21:22:00Z":6699.39700000,"2018-07-09T21:23:00Z":6700.54900000,"2018-07-09T21:24:00Z":6701.63300000,"2018-07-09T21:25:00Z":6702.44100000,"2018-07-09T21:26:00Z":6703.55400000,"2018-07-09T21:27:00Z":6704.66700000,"2018-07-09T21:28:00Z":6705.63800000,"2018-07-09T21:29:00Z":6706.43000000},"Inputs":{"PERIOD":10},"ModelStartTime":1531157418480.0,"ModelEndTime":1531157418480.0,"Interval":"OneMinute","Symbol":"BTCUSDT","Source":"BINANCE_KLINE.BTCUSDT.OneMinute"}</t>
   </si>
 </sst>
 </file>
@@ -296,291 +296,291 @@
           </c:marker>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$C$7:$C$100</c:f>
+              <c:f>Timeseries!$C$7:$C$100</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="94"/>
                 <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>43290.895138888889</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>6711.4930000000004</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="3">
                   <c:v>6711.92</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="4">
                   <c:v>6712.5320000000002</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="5">
                   <c:v>6712.4309999999996</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="6">
                   <c:v>6711.9340000000002</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="7">
                   <c:v>6712.1310000000003</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="8">
                   <c:v>6711.9809999999998</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="9">
                   <c:v>6711.7809999999999</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="10">
                   <c:v>6711.5860000000002</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="11">
                   <c:v>6711.1390000000001</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="12">
                   <c:v>6710.8620000000001</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="13">
                   <c:v>6710.37</c:v>
                 </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="14">
                   <c:v>6709.85</c:v>
                 </c:pt>
-                <c:pt idx="13">
+                <c:pt idx="15">
                   <c:v>6709.2870000000003</c:v>
                 </c:pt>
-                <c:pt idx="14">
+                <c:pt idx="16">
                   <c:v>6709.2759999999998</c:v>
                 </c:pt>
-                <c:pt idx="15">
+                <c:pt idx="17">
                   <c:v>6708.4809999999998</c:v>
                 </c:pt>
-                <c:pt idx="16">
+                <c:pt idx="18">
                   <c:v>6707.5770000000002</c:v>
                 </c:pt>
-                <c:pt idx="17">
+                <c:pt idx="19">
                   <c:v>6706.4260000000004</c:v>
                 </c:pt>
-                <c:pt idx="18">
+                <c:pt idx="20">
                   <c:v>6705.2619999999997</c:v>
                 </c:pt>
-                <c:pt idx="19">
+                <c:pt idx="21">
                   <c:v>6704.5550000000003</c:v>
                 </c:pt>
-                <c:pt idx="20">
+                <c:pt idx="22">
                   <c:v>6703.4350000000004</c:v>
                 </c:pt>
-                <c:pt idx="21">
+                <c:pt idx="23">
                   <c:v>6702.4989999999998</c:v>
                 </c:pt>
-                <c:pt idx="22">
+                <c:pt idx="24">
                   <c:v>6701.4059999999999</c:v>
                 </c:pt>
-                <c:pt idx="23">
+                <c:pt idx="25">
                   <c:v>6700.7640000000001</c:v>
                 </c:pt>
-                <c:pt idx="24">
+                <c:pt idx="26">
                   <c:v>6700.1719999999996</c:v>
                 </c:pt>
-                <c:pt idx="25">
+                <c:pt idx="27">
                   <c:v>6700.0680000000002</c:v>
                 </c:pt>
-                <c:pt idx="26">
+                <c:pt idx="28">
                   <c:v>6700.3689999999997</c:v>
                 </c:pt>
-                <c:pt idx="27">
+                <c:pt idx="29">
                   <c:v>6701.0910000000003</c:v>
                 </c:pt>
-                <c:pt idx="28">
+                <c:pt idx="30">
                   <c:v>6701.5379999999996</c:v>
                 </c:pt>
-                <c:pt idx="29">
+                <c:pt idx="31">
                   <c:v>6701.7380000000003</c:v>
                 </c:pt>
-                <c:pt idx="30">
+                <c:pt idx="32">
                   <c:v>6702.1189999999997</c:v>
                 </c:pt>
-                <c:pt idx="31">
+                <c:pt idx="33">
                   <c:v>6702.6189999999997</c:v>
                 </c:pt>
-                <c:pt idx="32">
+                <c:pt idx="34">
                   <c:v>6703.0140000000001</c:v>
                 </c:pt>
-                <c:pt idx="33">
+                <c:pt idx="35">
                   <c:v>6703</c:v>
                 </c:pt>
-                <c:pt idx="34">
+                <c:pt idx="36">
                   <c:v>6702.8990000000003</c:v>
                 </c:pt>
-                <c:pt idx="35">
+                <c:pt idx="37">
                   <c:v>6702.8220000000001</c:v>
                 </c:pt>
-                <c:pt idx="36">
+                <c:pt idx="38">
                   <c:v>6703.1459999999997</c:v>
                 </c:pt>
-                <c:pt idx="37">
+                <c:pt idx="39">
                   <c:v>6702.9960000000001</c:v>
                 </c:pt>
-                <c:pt idx="38">
+                <c:pt idx="40">
                   <c:v>6703.1189999999997</c:v>
                 </c:pt>
-                <c:pt idx="39">
+                <c:pt idx="41">
                   <c:v>6703.5010000000002</c:v>
                 </c:pt>
-                <c:pt idx="40">
+                <c:pt idx="42">
                   <c:v>6703.4970000000003</c:v>
                 </c:pt>
-                <c:pt idx="41">
+                <c:pt idx="43">
                   <c:v>6703.8310000000001</c:v>
                 </c:pt>
-                <c:pt idx="42">
+                <c:pt idx="44">
                   <c:v>6703.9269999999997</c:v>
                 </c:pt>
-                <c:pt idx="43">
+                <c:pt idx="45">
                   <c:v>6704.3069999999998</c:v>
                 </c:pt>
-                <c:pt idx="44">
+                <c:pt idx="46">
                   <c:v>6704.5709999999999</c:v>
                 </c:pt>
-                <c:pt idx="45">
+                <c:pt idx="47">
                   <c:v>6705.0479999999998</c:v>
                 </c:pt>
-                <c:pt idx="46">
+                <c:pt idx="48">
                   <c:v>6704.3320000000003</c:v>
                 </c:pt>
-                <c:pt idx="47">
+                <c:pt idx="49">
                   <c:v>6703.92</c:v>
                 </c:pt>
-                <c:pt idx="48">
+                <c:pt idx="50">
                   <c:v>6703.6850000000004</c:v>
                 </c:pt>
-                <c:pt idx="49">
+                <c:pt idx="51">
                   <c:v>6703.19</c:v>
                 </c:pt>
-                <c:pt idx="50">
+                <c:pt idx="52">
                   <c:v>6703.3450000000003</c:v>
                 </c:pt>
-                <c:pt idx="51">
+                <c:pt idx="53">
                   <c:v>6703.2079999999996</c:v>
                 </c:pt>
-                <c:pt idx="52">
+                <c:pt idx="54">
                   <c:v>6703.2179999999998</c:v>
                 </c:pt>
-                <c:pt idx="53">
+                <c:pt idx="55">
                   <c:v>6703.0569999999998</c:v>
                 </c:pt>
-                <c:pt idx="54">
+                <c:pt idx="56">
                   <c:v>6702.8360000000002</c:v>
                 </c:pt>
-                <c:pt idx="55">
+                <c:pt idx="57">
                   <c:v>6702.3789999999999</c:v>
                 </c:pt>
-                <c:pt idx="56">
+                <c:pt idx="58">
                   <c:v>6702.3680000000004</c:v>
                 </c:pt>
-                <c:pt idx="57">
+                <c:pt idx="59">
                   <c:v>6702.2809999999999</c:v>
                 </c:pt>
-                <c:pt idx="58">
+                <c:pt idx="60">
                   <c:v>6702.0169999999998</c:v>
                 </c:pt>
-                <c:pt idx="59">
+                <c:pt idx="61">
                   <c:v>6701.8509999999997</c:v>
                 </c:pt>
-                <c:pt idx="60">
+                <c:pt idx="62">
                   <c:v>6701.26</c:v>
                 </c:pt>
-                <c:pt idx="61">
+                <c:pt idx="63">
                   <c:v>6700.6840000000002</c:v>
                 </c:pt>
-                <c:pt idx="62">
+                <c:pt idx="64">
                   <c:v>6699.9989999999998</c:v>
                 </c:pt>
-                <c:pt idx="63">
+                <c:pt idx="65">
                   <c:v>6699.6</c:v>
                 </c:pt>
-                <c:pt idx="64">
+                <c:pt idx="66">
                   <c:v>6699.0870000000004</c:v>
                 </c:pt>
-                <c:pt idx="65">
+                <c:pt idx="67">
                   <c:v>6698.7449999999999</c:v>
                 </c:pt>
-                <c:pt idx="66">
+                <c:pt idx="68">
                   <c:v>6698.4489999999996</c:v>
                 </c:pt>
-                <c:pt idx="67">
+                <c:pt idx="69">
                   <c:v>6698.2910000000002</c:v>
                 </c:pt>
-                <c:pt idx="68">
+                <c:pt idx="70">
                   <c:v>6698.1329999999998</c:v>
                 </c:pt>
-                <c:pt idx="69">
+                <c:pt idx="71">
                   <c:v>6697.7380000000003</c:v>
                 </c:pt>
-                <c:pt idx="70">
+                <c:pt idx="72">
                   <c:v>6697.3190000000004</c:v>
                 </c:pt>
-                <c:pt idx="71">
+                <c:pt idx="73">
                   <c:v>6697.1610000000001</c:v>
                 </c:pt>
-                <c:pt idx="72">
+                <c:pt idx="74">
                   <c:v>6697.4449999999997</c:v>
                 </c:pt>
-                <c:pt idx="73">
+                <c:pt idx="75">
                   <c:v>6697.4440000000004</c:v>
                 </c:pt>
-                <c:pt idx="74">
+                <c:pt idx="76">
                   <c:v>6697.62</c:v>
                 </c:pt>
-                <c:pt idx="75">
+                <c:pt idx="77">
                   <c:v>6697.6189999999997</c:v>
                 </c:pt>
-                <c:pt idx="76">
+                <c:pt idx="78">
                   <c:v>6697.6419999999998</c:v>
                 </c:pt>
-                <c:pt idx="77">
+                <c:pt idx="79">
                   <c:v>6697.6040000000003</c:v>
                 </c:pt>
-                <c:pt idx="78">
+                <c:pt idx="80">
                   <c:v>6697.5649999999996</c:v>
                 </c:pt>
-                <c:pt idx="79">
+                <c:pt idx="81">
                   <c:v>6698.0389999999998</c:v>
                 </c:pt>
-                <c:pt idx="80">
+                <c:pt idx="82">
                   <c:v>6698.2290000000003</c:v>
                 </c:pt>
-                <c:pt idx="81">
+                <c:pt idx="83">
                   <c:v>6698.1580000000004</c:v>
                 </c:pt>
-                <c:pt idx="82">
+                <c:pt idx="84">
                   <c:v>6697.9949999999999</c:v>
                 </c:pt>
-                <c:pt idx="83">
+                <c:pt idx="85">
                   <c:v>6698.0770000000002</c:v>
                 </c:pt>
-                <c:pt idx="84">
+                <c:pt idx="86">
                   <c:v>6698.174</c:v>
                 </c:pt>
-                <c:pt idx="85">
+                <c:pt idx="87">
                   <c:v>6698.5739999999996</c:v>
                 </c:pt>
-                <c:pt idx="86">
+                <c:pt idx="88">
                   <c:v>6699.3969999999999</c:v>
                 </c:pt>
-                <c:pt idx="87">
+                <c:pt idx="89">
                   <c:v>6700.549</c:v>
                 </c:pt>
-                <c:pt idx="88">
+                <c:pt idx="90">
                   <c:v>6701.6329999999998</c:v>
                 </c:pt>
-                <c:pt idx="89">
+                <c:pt idx="91">
                   <c:v>6702.4409999999998</c:v>
                 </c:pt>
-                <c:pt idx="90">
+                <c:pt idx="92">
                   <c:v>6703.5540000000001</c:v>
                 </c:pt>
-                <c:pt idx="91">
+                <c:pt idx="93">
                   <c:v>6704.6670000000004</c:v>
-                </c:pt>
-                <c:pt idx="92">
-                  <c:v>6705.6379999999999</c:v>
-                </c:pt>
-                <c:pt idx="93">
-                  <c:v>6706.43</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2891,13 +2891,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{54B4FA4A-253A-4DC7-B007-BD642767BFAD}">
   <dimension ref="A1:D161"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="16.5703125" customWidth="1"/>
+    <col min="1" max="1" width="17.7109375" customWidth="1"/>
+    <col min="2" max="2" width="22.28515625" customWidth="1"/>
     <col min="3" max="3" width="11.85546875" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2918,1245 +2919,1248 @@
         <f>_xll.JsonLookup($A$1,A5)</f>
         <v>SMA</v>
       </c>
-      <c r="D5" t="e">
-        <f>_xll.JsonLookup(A1, "Data")</f>
-        <v>#N/A</v>
-      </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" t="str">
-        <v>TargetTime</v>
-      </c>
-      <c r="B6">
-        <v>43290.895138888889</v>
-      </c>
-      <c r="C6" s="3">
+        <v>Test.k</v>
+      </c>
+      <c r="B6" s="3" t="str">
+        <v>v</v>
+      </c>
+      <c r="C6" s="3" t="str">
         <f>_xll.JsonLookup($A$1,A6)</f>
-        <v>43290.895138888889</v>
+        <v>v</v>
+      </c>
+      <c r="D6" t="str">
+        <f>_xll.JsonLookup(A1,"Test")</f>
+        <v>{_x000D_
+  "k": "v",_x000D_
+  "k2": "v2"_x000D_
+}</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="str">
-        <v>Data.2018-07-09T19:56:00Z</v>
-      </c>
-      <c r="B7">
-        <v>6711.4930000000004</v>
-      </c>
-      <c r="C7">
+        <v>Test.k2</v>
+      </c>
+      <c r="B7" t="str">
+        <v>v2</v>
+      </c>
+      <c r="C7" t="str">
         <f>_xll.JsonLookup($A$1,A7)</f>
-        <v>6711.4930000000004</v>
+        <v>v2</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" t="str">
-        <v>Data.2018-07-09T19:57:00Z</v>
+        <v>TargetTime</v>
       </c>
       <c r="B8">
-        <v>6711.92</v>
+        <v>43290.895138888889</v>
       </c>
       <c r="C8">
         <f>_xll.JsonLookup($A$1,A8)</f>
-        <v>6711.92</v>
+        <v>43290.895138888889</v>
       </c>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" t="str">
-        <v>Data.2018-07-09T19:58:00Z</v>
+        <v>Data.2018-07-09T19:56:00Z</v>
       </c>
       <c r="B9">
-        <v>6712.5320000000002</v>
+        <v>6711.4930000000004</v>
       </c>
       <c r="C9">
         <f>_xll.JsonLookup($A$1,A9)</f>
-        <v>6712.5320000000002</v>
+        <v>6711.4930000000004</v>
       </c>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" t="str">
-        <v>Data.2018-07-09T19:59:00Z</v>
+        <v>Data.2018-07-09T19:57:00Z</v>
       </c>
       <c r="B10">
-        <v>6712.4309999999996</v>
+        <v>6711.92</v>
       </c>
       <c r="C10">
         <f>_xll.JsonLookup($A$1,A10)</f>
-        <v>6712.4309999999996</v>
+        <v>6711.92</v>
       </c>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" t="str">
-        <v>Data.2018-07-09T20:00:00Z</v>
+        <v>Data.2018-07-09T19:58:00Z</v>
       </c>
       <c r="B11">
-        <v>6711.9340000000002</v>
+        <v>6712.5320000000002</v>
       </c>
       <c r="C11">
         <f>_xll.JsonLookup($A$1,A11)</f>
-        <v>6711.9340000000002</v>
+        <v>6712.5320000000002</v>
       </c>
     </row>
     <row r="12" spans="1:4">
       <c r="A12" t="str">
-        <v>Data.2018-07-09T20:01:00Z</v>
+        <v>Data.2018-07-09T19:59:00Z</v>
       </c>
       <c r="B12">
-        <v>6712.1310000000003</v>
+        <v>6712.4309999999996</v>
       </c>
       <c r="C12">
         <f>_xll.JsonLookup($A$1,A12)</f>
-        <v>6712.1310000000003</v>
+        <v>6712.4309999999996</v>
       </c>
     </row>
     <row r="13" spans="1:4">
       <c r="A13" t="str">
-        <v>Data.2018-07-09T20:02:00Z</v>
+        <v>Data.2018-07-09T20:00:00Z</v>
       </c>
       <c r="B13">
-        <v>6711.9809999999998</v>
+        <v>6711.9340000000002</v>
       </c>
       <c r="C13">
         <f>_xll.JsonLookup($A$1,A13)</f>
-        <v>6711.9809999999998</v>
+        <v>6711.9340000000002</v>
       </c>
     </row>
     <row r="14" spans="1:4">
       <c r="A14" t="str">
-        <v>Data.2018-07-09T20:03:00Z</v>
+        <v>Data.2018-07-09T20:01:00Z</v>
       </c>
       <c r="B14">
-        <v>6711.7809999999999</v>
+        <v>6712.1310000000003</v>
       </c>
       <c r="C14">
         <f>_xll.JsonLookup($A$1,A14)</f>
-        <v>6711.7809999999999</v>
+        <v>6712.1310000000003</v>
       </c>
     </row>
     <row r="15" spans="1:4">
       <c r="A15" t="str">
-        <v>Data.2018-07-09T20:04:00Z</v>
+        <v>Data.2018-07-09T20:02:00Z</v>
       </c>
       <c r="B15">
-        <v>6711.5860000000002</v>
+        <v>6711.9809999999998</v>
       </c>
       <c r="C15">
         <f>_xll.JsonLookup($A$1,A15)</f>
-        <v>6711.5860000000002</v>
+        <v>6711.9809999999998</v>
       </c>
     </row>
     <row r="16" spans="1:4">
       <c r="A16" t="str">
-        <v>Data.2018-07-09T20:05:00Z</v>
+        <v>Data.2018-07-09T20:03:00Z</v>
       </c>
       <c r="B16">
-        <v>6711.1390000000001</v>
+        <v>6711.7809999999999</v>
       </c>
       <c r="C16">
         <f>_xll.JsonLookup($A$1,A16)</f>
-        <v>6711.1390000000001</v>
+        <v>6711.7809999999999</v>
       </c>
     </row>
     <row r="17" spans="1:3">
       <c r="A17" t="str">
-        <v>Data.2018-07-09T20:06:00Z</v>
+        <v>Data.2018-07-09T20:04:00Z</v>
       </c>
       <c r="B17">
-        <v>6710.8620000000001</v>
+        <v>6711.5860000000002</v>
       </c>
       <c r="C17">
         <f>_xll.JsonLookup($A$1,A17)</f>
-        <v>6710.8620000000001</v>
+        <v>6711.5860000000002</v>
       </c>
     </row>
     <row r="18" spans="1:3">
       <c r="A18" t="str">
-        <v>Data.2018-07-09T20:07:00Z</v>
+        <v>Data.2018-07-09T20:05:00Z</v>
       </c>
       <c r="B18">
-        <v>6710.37</v>
+        <v>6711.1390000000001</v>
       </c>
       <c r="C18">
         <f>_xll.JsonLookup($A$1,A18)</f>
-        <v>6710.37</v>
+        <v>6711.1390000000001</v>
       </c>
     </row>
     <row r="19" spans="1:3">
       <c r="A19" t="str">
-        <v>Data.2018-07-09T20:08:00Z</v>
+        <v>Data.2018-07-09T20:06:00Z</v>
       </c>
       <c r="B19">
-        <v>6709.85</v>
+        <v>6710.8620000000001</v>
       </c>
       <c r="C19">
         <f>_xll.JsonLookup($A$1,A19)</f>
-        <v>6709.85</v>
+        <v>6710.8620000000001</v>
       </c>
     </row>
     <row r="20" spans="1:3">
       <c r="A20" t="str">
-        <v>Data.2018-07-09T20:09:00Z</v>
+        <v>Data.2018-07-09T20:07:00Z</v>
       </c>
       <c r="B20">
-        <v>6709.2870000000003</v>
+        <v>6710.37</v>
       </c>
       <c r="C20">
         <f>_xll.JsonLookup($A$1,A20)</f>
-        <v>6709.2870000000003</v>
+        <v>6710.37</v>
       </c>
     </row>
     <row r="21" spans="1:3">
       <c r="A21" t="str">
-        <v>Data.2018-07-09T20:10:00Z</v>
+        <v>Data.2018-07-09T20:08:00Z</v>
       </c>
       <c r="B21">
-        <v>6709.2759999999998</v>
+        <v>6709.85</v>
       </c>
       <c r="C21">
         <f>_xll.JsonLookup($A$1,A21)</f>
-        <v>6709.2759999999998</v>
+        <v>6709.85</v>
       </c>
     </row>
     <row r="22" spans="1:3">
       <c r="A22" t="str">
-        <v>Data.2018-07-09T20:11:00Z</v>
+        <v>Data.2018-07-09T20:09:00Z</v>
       </c>
       <c r="B22">
-        <v>6708.4809999999998</v>
+        <v>6709.2870000000003</v>
       </c>
       <c r="C22">
         <f>_xll.JsonLookup($A$1,A22)</f>
-        <v>6708.4809999999998</v>
+        <v>6709.2870000000003</v>
       </c>
     </row>
     <row r="23" spans="1:3">
       <c r="A23" t="str">
-        <v>Data.2018-07-09T20:12:00Z</v>
+        <v>Data.2018-07-09T20:10:00Z</v>
       </c>
       <c r="B23">
-        <v>6707.5770000000002</v>
+        <v>6709.2759999999998</v>
       </c>
       <c r="C23">
         <f>_xll.JsonLookup($A$1,A23)</f>
-        <v>6707.5770000000002</v>
+        <v>6709.2759999999998</v>
       </c>
     </row>
     <row r="24" spans="1:3">
       <c r="A24" t="str">
-        <v>Data.2018-07-09T20:13:00Z</v>
+        <v>Data.2018-07-09T20:11:00Z</v>
       </c>
       <c r="B24">
-        <v>6706.4260000000004</v>
+        <v>6708.4809999999998</v>
       </c>
       <c r="C24">
         <f>_xll.JsonLookup($A$1,A24)</f>
-        <v>6706.4260000000004</v>
+        <v>6708.4809999999998</v>
       </c>
     </row>
     <row r="25" spans="1:3">
       <c r="A25" t="str">
-        <v>Data.2018-07-09T20:14:00Z</v>
+        <v>Data.2018-07-09T20:12:00Z</v>
       </c>
       <c r="B25">
-        <v>6705.2619999999997</v>
+        <v>6707.5770000000002</v>
       </c>
       <c r="C25">
         <f>_xll.JsonLookup($A$1,A25)</f>
-        <v>6705.2619999999997</v>
+        <v>6707.5770000000002</v>
       </c>
     </row>
     <row r="26" spans="1:3">
       <c r="A26" t="str">
-        <v>Data.2018-07-09T20:15:00Z</v>
+        <v>Data.2018-07-09T20:13:00Z</v>
       </c>
       <c r="B26">
-        <v>6704.5550000000003</v>
+        <v>6706.4260000000004</v>
       </c>
       <c r="C26">
         <f>_xll.JsonLookup($A$1,A26)</f>
-        <v>6704.5550000000003</v>
+        <v>6706.4260000000004</v>
       </c>
     </row>
     <row r="27" spans="1:3">
       <c r="A27" t="str">
-        <v>Data.2018-07-09T20:16:00Z</v>
+        <v>Data.2018-07-09T20:14:00Z</v>
       </c>
       <c r="B27">
-        <v>6703.4350000000004</v>
+        <v>6705.2619999999997</v>
       </c>
       <c r="C27">
         <f>_xll.JsonLookup($A$1,A27)</f>
-        <v>6703.4350000000004</v>
+        <v>6705.2619999999997</v>
       </c>
     </row>
     <row r="28" spans="1:3">
       <c r="A28" t="str">
-        <v>Data.2018-07-09T20:17:00Z</v>
+        <v>Data.2018-07-09T20:15:00Z</v>
       </c>
       <c r="B28">
-        <v>6702.4989999999998</v>
+        <v>6704.5550000000003</v>
       </c>
       <c r="C28">
         <f>_xll.JsonLookup($A$1,A28)</f>
-        <v>6702.4989999999998</v>
+        <v>6704.5550000000003</v>
       </c>
     </row>
     <row r="29" spans="1:3">
       <c r="A29" t="str">
-        <v>Data.2018-07-09T20:18:00Z</v>
+        <v>Data.2018-07-09T20:16:00Z</v>
       </c>
       <c r="B29">
-        <v>6701.4059999999999</v>
+        <v>6703.4350000000004</v>
       </c>
       <c r="C29">
         <f>_xll.JsonLookup($A$1,A29)</f>
-        <v>6701.4059999999999</v>
+        <v>6703.4350000000004</v>
       </c>
     </row>
     <row r="30" spans="1:3">
       <c r="A30" t="str">
-        <v>Data.2018-07-09T20:19:00Z</v>
+        <v>Data.2018-07-09T20:17:00Z</v>
       </c>
       <c r="B30">
-        <v>6700.7640000000001</v>
+        <v>6702.4989999999998</v>
       </c>
       <c r="C30">
         <f>_xll.JsonLookup($A$1,A30)</f>
-        <v>6700.7640000000001</v>
+        <v>6702.4989999999998</v>
       </c>
     </row>
     <row r="31" spans="1:3">
       <c r="A31" t="str">
-        <v>Data.2018-07-09T20:20:00Z</v>
+        <v>Data.2018-07-09T20:18:00Z</v>
       </c>
       <c r="B31">
-        <v>6700.1719999999996</v>
+        <v>6701.4059999999999</v>
       </c>
       <c r="C31">
         <f>_xll.JsonLookup($A$1,A31)</f>
-        <v>6700.1719999999996</v>
+        <v>6701.4059999999999</v>
       </c>
     </row>
     <row r="32" spans="1:3">
       <c r="A32" t="str">
-        <v>Data.2018-07-09T20:21:00Z</v>
+        <v>Data.2018-07-09T20:19:00Z</v>
       </c>
       <c r="B32">
-        <v>6700.0680000000002</v>
+        <v>6700.7640000000001</v>
       </c>
       <c r="C32">
         <f>_xll.JsonLookup($A$1,A32)</f>
-        <v>6700.0680000000002</v>
+        <v>6700.7640000000001</v>
       </c>
     </row>
     <row r="33" spans="1:3">
       <c r="A33" t="str">
-        <v>Data.2018-07-09T20:22:00Z</v>
+        <v>Data.2018-07-09T20:20:00Z</v>
       </c>
       <c r="B33">
-        <v>6700.3689999999997</v>
+        <v>6700.1719999999996</v>
       </c>
       <c r="C33">
         <f>_xll.JsonLookup($A$1,A33)</f>
-        <v>6700.3689999999997</v>
+        <v>6700.1719999999996</v>
       </c>
     </row>
     <row r="34" spans="1:3">
       <c r="A34" t="str">
-        <v>Data.2018-07-09T20:23:00Z</v>
+        <v>Data.2018-07-09T20:21:00Z</v>
       </c>
       <c r="B34">
-        <v>6701.0910000000003</v>
+        <v>6700.0680000000002</v>
       </c>
       <c r="C34">
         <f>_xll.JsonLookup($A$1,A34)</f>
-        <v>6701.0910000000003</v>
+        <v>6700.0680000000002</v>
       </c>
     </row>
     <row r="35" spans="1:3">
       <c r="A35" t="str">
-        <v>Data.2018-07-09T20:24:00Z</v>
+        <v>Data.2018-07-09T20:22:00Z</v>
       </c>
       <c r="B35">
-        <v>6701.5379999999996</v>
+        <v>6700.3689999999997</v>
       </c>
       <c r="C35">
         <f>_xll.JsonLookup($A$1,A35)</f>
-        <v>6701.5379999999996</v>
+        <v>6700.3689999999997</v>
       </c>
     </row>
     <row r="36" spans="1:3">
       <c r="A36" t="str">
-        <v>Data.2018-07-09T20:25:00Z</v>
+        <v>Data.2018-07-09T20:23:00Z</v>
       </c>
       <c r="B36">
-        <v>6701.7380000000003</v>
+        <v>6701.0910000000003</v>
       </c>
       <c r="C36">
         <f>_xll.JsonLookup($A$1,A36)</f>
-        <v>6701.7380000000003</v>
+        <v>6701.0910000000003</v>
       </c>
     </row>
     <row r="37" spans="1:3">
       <c r="A37" t="str">
-        <v>Data.2018-07-09T20:26:00Z</v>
+        <v>Data.2018-07-09T20:24:00Z</v>
       </c>
       <c r="B37">
-        <v>6702.1189999999997</v>
+        <v>6701.5379999999996</v>
       </c>
       <c r="C37">
         <f>_xll.JsonLookup($A$1,A37)</f>
-        <v>6702.1189999999997</v>
+        <v>6701.5379999999996</v>
       </c>
     </row>
     <row r="38" spans="1:3">
       <c r="A38" t="str">
-        <v>Data.2018-07-09T20:27:00Z</v>
+        <v>Data.2018-07-09T20:25:00Z</v>
       </c>
       <c r="B38">
-        <v>6702.6189999999997</v>
+        <v>6701.7380000000003</v>
       </c>
       <c r="C38">
         <f>_xll.JsonLookup($A$1,A38)</f>
-        <v>6702.6189999999997</v>
+        <v>6701.7380000000003</v>
       </c>
     </row>
     <row r="39" spans="1:3">
       <c r="A39" t="str">
-        <v>Data.2018-07-09T20:28:00Z</v>
+        <v>Data.2018-07-09T20:26:00Z</v>
       </c>
       <c r="B39">
-        <v>6703.0140000000001</v>
+        <v>6702.1189999999997</v>
       </c>
       <c r="C39">
         <f>_xll.JsonLookup($A$1,A39)</f>
-        <v>6703.0140000000001</v>
+        <v>6702.1189999999997</v>
       </c>
     </row>
     <row r="40" spans="1:3">
       <c r="A40" t="str">
-        <v>Data.2018-07-09T20:29:00Z</v>
+        <v>Data.2018-07-09T20:27:00Z</v>
       </c>
       <c r="B40">
-        <v>6703</v>
+        <v>6702.6189999999997</v>
       </c>
       <c r="C40">
         <f>_xll.JsonLookup($A$1,A40)</f>
-        <v>6703</v>
+        <v>6702.6189999999997</v>
       </c>
     </row>
     <row r="41" spans="1:3">
       <c r="A41" t="str">
-        <v>Data.2018-07-09T20:30:00Z</v>
+        <v>Data.2018-07-09T20:28:00Z</v>
       </c>
       <c r="B41">
-        <v>6702.8990000000003</v>
+        <v>6703.0140000000001</v>
       </c>
       <c r="C41">
         <f>_xll.JsonLookup($A$1,A41)</f>
-        <v>6702.8990000000003</v>
+        <v>6703.0140000000001</v>
       </c>
     </row>
     <row r="42" spans="1:3">
       <c r="A42" t="str">
-        <v>Data.2018-07-09T20:31:00Z</v>
+        <v>Data.2018-07-09T20:29:00Z</v>
       </c>
       <c r="B42">
-        <v>6702.8220000000001</v>
+        <v>6703</v>
       </c>
       <c r="C42">
         <f>_xll.JsonLookup($A$1,A42)</f>
-        <v>6702.8220000000001</v>
+        <v>6703</v>
       </c>
     </row>
     <row r="43" spans="1:3">
       <c r="A43" t="str">
-        <v>Data.2018-07-09T20:32:00Z</v>
+        <v>Data.2018-07-09T20:30:00Z</v>
       </c>
       <c r="B43">
-        <v>6703.1459999999997</v>
+        <v>6702.8990000000003</v>
       </c>
       <c r="C43">
         <f>_xll.JsonLookup($A$1,A43)</f>
-        <v>6703.1459999999997</v>
+        <v>6702.8990000000003</v>
       </c>
     </row>
     <row r="44" spans="1:3">
       <c r="A44" t="str">
-        <v>Data.2018-07-09T20:33:00Z</v>
+        <v>Data.2018-07-09T20:31:00Z</v>
       </c>
       <c r="B44">
-        <v>6702.9960000000001</v>
+        <v>6702.8220000000001</v>
       </c>
       <c r="C44">
         <f>_xll.JsonLookup($A$1,A44)</f>
-        <v>6702.9960000000001</v>
+        <v>6702.8220000000001</v>
       </c>
     </row>
     <row r="45" spans="1:3">
       <c r="A45" t="str">
-        <v>Data.2018-07-09T20:34:00Z</v>
+        <v>Data.2018-07-09T20:32:00Z</v>
       </c>
       <c r="B45">
-        <v>6703.1189999999997</v>
+        <v>6703.1459999999997</v>
       </c>
       <c r="C45">
         <f>_xll.JsonLookup($A$1,A45)</f>
-        <v>6703.1189999999997</v>
+        <v>6703.1459999999997</v>
       </c>
     </row>
     <row r="46" spans="1:3">
       <c r="A46" t="str">
-        <v>Data.2018-07-09T20:35:00Z</v>
+        <v>Data.2018-07-09T20:33:00Z</v>
       </c>
       <c r="B46">
-        <v>6703.5010000000002</v>
+        <v>6702.9960000000001</v>
       </c>
       <c r="C46">
         <f>_xll.JsonLookup($A$1,A46)</f>
-        <v>6703.5010000000002</v>
+        <v>6702.9960000000001</v>
       </c>
     </row>
     <row r="47" spans="1:3">
       <c r="A47" t="str">
-        <v>Data.2018-07-09T20:36:00Z</v>
+        <v>Data.2018-07-09T20:34:00Z</v>
       </c>
       <c r="B47">
-        <v>6703.4970000000003</v>
+        <v>6703.1189999999997</v>
       </c>
       <c r="C47">
         <f>_xll.JsonLookup($A$1,A47)</f>
-        <v>6703.4970000000003</v>
+        <v>6703.1189999999997</v>
       </c>
     </row>
     <row r="48" spans="1:3">
       <c r="A48" t="str">
-        <v>Data.2018-07-09T20:37:00Z</v>
+        <v>Data.2018-07-09T20:35:00Z</v>
       </c>
       <c r="B48">
-        <v>6703.8310000000001</v>
+        <v>6703.5010000000002</v>
       </c>
       <c r="C48">
         <f>_xll.JsonLookup($A$1,A48)</f>
-        <v>6703.8310000000001</v>
+        <v>6703.5010000000002</v>
       </c>
     </row>
     <row r="49" spans="1:3">
       <c r="A49" t="str">
-        <v>Data.2018-07-09T20:38:00Z</v>
+        <v>Data.2018-07-09T20:36:00Z</v>
       </c>
       <c r="B49">
-        <v>6703.9269999999997</v>
+        <v>6703.4970000000003</v>
       </c>
       <c r="C49">
         <f>_xll.JsonLookup($A$1,A49)</f>
-        <v>6703.9269999999997</v>
+        <v>6703.4970000000003</v>
       </c>
     </row>
     <row r="50" spans="1:3">
       <c r="A50" t="str">
-        <v>Data.2018-07-09T20:39:00Z</v>
+        <v>Data.2018-07-09T20:37:00Z</v>
       </c>
       <c r="B50">
-        <v>6704.3069999999998</v>
+        <v>6703.8310000000001</v>
       </c>
       <c r="C50">
         <f>_xll.JsonLookup($A$1,A50)</f>
-        <v>6704.3069999999998</v>
+        <v>6703.8310000000001</v>
       </c>
     </row>
     <row r="51" spans="1:3">
       <c r="A51" t="str">
-        <v>Data.2018-07-09T20:40:00Z</v>
+        <v>Data.2018-07-09T20:38:00Z</v>
       </c>
       <c r="B51">
-        <v>6704.5709999999999</v>
+        <v>6703.9269999999997</v>
       </c>
       <c r="C51">
         <f>_xll.JsonLookup($A$1,A51)</f>
-        <v>6704.5709999999999</v>
+        <v>6703.9269999999997</v>
       </c>
     </row>
     <row r="52" spans="1:3">
       <c r="A52" t="str">
-        <v>Data.2018-07-09T20:41:00Z</v>
+        <v>Data.2018-07-09T20:39:00Z</v>
       </c>
       <c r="B52">
-        <v>6705.0479999999998</v>
+        <v>6704.3069999999998</v>
       </c>
       <c r="C52">
         <f>_xll.JsonLookup($A$1,A52)</f>
-        <v>6705.0479999999998</v>
+        <v>6704.3069999999998</v>
       </c>
     </row>
     <row r="53" spans="1:3">
       <c r="A53" t="str">
-        <v>Data.2018-07-09T20:42:00Z</v>
+        <v>Data.2018-07-09T20:40:00Z</v>
       </c>
       <c r="B53">
-        <v>6704.3320000000003</v>
+        <v>6704.5709999999999</v>
       </c>
       <c r="C53">
         <f>_xll.JsonLookup($A$1,A53)</f>
-        <v>6704.3320000000003</v>
+        <v>6704.5709999999999</v>
       </c>
     </row>
     <row r="54" spans="1:3">
       <c r="A54" t="str">
-        <v>Data.2018-07-09T20:43:00Z</v>
+        <v>Data.2018-07-09T20:41:00Z</v>
       </c>
       <c r="B54">
-        <v>6703.92</v>
+        <v>6705.0479999999998</v>
       </c>
       <c r="C54">
         <f>_xll.JsonLookup($A$1,A54)</f>
-        <v>6703.92</v>
+        <v>6705.0479999999998</v>
       </c>
     </row>
     <row r="55" spans="1:3">
       <c r="A55" t="str">
-        <v>Data.2018-07-09T20:44:00Z</v>
+        <v>Data.2018-07-09T20:42:00Z</v>
       </c>
       <c r="B55">
-        <v>6703.6850000000004</v>
+        <v>6704.3320000000003</v>
       </c>
       <c r="C55">
         <f>_xll.JsonLookup($A$1,A55)</f>
-        <v>6703.6850000000004</v>
+        <v>6704.3320000000003</v>
       </c>
     </row>
     <row r="56" spans="1:3">
       <c r="A56" t="str">
-        <v>Data.2018-07-09T20:45:00Z</v>
+        <v>Data.2018-07-09T20:43:00Z</v>
       </c>
       <c r="B56">
-        <v>6703.19</v>
+        <v>6703.92</v>
       </c>
       <c r="C56">
         <f>_xll.JsonLookup($A$1,A56)</f>
-        <v>6703.19</v>
+        <v>6703.92</v>
       </c>
     </row>
     <row r="57" spans="1:3">
       <c r="A57" t="str">
-        <v>Data.2018-07-09T20:46:00Z</v>
+        <v>Data.2018-07-09T20:44:00Z</v>
       </c>
       <c r="B57">
-        <v>6703.3450000000003</v>
+        <v>6703.6850000000004</v>
       </c>
       <c r="C57">
         <f>_xll.JsonLookup($A$1,A57)</f>
-        <v>6703.3450000000003</v>
+        <v>6703.6850000000004</v>
       </c>
     </row>
     <row r="58" spans="1:3">
       <c r="A58" t="str">
-        <v>Data.2018-07-09T20:47:00Z</v>
+        <v>Data.2018-07-09T20:45:00Z</v>
       </c>
       <c r="B58">
-        <v>6703.2079999999996</v>
+        <v>6703.19</v>
       </c>
       <c r="C58">
         <f>_xll.JsonLookup($A$1,A58)</f>
-        <v>6703.2079999999996</v>
+        <v>6703.19</v>
       </c>
     </row>
     <row r="59" spans="1:3">
       <c r="A59" t="str">
-        <v>Data.2018-07-09T20:48:00Z</v>
+        <v>Data.2018-07-09T20:46:00Z</v>
       </c>
       <c r="B59">
-        <v>6703.2179999999998</v>
+        <v>6703.3450000000003</v>
       </c>
       <c r="C59">
         <f>_xll.JsonLookup($A$1,A59)</f>
-        <v>6703.2179999999998</v>
+        <v>6703.3450000000003</v>
       </c>
     </row>
     <row r="60" spans="1:3">
       <c r="A60" t="str">
-        <v>Data.2018-07-09T20:49:00Z</v>
+        <v>Data.2018-07-09T20:47:00Z</v>
       </c>
       <c r="B60">
-        <v>6703.0569999999998</v>
+        <v>6703.2079999999996</v>
       </c>
       <c r="C60">
         <f>_xll.JsonLookup($A$1,A60)</f>
-        <v>6703.0569999999998</v>
+        <v>6703.2079999999996</v>
       </c>
     </row>
     <row r="61" spans="1:3">
       <c r="A61" t="str">
-        <v>Data.2018-07-09T20:50:00Z</v>
+        <v>Data.2018-07-09T20:48:00Z</v>
       </c>
       <c r="B61">
-        <v>6702.8360000000002</v>
+        <v>6703.2179999999998</v>
       </c>
       <c r="C61">
         <f>_xll.JsonLookup($A$1,A61)</f>
-        <v>6702.8360000000002</v>
+        <v>6703.2179999999998</v>
       </c>
     </row>
     <row r="62" spans="1:3">
       <c r="A62" t="str">
-        <v>Data.2018-07-09T20:51:00Z</v>
+        <v>Data.2018-07-09T20:49:00Z</v>
       </c>
       <c r="B62">
-        <v>6702.3789999999999</v>
+        <v>6703.0569999999998</v>
       </c>
       <c r="C62">
         <f>_xll.JsonLookup($A$1,A62)</f>
-        <v>6702.3789999999999</v>
+        <v>6703.0569999999998</v>
       </c>
     </row>
     <row r="63" spans="1:3">
       <c r="A63" t="str">
-        <v>Data.2018-07-09T20:52:00Z</v>
+        <v>Data.2018-07-09T20:50:00Z</v>
       </c>
       <c r="B63">
-        <v>6702.3680000000004</v>
+        <v>6702.8360000000002</v>
       </c>
       <c r="C63">
         <f>_xll.JsonLookup($A$1,A63)</f>
-        <v>6702.3680000000004</v>
+        <v>6702.8360000000002</v>
       </c>
     </row>
     <row r="64" spans="1:3">
       <c r="A64" t="str">
-        <v>Data.2018-07-09T20:53:00Z</v>
+        <v>Data.2018-07-09T20:51:00Z</v>
       </c>
       <c r="B64">
-        <v>6702.2809999999999</v>
+        <v>6702.3789999999999</v>
       </c>
       <c r="C64">
         <f>_xll.JsonLookup($A$1,A64)</f>
-        <v>6702.2809999999999</v>
+        <v>6702.3789999999999</v>
       </c>
     </row>
     <row r="65" spans="1:3">
       <c r="A65" t="str">
-        <v>Data.2018-07-09T20:54:00Z</v>
+        <v>Data.2018-07-09T20:52:00Z</v>
       </c>
       <c r="B65">
-        <v>6702.0169999999998</v>
+        <v>6702.3680000000004</v>
       </c>
       <c r="C65">
         <f>_xll.JsonLookup($A$1,A65)</f>
-        <v>6702.0169999999998</v>
+        <v>6702.3680000000004</v>
       </c>
     </row>
     <row r="66" spans="1:3">
       <c r="A66" t="str">
-        <v>Data.2018-07-09T20:55:00Z</v>
+        <v>Data.2018-07-09T20:53:00Z</v>
       </c>
       <c r="B66">
-        <v>6701.8509999999997</v>
+        <v>6702.2809999999999</v>
       </c>
       <c r="C66">
         <f>_xll.JsonLookup($A$1,A66)</f>
-        <v>6701.8509999999997</v>
+        <v>6702.2809999999999</v>
       </c>
     </row>
     <row r="67" spans="1:3">
       <c r="A67" t="str">
-        <v>Data.2018-07-09T20:56:00Z</v>
+        <v>Data.2018-07-09T20:54:00Z</v>
       </c>
       <c r="B67">
-        <v>6701.26</v>
+        <v>6702.0169999999998</v>
       </c>
       <c r="C67">
         <f>_xll.JsonLookup($A$1,A67)</f>
-        <v>6701.26</v>
+        <v>6702.0169999999998</v>
       </c>
     </row>
     <row r="68" spans="1:3">
       <c r="A68" t="str">
-        <v>Data.2018-07-09T20:57:00Z</v>
+        <v>Data.2018-07-09T20:55:00Z</v>
       </c>
       <c r="B68">
-        <v>6700.6840000000002</v>
+        <v>6701.8509999999997</v>
       </c>
       <c r="C68">
         <f>_xll.JsonLookup($A$1,A68)</f>
-        <v>6700.6840000000002</v>
+        <v>6701.8509999999997</v>
       </c>
     </row>
     <row r="69" spans="1:3">
       <c r="A69" t="str">
-        <v>Data.2018-07-09T20:58:00Z</v>
+        <v>Data.2018-07-09T20:56:00Z</v>
       </c>
       <c r="B69">
-        <v>6699.9989999999998</v>
+        <v>6701.26</v>
       </c>
       <c r="C69">
         <f>_xll.JsonLookup($A$1,A69)</f>
-        <v>6699.9989999999998</v>
+        <v>6701.26</v>
       </c>
     </row>
     <row r="70" spans="1:3">
       <c r="A70" t="str">
-        <v>Data.2018-07-09T20:59:00Z</v>
+        <v>Data.2018-07-09T20:57:00Z</v>
       </c>
       <c r="B70">
-        <v>6699.6</v>
+        <v>6700.6840000000002</v>
       </c>
       <c r="C70">
         <f>_xll.JsonLookup($A$1,A70)</f>
-        <v>6699.6</v>
+        <v>6700.6840000000002</v>
       </c>
     </row>
     <row r="71" spans="1:3">
       <c r="A71" t="str">
-        <v>Data.2018-07-09T21:00:00Z</v>
+        <v>Data.2018-07-09T20:58:00Z</v>
       </c>
       <c r="B71">
-        <v>6699.0870000000004</v>
+        <v>6699.9989999999998</v>
       </c>
       <c r="C71">
         <f>_xll.JsonLookup($A$1,A71)</f>
-        <v>6699.0870000000004</v>
+        <v>6699.9989999999998</v>
       </c>
     </row>
     <row r="72" spans="1:3">
       <c r="A72" t="str">
-        <v>Data.2018-07-09T21:01:00Z</v>
+        <v>Data.2018-07-09T20:59:00Z</v>
       </c>
       <c r="B72">
-        <v>6698.7449999999999</v>
+        <v>6699.6</v>
       </c>
       <c r="C72">
         <f>_xll.JsonLookup($A$1,A72)</f>
-        <v>6698.7449999999999</v>
+        <v>6699.6</v>
       </c>
     </row>
     <row r="73" spans="1:3">
       <c r="A73" t="str">
-        <v>Data.2018-07-09T21:02:00Z</v>
+        <v>Data.2018-07-09T21:00:00Z</v>
       </c>
       <c r="B73">
-        <v>6698.4489999999996</v>
+        <v>6699.0870000000004</v>
       </c>
       <c r="C73">
         <f>_xll.JsonLookup($A$1,A73)</f>
-        <v>6698.4489999999996</v>
+        <v>6699.0870000000004</v>
       </c>
     </row>
     <row r="74" spans="1:3">
       <c r="A74" t="str">
-        <v>Data.2018-07-09T21:03:00Z</v>
+        <v>Data.2018-07-09T21:01:00Z</v>
       </c>
       <c r="B74">
-        <v>6698.2910000000002</v>
+        <v>6698.7449999999999</v>
       </c>
       <c r="C74">
         <f>_xll.JsonLookup($A$1,A74)</f>
-        <v>6698.2910000000002</v>
+        <v>6698.7449999999999</v>
       </c>
     </row>
     <row r="75" spans="1:3">
       <c r="A75" t="str">
-        <v>Data.2018-07-09T21:04:00Z</v>
+        <v>Data.2018-07-09T21:02:00Z</v>
       </c>
       <c r="B75">
-        <v>6698.1329999999998</v>
+        <v>6698.4489999999996</v>
       </c>
       <c r="C75">
         <f>_xll.JsonLookup($A$1,A75)</f>
-        <v>6698.1329999999998</v>
+        <v>6698.4489999999996</v>
       </c>
     </row>
     <row r="76" spans="1:3">
       <c r="A76" t="str">
-        <v>Data.2018-07-09T21:05:00Z</v>
+        <v>Data.2018-07-09T21:03:00Z</v>
       </c>
       <c r="B76">
-        <v>6697.7380000000003</v>
+        <v>6698.2910000000002</v>
       </c>
       <c r="C76">
         <f>_xll.JsonLookup($A$1,A76)</f>
-        <v>6697.7380000000003</v>
+        <v>6698.2910000000002</v>
       </c>
     </row>
     <row r="77" spans="1:3">
       <c r="A77" t="str">
-        <v>Data.2018-07-09T21:06:00Z</v>
+        <v>Data.2018-07-09T21:04:00Z</v>
       </c>
       <c r="B77">
-        <v>6697.3190000000004</v>
+        <v>6698.1329999999998</v>
       </c>
       <c r="C77">
         <f>_xll.JsonLookup($A$1,A77)</f>
-        <v>6697.3190000000004</v>
+        <v>6698.1329999999998</v>
       </c>
     </row>
     <row r="78" spans="1:3">
       <c r="A78" t="str">
-        <v>Data.2018-07-09T21:07:00Z</v>
+        <v>Data.2018-07-09T21:05:00Z</v>
       </c>
       <c r="B78">
-        <v>6697.1610000000001</v>
+        <v>6697.7380000000003</v>
       </c>
       <c r="C78">
         <f>_xll.JsonLookup($A$1,A78)</f>
-        <v>6697.1610000000001</v>
+        <v>6697.7380000000003</v>
       </c>
     </row>
     <row r="79" spans="1:3">
       <c r="A79" t="str">
-        <v>Data.2018-07-09T21:08:00Z</v>
+        <v>Data.2018-07-09T21:06:00Z</v>
       </c>
       <c r="B79">
-        <v>6697.4449999999997</v>
+        <v>6697.3190000000004</v>
       </c>
       <c r="C79">
         <f>_xll.JsonLookup($A$1,A79)</f>
-        <v>6697.4449999999997</v>
+        <v>6697.3190000000004</v>
       </c>
     </row>
     <row r="80" spans="1:3">
       <c r="A80" t="str">
-        <v>Data.2018-07-09T21:09:00Z</v>
+        <v>Data.2018-07-09T21:07:00Z</v>
       </c>
       <c r="B80">
-        <v>6697.4440000000004</v>
+        <v>6697.1610000000001</v>
       </c>
       <c r="C80">
         <f>_xll.JsonLookup($A$1,A80)</f>
-        <v>6697.4440000000004</v>
+        <v>6697.1610000000001</v>
       </c>
     </row>
     <row r="81" spans="1:3">
       <c r="A81" t="str">
-        <v>Data.2018-07-09T21:10:00Z</v>
+        <v>Data.2018-07-09T21:08:00Z</v>
       </c>
       <c r="B81">
-        <v>6697.62</v>
+        <v>6697.4449999999997</v>
       </c>
       <c r="C81">
         <f>_xll.JsonLookup($A$1,A81)</f>
-        <v>6697.62</v>
+        <v>6697.4449999999997</v>
       </c>
     </row>
     <row r="82" spans="1:3">
       <c r="A82" t="str">
-        <v>Data.2018-07-09T21:11:00Z</v>
+        <v>Data.2018-07-09T21:09:00Z</v>
       </c>
       <c r="B82">
-        <v>6697.6189999999997</v>
+        <v>6697.4440000000004</v>
       </c>
       <c r="C82">
         <f>_xll.JsonLookup($A$1,A82)</f>
-        <v>6697.6189999999997</v>
+        <v>6697.4440000000004</v>
       </c>
     </row>
     <row r="83" spans="1:3">
       <c r="A83" t="str">
-        <v>Data.2018-07-09T21:12:00Z</v>
+        <v>Data.2018-07-09T21:10:00Z</v>
       </c>
       <c r="B83">
-        <v>6697.6419999999998</v>
+        <v>6697.62</v>
       </c>
       <c r="C83">
         <f>_xll.JsonLookup($A$1,A83)</f>
-        <v>6697.6419999999998</v>
+        <v>6697.62</v>
       </c>
     </row>
     <row r="84" spans="1:3">
       <c r="A84" t="str">
-        <v>Data.2018-07-09T21:13:00Z</v>
+        <v>Data.2018-07-09T21:11:00Z</v>
       </c>
       <c r="B84">
-        <v>6697.6040000000003</v>
+        <v>6697.6189999999997</v>
       </c>
       <c r="C84">
         <f>_xll.JsonLookup($A$1,A84)</f>
-        <v>6697.6040000000003</v>
+        <v>6697.6189999999997</v>
       </c>
     </row>
     <row r="85" spans="1:3">
       <c r="A85" t="str">
-        <v>Data.2018-07-09T21:14:00Z</v>
+        <v>Data.2018-07-09T21:12:00Z</v>
       </c>
       <c r="B85">
-        <v>6697.5649999999996</v>
+        <v>6697.6419999999998</v>
       </c>
       <c r="C85">
         <f>_xll.JsonLookup($A$1,A85)</f>
-        <v>6697.5649999999996</v>
+        <v>6697.6419999999998</v>
       </c>
     </row>
     <row r="86" spans="1:3">
       <c r="A86" t="str">
-        <v>Data.2018-07-09T21:15:00Z</v>
+        <v>Data.2018-07-09T21:13:00Z</v>
       </c>
       <c r="B86">
-        <v>6698.0389999999998</v>
+        <v>6697.6040000000003</v>
       </c>
       <c r="C86">
         <f>_xll.JsonLookup($A$1,A86)</f>
-        <v>6698.0389999999998</v>
+        <v>6697.6040000000003</v>
       </c>
     </row>
     <row r="87" spans="1:3">
       <c r="A87" t="str">
-        <v>Data.2018-07-09T21:16:00Z</v>
+        <v>Data.2018-07-09T21:14:00Z</v>
       </c>
       <c r="B87">
-        <v>6698.2290000000003</v>
+        <v>6697.5649999999996</v>
       </c>
       <c r="C87">
         <f>_xll.JsonLookup($A$1,A87)</f>
-        <v>6698.2290000000003</v>
+        <v>6697.5649999999996</v>
       </c>
     </row>
     <row r="88" spans="1:3">
       <c r="A88" t="str">
-        <v>Data.2018-07-09T21:17:00Z</v>
+        <v>Data.2018-07-09T21:15:00Z</v>
       </c>
       <c r="B88">
-        <v>6698.1580000000004</v>
+        <v>6698.0389999999998</v>
       </c>
       <c r="C88">
         <f>_xll.JsonLookup($A$1,A88)</f>
-        <v>6698.1580000000004</v>
+        <v>6698.0389999999998</v>
       </c>
     </row>
     <row r="89" spans="1:3">
       <c r="A89" t="str">
-        <v>Data.2018-07-09T21:18:00Z</v>
+        <v>Data.2018-07-09T21:16:00Z</v>
       </c>
       <c r="B89">
-        <v>6697.9949999999999</v>
+        <v>6698.2290000000003</v>
       </c>
       <c r="C89">
         <f>_xll.JsonLookup($A$1,A89)</f>
-        <v>6697.9949999999999</v>
+        <v>6698.2290000000003</v>
       </c>
     </row>
     <row r="90" spans="1:3">
       <c r="A90" t="str">
-        <v>Data.2018-07-09T21:19:00Z</v>
+        <v>Data.2018-07-09T21:17:00Z</v>
       </c>
       <c r="B90">
-        <v>6698.0770000000002</v>
+        <v>6698.1580000000004</v>
       </c>
       <c r="C90">
         <f>_xll.JsonLookup($A$1,A90)</f>
-        <v>6698.0770000000002</v>
+        <v>6698.1580000000004</v>
       </c>
     </row>
     <row r="91" spans="1:3">
       <c r="A91" t="str">
-        <v>Data.2018-07-09T21:20:00Z</v>
+        <v>Data.2018-07-09T21:18:00Z</v>
       </c>
       <c r="B91">
-        <v>6698.174</v>
+        <v>6697.9949999999999</v>
       </c>
       <c r="C91">
         <f>_xll.JsonLookup($A$1,A91)</f>
-        <v>6698.174</v>
+        <v>6697.9949999999999</v>
       </c>
     </row>
     <row r="92" spans="1:3">
       <c r="A92" t="str">
-        <v>Data.2018-07-09T21:21:00Z</v>
+        <v>Data.2018-07-09T21:19:00Z</v>
       </c>
       <c r="B92">
-        <v>6698.5739999999996</v>
+        <v>6698.0770000000002</v>
       </c>
       <c r="C92">
         <f>_xll.JsonLookup($A$1,A92)</f>
-        <v>6698.5739999999996</v>
+        <v>6698.0770000000002</v>
       </c>
     </row>
     <row r="93" spans="1:3">
       <c r="A93" t="str">
-        <v>Data.2018-07-09T21:22:00Z</v>
+        <v>Data.2018-07-09T21:20:00Z</v>
       </c>
       <c r="B93">
-        <v>6699.3969999999999</v>
+        <v>6698.174</v>
       </c>
       <c r="C93">
         <f>_xll.JsonLookup($A$1,A93)</f>
-        <v>6699.3969999999999</v>
+        <v>6698.174</v>
       </c>
     </row>
     <row r="94" spans="1:3">
       <c r="A94" t="str">
-        <v>Data.2018-07-09T21:23:00Z</v>
+        <v>Data.2018-07-09T21:21:00Z</v>
       </c>
       <c r="B94">
-        <v>6700.549</v>
+        <v>6698.5739999999996</v>
       </c>
       <c r="C94">
         <f>_xll.JsonLookup($A$1,A94)</f>
-        <v>6700.549</v>
+        <v>6698.5739999999996</v>
       </c>
     </row>
     <row r="95" spans="1:3">
       <c r="A95" t="str">
-        <v>Data.2018-07-09T21:24:00Z</v>
+        <v>Data.2018-07-09T21:22:00Z</v>
       </c>
       <c r="B95">
-        <v>6701.6329999999998</v>
+        <v>6699.3969999999999</v>
       </c>
       <c r="C95">
         <f>_xll.JsonLookup($A$1,A95)</f>
-        <v>6701.6329999999998</v>
+        <v>6699.3969999999999</v>
       </c>
     </row>
     <row r="96" spans="1:3">
       <c r="A96" t="str">
-        <v>Data.2018-07-09T21:25:00Z</v>
+        <v>Data.2018-07-09T21:23:00Z</v>
       </c>
       <c r="B96">
-        <v>6702.4409999999998</v>
+        <v>6700.549</v>
       </c>
       <c r="C96">
         <f>_xll.JsonLookup($A$1,A96)</f>
-        <v>6702.4409999999998</v>
+        <v>6700.549</v>
       </c>
     </row>
     <row r="97" spans="1:3">
       <c r="A97" t="str">
-        <v>Data.2018-07-09T21:26:00Z</v>
+        <v>Data.2018-07-09T21:24:00Z</v>
       </c>
       <c r="B97">
-        <v>6703.5540000000001</v>
+        <v>6701.6329999999998</v>
       </c>
       <c r="C97">
         <f>_xll.JsonLookup($A$1,A97)</f>
-        <v>6703.5540000000001</v>
+        <v>6701.6329999999998</v>
       </c>
     </row>
     <row r="98" spans="1:3">
       <c r="A98" t="str">
-        <v>Data.2018-07-09T21:27:00Z</v>
+        <v>Data.2018-07-09T21:25:00Z</v>
       </c>
       <c r="B98">
-        <v>6704.6670000000004</v>
+        <v>6702.4409999999998</v>
       </c>
       <c r="C98">
         <f>_xll.JsonLookup($A$1,A98)</f>
-        <v>6704.6670000000004</v>
+        <v>6702.4409999999998</v>
       </c>
     </row>
     <row r="99" spans="1:3">
       <c r="A99" t="str">
-        <v>Data.2018-07-09T21:28:00Z</v>
+        <v>Data.2018-07-09T21:26:00Z</v>
       </c>
       <c r="B99">
-        <v>6705.6379999999999</v>
+        <v>6703.5540000000001</v>
       </c>
       <c r="C99">
         <f>_xll.JsonLookup($A$1,A99)</f>
-        <v>6705.6379999999999</v>
+        <v>6703.5540000000001</v>
       </c>
     </row>
     <row r="100" spans="1:3">
       <c r="A100" t="str">
-        <v>Data.2018-07-09T21:29:00Z</v>
+        <v>Data.2018-07-09T21:27:00Z</v>
       </c>
       <c r="B100">
-        <v>6706.43</v>
+        <v>6704.6670000000004</v>
       </c>
       <c r="C100">
         <f>_xll.JsonLookup($A$1,A100)</f>
-        <v>6706.43</v>
+        <v>6704.6670000000004</v>
       </c>
     </row>
     <row r="101" spans="1:3">
       <c r="A101" t="str">
-        <v>Inputs.PERIOD</v>
+        <v>Data.2018-07-09T21:28:00Z</v>
       </c>
       <c r="B101">
-        <v>10</v>
+        <v>6705.6379999999999</v>
       </c>
       <c r="C101">
         <f>_xll.JsonLookup($A$1,A101)</f>
-        <v>10</v>
+        <v>6705.6379999999999</v>
       </c>
     </row>
     <row r="102" spans="1:3">
       <c r="A102" t="str">
-        <v>ModelStartTime</v>
+        <v>Data.2018-07-09T21:29:00Z</v>
       </c>
       <c r="B102">
-        <v>1531157418480</v>
+        <v>6706.43</v>
       </c>
       <c r="C102">
         <f>_xll.JsonLookup($A$1,A102)</f>
-        <v>1531157418480</v>
+        <v>6706.43</v>
       </c>
     </row>
     <row r="103" spans="1:3">
       <c r="A103" t="str">
-        <v>ModelEndTime</v>
+        <v>Inputs.PERIOD</v>
       </c>
       <c r="B103">
-        <v>1531157418480</v>
+        <v>10</v>
       </c>
       <c r="C103">
         <f>_xll.JsonLookup($A$1,A103)</f>
-        <v>1531157418480</v>
+        <v>10</v>
       </c>
     </row>
     <row r="104" spans="1:3">
       <c r="A104" t="str">
-        <v>Interval</v>
-      </c>
-      <c r="B104" t="str">
-        <v>OneMinute</v>
-      </c>
-      <c r="C104" t="str">
+        <v>ModelStartTime</v>
+      </c>
+      <c r="B104">
+        <v>1531157418480</v>
+      </c>
+      <c r="C104">
         <f>_xll.JsonLookup($A$1,A104)</f>
-        <v>OneMinute</v>
+        <v>1531157418480</v>
       </c>
     </row>
     <row r="105" spans="1:3">
       <c r="A105" t="str">
-        <v>Symbol</v>
-      </c>
-      <c r="B105" t="str">
-        <v>BTCUSDT</v>
-      </c>
-      <c r="C105" t="str">
+        <v>ModelEndTime</v>
+      </c>
+      <c r="B105">
+        <v>1531157418480</v>
+      </c>
+      <c r="C105">
         <f>_xll.JsonLookup($A$1,A105)</f>
-        <v>BTCUSDT</v>
+        <v>1531157418480</v>
       </c>
     </row>
     <row r="106" spans="1:3">
       <c r="A106" t="str">
-        <v>Source</v>
+        <v>Interval</v>
       </c>
       <c r="B106" t="str">
-        <v>BINANCE_KLINE.BTCUSDT.OneMinute</v>
+        <v>OneMinute</v>
       </c>
       <c r="C106" t="str">
         <f>_xll.JsonLookup($A$1,A106)</f>
+        <v>OneMinute</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3">
+      <c r="A107" t="str">
+        <v>Symbol</v>
+      </c>
+      <c r="B107" t="str">
+        <v>BTCUSDT</v>
+      </c>
+      <c r="C107" t="str">
+        <f>_xll.JsonLookup($A$1,A107)</f>
+        <v>BTCUSDT</v>
+      </c>
+    </row>
+    <row r="108" spans="1:3">
+      <c r="A108" t="str">
+        <v>Source</v>
+      </c>
+      <c r="B108" t="str">
         <v>BINANCE_KLINE.BTCUSDT.OneMinute</v>
       </c>
-    </row>
-    <row r="107" spans="1:3">
-      <c r="A107" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="B107" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="C107" t="e">
-        <f>_xll.JsonLookup($A$1,A107)</f>
-        <v>#VALUE!</v>
-      </c>
-    </row>
-    <row r="108" spans="1:3">
-      <c r="A108" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="B108" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="C108" t="e">
+      <c r="C108" t="str">
         <f>_xll.JsonLookup($A$1,A108)</f>
-        <v>#VALUE!</v>
+        <v>BINANCE_KLINE.BTCUSDT.OneMinute</v>
       </c>
     </row>
     <row r="109" spans="1:3">

</xml_diff>

<commit_message>
support for json arrays
</commit_message>
<xml_diff>
--- a/JsonExcel/doc/JsonExcel-test.xlsx
+++ b/JsonExcel/doc/JsonExcel-test.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="P:\OpenSource\JsonExcel\JsonExcel\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F9810D7-CEA4-4DCE-87D9-2CEFCCAD4C6B}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F86B41BD-385A-42A6-9943-DC9975470ED6}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18885" windowHeight="5910" activeTab="2" xr2:uid="{90F70DC4-6E6D-491C-88DA-FF972DBF519E}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18885" windowHeight="5910" activeTab="3" xr2:uid="{90F70DC4-6E6D-491C-88DA-FF972DBF519E}"/>
   </bookViews>
   <sheets>
     <sheet name="Simple Json" sheetId="1" r:id="rId1"/>
     <sheet name="complex" sheetId="2" r:id="rId2"/>
     <sheet name="Timeseries" sheetId="3" r:id="rId3"/>
+    <sheet name="Array" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="JSON">'Simple Json'!$M$2</definedName>
@@ -25,12 +26,17 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>bbb</t>
   </si>
@@ -148,6 +154,9 @@
   </si>
   <si>
     <t>{"Model":"SMA", "Test": {"k":"v", "k2":"v2"},"TargetTime":"2018-07-09T21:29:00Z","Data":{"2018-07-09T19:56:00Z":6711.49300000,"2018-07-09T19:57:00Z":6711.92000000,"2018-07-09T19:58:00Z":6712.53200000,"2018-07-09T19:59:00Z":6712.43100000,"2018-07-09T20:00:00Z":6711.93400000,"2018-07-09T20:01:00Z":6712.13100000,"2018-07-09T20:02:00Z":6711.98100000,"2018-07-09T20:03:00Z":6711.78100000,"2018-07-09T20:04:00Z":6711.58600000,"2018-07-09T20:05:00Z":6711.13900000,"2018-07-09T20:06:00Z":6710.86200000,"2018-07-09T20:07:00Z":6710.37000000,"2018-07-09T20:08:00Z":6709.85000000,"2018-07-09T20:09:00Z":6709.28700000,"2018-07-09T20:10:00Z":6709.27600000,"2018-07-09T20:11:00Z":6708.48100000,"2018-07-09T20:12:00Z":6707.57700000,"2018-07-09T20:13:00Z":6706.42600000,"2018-07-09T20:14:00Z":6705.26200000,"2018-07-09T20:15:00Z":6704.55500000,"2018-07-09T20:16:00Z":6703.43500000,"2018-07-09T20:17:00Z":6702.49900000,"2018-07-09T20:18:00Z":6701.40600000,"2018-07-09T20:19:00Z":6700.76400000,"2018-07-09T20:20:00Z":6700.17200000,"2018-07-09T20:21:00Z":6700.06800000,"2018-07-09T20:22:00Z":6700.36900000,"2018-07-09T20:23:00Z":6701.09100000,"2018-07-09T20:24:00Z":6701.53800000,"2018-07-09T20:25:00Z":6701.73800000,"2018-07-09T20:26:00Z":6702.11900000,"2018-07-09T20:27:00Z":6702.61900000,"2018-07-09T20:28:00Z":6703.01400000,"2018-07-09T20:29:00Z":6703.00000000,"2018-07-09T20:30:00Z":6702.89900000,"2018-07-09T20:31:00Z":6702.82200000,"2018-07-09T20:32:00Z":6703.14600000,"2018-07-09T20:33:00Z":6702.99600000,"2018-07-09T20:34:00Z":6703.11900000,"2018-07-09T20:35:00Z":6703.50100000,"2018-07-09T20:36:00Z":6703.49700000,"2018-07-09T20:37:00Z":6703.83100000,"2018-07-09T20:38:00Z":6703.92700000,"2018-07-09T20:39:00Z":6704.30700000,"2018-07-09T20:40:00Z":6704.57100000,"2018-07-09T20:41:00Z":6705.04800000,"2018-07-09T20:42:00Z":6704.33200000,"2018-07-09T20:43:00Z":6703.92000000,"2018-07-09T20:44:00Z":6703.68500000,"2018-07-09T20:45:00Z":6703.19000000,"2018-07-09T20:46:00Z":6703.34500000,"2018-07-09T20:47:00Z":6703.20800000,"2018-07-09T20:48:00Z":6703.21800000,"2018-07-09T20:49:00Z":6703.05700000,"2018-07-09T20:50:00Z":6702.83600000,"2018-07-09T20:51:00Z":6702.37900000,"2018-07-09T20:52:00Z":6702.36800000,"2018-07-09T20:53:00Z":6702.28100000,"2018-07-09T20:54:00Z":6702.01700000,"2018-07-09T20:55:00Z":6701.85100000,"2018-07-09T20:56:00Z":6701.26000000,"2018-07-09T20:57:00Z":6700.68400000,"2018-07-09T20:58:00Z":6699.99900000,"2018-07-09T20:59:00Z":6699.60000000,"2018-07-09T21:00:00Z":6699.08700000,"2018-07-09T21:01:00Z":6698.74500000,"2018-07-09T21:02:00Z":6698.44900000,"2018-07-09T21:03:00Z":6698.29100000,"2018-07-09T21:04:00Z":6698.13300000,"2018-07-09T21:05:00Z":6697.73800000,"2018-07-09T21:06:00Z":6697.31900000,"2018-07-09T21:07:00Z":6697.16100000,"2018-07-09T21:08:00Z":6697.44500000,"2018-07-09T21:09:00Z":6697.44400000,"2018-07-09T21:10:00Z":6697.62000000,"2018-07-09T21:11:00Z":6697.61900000,"2018-07-09T21:12:00Z":6697.64200000,"2018-07-09T21:13:00Z":6697.60400000,"2018-07-09T21:14:00Z":6697.56500000,"2018-07-09T21:15:00Z":6698.03900000,"2018-07-09T21:16:00Z":6698.22900000,"2018-07-09T21:17:00Z":6698.15800000,"2018-07-09T21:18:00Z":6697.99500000,"2018-07-09T21:19:00Z":6698.07700000,"2018-07-09T21:20:00Z":6698.17400000,"2018-07-09T21:21:00Z":6698.57400000,"2018-07-09T21:22:00Z":6699.39700000,"2018-07-09T21:23:00Z":6700.54900000,"2018-07-09T21:24:00Z":6701.63300000,"2018-07-09T21:25:00Z":6702.44100000,"2018-07-09T21:26:00Z":6703.55400000,"2018-07-09T21:27:00Z":6704.66700000,"2018-07-09T21:28:00Z":6705.63800000,"2018-07-09T21:29:00Z":6706.43000000},"Inputs":{"PERIOD":10},"ModelStartTime":1531157418480.0,"ModelEndTime":1531157418480.0,"Interval":"OneMinute","Symbol":"BTCUSDT","Source":"BINANCE_KLINE.BTCUSDT.OneMinute"}</t>
+  </si>
+  <si>
+    <t>["aaa","bbb","cccc"]</t>
   </si>
 </sst>
 </file>
@@ -273,7 +282,7 @@
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:spPr>
-            <a:ln w="19050" cap="rnd">
+            <a:ln w="25400" cap="rnd">
               <a:noFill/>
               <a:round/>
             </a:ln>
@@ -296,291 +305,291 @@
           </c:marker>
           <c:yVal>
             <c:numRef>
-              <c:f>Timeseries!$C$7:$C$100</c:f>
+              <c:f>Timeseries!$F$9:$F$102</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="94"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>6711.4930000000004</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>43290.895138888889</c:v>
+                  <c:v>6711.92</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>6711.4930000000004</c:v>
+                  <c:v>6712.5320000000002</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>6711.92</c:v>
+                  <c:v>6712.4309999999996</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>6712.5320000000002</c:v>
+                  <c:v>6711.9340000000002</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>6712.4309999999996</c:v>
+                  <c:v>6712.1310000000003</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>6711.9340000000002</c:v>
+                  <c:v>6711.9809999999998</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>6712.1310000000003</c:v>
+                  <c:v>6711.7809999999999</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>6711.9809999999998</c:v>
+                  <c:v>6711.5860000000002</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>6711.7809999999999</c:v>
+                  <c:v>6711.1390000000001</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>6711.5860000000002</c:v>
+                  <c:v>6710.8620000000001</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>6711.1390000000001</c:v>
+                  <c:v>6710.37</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>6710.8620000000001</c:v>
+                  <c:v>6709.85</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>6710.37</c:v>
+                  <c:v>6709.2870000000003</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>6709.85</c:v>
+                  <c:v>6709.2759999999998</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>6709.2870000000003</c:v>
+                  <c:v>6708.4809999999998</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>6709.2759999999998</c:v>
+                  <c:v>6707.5770000000002</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>6708.4809999999998</c:v>
+                  <c:v>6706.4260000000004</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>6707.5770000000002</c:v>
+                  <c:v>6705.2619999999997</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>6706.4260000000004</c:v>
+                  <c:v>6704.5550000000003</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>6705.2619999999997</c:v>
+                  <c:v>6703.4350000000004</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>6704.5550000000003</c:v>
+                  <c:v>6702.4989999999998</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>6703.4350000000004</c:v>
+                  <c:v>6701.4059999999999</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>6702.4989999999998</c:v>
+                  <c:v>6700.7640000000001</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>6701.4059999999999</c:v>
+                  <c:v>6700.1719999999996</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>6700.7640000000001</c:v>
+                  <c:v>6700.0680000000002</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>6700.1719999999996</c:v>
+                  <c:v>6700.3689999999997</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>6700.0680000000002</c:v>
+                  <c:v>6701.0910000000003</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>6700.3689999999997</c:v>
+                  <c:v>6701.5379999999996</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>6701.0910000000003</c:v>
+                  <c:v>6701.7380000000003</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>6701.5379999999996</c:v>
+                  <c:v>6702.1189999999997</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>6701.7380000000003</c:v>
+                  <c:v>6702.6189999999997</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>6702.1189999999997</c:v>
+                  <c:v>6703.0140000000001</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>6702.6189999999997</c:v>
+                  <c:v>6703</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>6703.0140000000001</c:v>
+                  <c:v>6702.8990000000003</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>6703</c:v>
+                  <c:v>6702.8220000000001</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>6702.8990000000003</c:v>
+                  <c:v>6703.1459999999997</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>6702.8220000000001</c:v>
+                  <c:v>6702.9960000000001</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>6703.1459999999997</c:v>
+                  <c:v>6703.1189999999997</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>6702.9960000000001</c:v>
+                  <c:v>6703.5010000000002</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>6703.1189999999997</c:v>
+                  <c:v>6703.4970000000003</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>6703.5010000000002</c:v>
+                  <c:v>6703.8310000000001</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>6703.4970000000003</c:v>
+                  <c:v>6703.9269999999997</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>6703.8310000000001</c:v>
+                  <c:v>6704.3069999999998</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>6703.9269999999997</c:v>
+                  <c:v>6704.5709999999999</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>6704.3069999999998</c:v>
+                  <c:v>6705.0479999999998</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>6704.5709999999999</c:v>
+                  <c:v>6704.3320000000003</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>6705.0479999999998</c:v>
+                  <c:v>6703.92</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>6704.3320000000003</c:v>
+                  <c:v>6703.6850000000004</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>6703.92</c:v>
+                  <c:v>6703.19</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>6703.6850000000004</c:v>
+                  <c:v>6703.3450000000003</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>6703.19</c:v>
+                  <c:v>6703.2079999999996</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>6703.3450000000003</c:v>
+                  <c:v>6703.2179999999998</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>6703.2079999999996</c:v>
+                  <c:v>6703.0569999999998</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>6703.2179999999998</c:v>
+                  <c:v>6702.8360000000002</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>6703.0569999999998</c:v>
+                  <c:v>6702.3789999999999</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>6702.8360000000002</c:v>
+                  <c:v>6702.3680000000004</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>6702.3789999999999</c:v>
+                  <c:v>6702.2809999999999</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>6702.3680000000004</c:v>
+                  <c:v>6702.0169999999998</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>6702.2809999999999</c:v>
+                  <c:v>6701.8509999999997</c:v>
                 </c:pt>
                 <c:pt idx="60">
-                  <c:v>6702.0169999999998</c:v>
+                  <c:v>6701.26</c:v>
                 </c:pt>
                 <c:pt idx="61">
-                  <c:v>6701.8509999999997</c:v>
+                  <c:v>6700.6840000000002</c:v>
                 </c:pt>
                 <c:pt idx="62">
-                  <c:v>6701.26</c:v>
+                  <c:v>6699.9989999999998</c:v>
                 </c:pt>
                 <c:pt idx="63">
-                  <c:v>6700.6840000000002</c:v>
+                  <c:v>6699.6</c:v>
                 </c:pt>
                 <c:pt idx="64">
-                  <c:v>6699.9989999999998</c:v>
+                  <c:v>6699.0870000000004</c:v>
                 </c:pt>
                 <c:pt idx="65">
-                  <c:v>6699.6</c:v>
+                  <c:v>6698.7449999999999</c:v>
                 </c:pt>
                 <c:pt idx="66">
-                  <c:v>6699.0870000000004</c:v>
+                  <c:v>6698.4489999999996</c:v>
                 </c:pt>
                 <c:pt idx="67">
-                  <c:v>6698.7449999999999</c:v>
+                  <c:v>6698.2910000000002</c:v>
                 </c:pt>
                 <c:pt idx="68">
-                  <c:v>6698.4489999999996</c:v>
+                  <c:v>6698.1329999999998</c:v>
                 </c:pt>
                 <c:pt idx="69">
-                  <c:v>6698.2910000000002</c:v>
+                  <c:v>6697.7380000000003</c:v>
                 </c:pt>
                 <c:pt idx="70">
-                  <c:v>6698.1329999999998</c:v>
+                  <c:v>6697.3190000000004</c:v>
                 </c:pt>
                 <c:pt idx="71">
-                  <c:v>6697.7380000000003</c:v>
+                  <c:v>6697.1610000000001</c:v>
                 </c:pt>
                 <c:pt idx="72">
-                  <c:v>6697.3190000000004</c:v>
+                  <c:v>6697.4449999999997</c:v>
                 </c:pt>
                 <c:pt idx="73">
-                  <c:v>6697.1610000000001</c:v>
+                  <c:v>6697.4440000000004</c:v>
                 </c:pt>
                 <c:pt idx="74">
-                  <c:v>6697.4449999999997</c:v>
+                  <c:v>6697.62</c:v>
                 </c:pt>
                 <c:pt idx="75">
-                  <c:v>6697.4440000000004</c:v>
+                  <c:v>6697.6189999999997</c:v>
                 </c:pt>
                 <c:pt idx="76">
-                  <c:v>6697.62</c:v>
+                  <c:v>6697.6419999999998</c:v>
                 </c:pt>
                 <c:pt idx="77">
-                  <c:v>6697.6189999999997</c:v>
+                  <c:v>6697.6040000000003</c:v>
                 </c:pt>
                 <c:pt idx="78">
-                  <c:v>6697.6419999999998</c:v>
+                  <c:v>6697.5649999999996</c:v>
                 </c:pt>
                 <c:pt idx="79">
-                  <c:v>6697.6040000000003</c:v>
+                  <c:v>6698.0389999999998</c:v>
                 </c:pt>
                 <c:pt idx="80">
-                  <c:v>6697.5649999999996</c:v>
+                  <c:v>6698.2290000000003</c:v>
                 </c:pt>
                 <c:pt idx="81">
-                  <c:v>6698.0389999999998</c:v>
+                  <c:v>6698.1580000000004</c:v>
                 </c:pt>
                 <c:pt idx="82">
-                  <c:v>6698.2290000000003</c:v>
+                  <c:v>6697.9949999999999</c:v>
                 </c:pt>
                 <c:pt idx="83">
-                  <c:v>6698.1580000000004</c:v>
+                  <c:v>6698.0770000000002</c:v>
                 </c:pt>
                 <c:pt idx="84">
-                  <c:v>6697.9949999999999</c:v>
+                  <c:v>6698.174</c:v>
                 </c:pt>
                 <c:pt idx="85">
-                  <c:v>6698.0770000000002</c:v>
+                  <c:v>6698.5739999999996</c:v>
                 </c:pt>
                 <c:pt idx="86">
-                  <c:v>6698.174</c:v>
+                  <c:v>6699.3969999999999</c:v>
                 </c:pt>
                 <c:pt idx="87">
-                  <c:v>6698.5739999999996</c:v>
+                  <c:v>6700.549</c:v>
                 </c:pt>
                 <c:pt idx="88">
-                  <c:v>6699.3969999999999</c:v>
+                  <c:v>6701.6329999999998</c:v>
                 </c:pt>
                 <c:pt idx="89">
-                  <c:v>6700.549</c:v>
+                  <c:v>6702.4409999999998</c:v>
                 </c:pt>
                 <c:pt idx="90">
-                  <c:v>6701.6329999999998</c:v>
+                  <c:v>6703.5540000000001</c:v>
                 </c:pt>
                 <c:pt idx="91">
-                  <c:v>6702.4409999999998</c:v>
+                  <c:v>6704.6670000000004</c:v>
                 </c:pt>
                 <c:pt idx="92">
-                  <c:v>6703.5540000000001</c:v>
+                  <c:v>6705.6379999999999</c:v>
                 </c:pt>
                 <c:pt idx="93">
-                  <c:v>6704.6670000000004</c:v>
+                  <c:v>6706.43</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1338,16 +1347,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>533400</xdr:colOff>
-      <xdr:row>84</xdr:row>
-      <xdr:rowOff>23812</xdr:rowOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>57149</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>228600</xdr:colOff>
-      <xdr:row>98</xdr:row>
-      <xdr:rowOff>100012</xdr:rowOff>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>9524</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>114299</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1675,7 +1684,7 @@
   <dimension ref="C1:M14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L6" sqref="L6"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1693,8 +1702,8 @@
         <v>6</v>
       </c>
       <c r="M2" t="str">
-        <f>"{ 'aaaa': 123,'bbb': 456,3: 789}"</f>
-        <v>{ 'aaaa': 123,'bbb': 456,3: 789}</v>
+        <f>"{ 'aaaa': 124,'bbb': 456,3: 789}"</f>
+        <v>{ 'aaaa': 124,'bbb': 456,3: 789}</v>
       </c>
     </row>
     <row r="4" spans="3:13">
@@ -1713,8 +1722,8 @@
         <f t="array" ref="C5:E8">_xll.JsonToArray(JSON)</f>
         <v>aaaa</v>
       </c>
-      <c r="D5" t="str">
-        <v>123</v>
+      <c r="D5">
+        <v>124</v>
       </c>
       <c r="E5" t="e">
         <v>#N/A</v>
@@ -1731,26 +1740,26 @@
       </c>
       <c r="L5" t="str">
         <f>_xll.JsonFromCells(C5:E8)</f>
-        <v>{"aaaa":"123","bbb":"456","3":"789"}</v>
+        <v>{"aaaa":124.0,"bbb":456.0,"3":789.0}</v>
       </c>
     </row>
     <row r="6" spans="3:13">
       <c r="C6" t="str">
         <v>bbb</v>
       </c>
-      <c r="D6" t="str">
+      <c r="D6">
         <v>456</v>
       </c>
       <c r="E6" t="e">
         <v>#N/A</v>
       </c>
-      <c r="G6" t="str">
-        <v>123</v>
-      </c>
-      <c r="H6" t="str">
+      <c r="G6">
+        <v>124</v>
+      </c>
+      <c r="H6">
         <v>456</v>
       </c>
-      <c r="I6" t="str">
+      <c r="I6">
         <v>789</v>
       </c>
     </row>
@@ -1758,7 +1767,7 @@
       <c r="C7" t="str">
         <v>3</v>
       </c>
-      <c r="D7" t="str">
+      <c r="D7">
         <v>789</v>
       </c>
       <c r="E7" t="e">
@@ -1822,7 +1831,7 @@
       <c r="C14">
         <v>3</v>
       </c>
-      <c r="D14" t="str">
+      <c r="D14">
         <f>_xll.JsonLookup(JSON,$C14)</f>
         <v>789</v>
       </c>
@@ -1836,8 +1845,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{476E53B7-47D8-4C73-9AFD-D21323878C5A}">
   <dimension ref="A1:E89"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView topLeftCell="A55" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2025,12 +2034,12 @@
       <c r="C14" t="str">
         <v>web-app.servlet[0].init-param.useJSP</v>
       </c>
-      <c r="D14" t="str">
-        <v>False</v>
-      </c>
-      <c r="E14" t="str">
+      <c r="D14" t="b">
+        <v>0</v>
+      </c>
+      <c r="E14" t="b">
         <f>_xll.JsonLookup($A$1,C14)</f>
-        <v>False</v>
+        <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:5">
@@ -2064,10 +2073,10 @@
       <c r="C17" t="str">
         <v>web-app.servlet[0].init-param.cachePackageTagsTrack</v>
       </c>
-      <c r="D17" t="str">
+      <c r="D17">
         <v>200</v>
       </c>
-      <c r="E17" t="str">
+      <c r="E17">
         <f>_xll.JsonLookup($A$1,C17)</f>
         <v>200</v>
       </c>
@@ -2077,10 +2086,10 @@
       <c r="C18" t="str">
         <v>web-app.servlet[0].init-param.cachePackageTagsStore</v>
       </c>
-      <c r="D18" t="str">
+      <c r="D18">
         <v>200</v>
       </c>
-      <c r="E18" t="str">
+      <c r="E18">
         <f>_xll.JsonLookup($A$1,C18)</f>
         <v>200</v>
       </c>
@@ -2090,10 +2099,10 @@
       <c r="C19" t="str">
         <v>web-app.servlet[0].init-param.cachePackageTagsRefresh</v>
       </c>
-      <c r="D19" t="str">
+      <c r="D19">
         <v>60</v>
       </c>
-      <c r="E19" t="str">
+      <c r="E19">
         <f>_xll.JsonLookup($A$1,C19)</f>
         <v>60</v>
       </c>
@@ -2103,10 +2112,10 @@
       <c r="C20" t="str">
         <v>web-app.servlet[0].init-param.cacheTemplatesTrack</v>
       </c>
-      <c r="D20" t="str">
+      <c r="D20">
         <v>100</v>
       </c>
-      <c r="E20" t="str">
+      <c r="E20">
         <f>_xll.JsonLookup($A$1,C20)</f>
         <v>100</v>
       </c>
@@ -2116,10 +2125,10 @@
       <c r="C21" t="str">
         <v>web-app.servlet[0].init-param.cacheTemplatesStore</v>
       </c>
-      <c r="D21" t="str">
+      <c r="D21">
         <v>50</v>
       </c>
-      <c r="E21" t="str">
+      <c r="E21">
         <f>_xll.JsonLookup($A$1,C21)</f>
         <v>50</v>
       </c>
@@ -2129,10 +2138,10 @@
       <c r="C22" t="str">
         <v>web-app.servlet[0].init-param.cacheTemplatesRefresh</v>
       </c>
-      <c r="D22" t="str">
+      <c r="D22">
         <v>15</v>
       </c>
-      <c r="E22" t="str">
+      <c r="E22">
         <f>_xll.JsonLookup($A$1,C22)</f>
         <v>15</v>
       </c>
@@ -2142,10 +2151,10 @@
       <c r="C23" t="str">
         <v>web-app.servlet[0].init-param.cachePagesTrack</v>
       </c>
-      <c r="D23" t="str">
+      <c r="D23">
         <v>200</v>
       </c>
-      <c r="E23" t="str">
+      <c r="E23">
         <f>_xll.JsonLookup($A$1,C23)</f>
         <v>200</v>
       </c>
@@ -2155,10 +2164,10 @@
       <c r="C24" t="str">
         <v>web-app.servlet[0].init-param.cachePagesStore</v>
       </c>
-      <c r="D24" t="str">
+      <c r="D24">
         <v>100</v>
       </c>
-      <c r="E24" t="str">
+      <c r="E24">
         <f>_xll.JsonLookup($A$1,C24)</f>
         <v>100</v>
       </c>
@@ -2168,10 +2177,10 @@
       <c r="C25" t="str">
         <v>web-app.servlet[0].init-param.cachePagesRefresh</v>
       </c>
-      <c r="D25" t="str">
+      <c r="D25">
         <v>10</v>
       </c>
-      <c r="E25" t="str">
+      <c r="E25">
         <f>_xll.JsonLookup($A$1,C25)</f>
         <v>10</v>
       </c>
@@ -2181,10 +2190,10 @@
       <c r="C26" t="str">
         <v>web-app.servlet[0].init-param.cachePagesDirtyRead</v>
       </c>
-      <c r="D26" t="str">
+      <c r="D26">
         <v>10</v>
       </c>
-      <c r="E26" t="str">
+      <c r="E26">
         <f>_xll.JsonLookup($A$1,C26)</f>
         <v>10</v>
       </c>
@@ -2233,12 +2242,12 @@
       <c r="C30" t="str">
         <v>web-app.servlet[0].init-param.useDataStore</v>
       </c>
-      <c r="D30" t="str">
-        <v>True</v>
-      </c>
-      <c r="E30" t="str">
+      <c r="D30" t="b">
+        <v>1</v>
+      </c>
+      <c r="E30" t="b">
         <f>_xll.JsonLookup($A$1,C30)</f>
-        <v>True</v>
+        <v>1</v>
       </c>
     </row>
     <row r="31" spans="1:5">
@@ -2363,10 +2372,10 @@
       <c r="C40" t="str">
         <v>web-app.servlet[0].init-param.dataStoreInitConns</v>
       </c>
-      <c r="D40" t="str">
+      <c r="D40">
         <v>10</v>
       </c>
-      <c r="E40" t="str">
+      <c r="E40">
         <f>_xll.JsonLookup($A$1,C40)</f>
         <v>10</v>
       </c>
@@ -2376,10 +2385,10 @@
       <c r="C41" t="str">
         <v>web-app.servlet[0].init-param.dataStoreMaxConns</v>
       </c>
-      <c r="D41" t="str">
+      <c r="D41">
         <v>100</v>
       </c>
-      <c r="E41" t="str">
+      <c r="E41">
         <f>_xll.JsonLookup($A$1,C41)</f>
         <v>100</v>
       </c>
@@ -2389,10 +2398,10 @@
       <c r="C42" t="str">
         <v>web-app.servlet[0].init-param.dataStoreConnUsageLimit</v>
       </c>
-      <c r="D42" t="str">
+      <c r="D42">
         <v>100</v>
       </c>
-      <c r="E42" t="str">
+      <c r="E42">
         <f>_xll.JsonLookup($A$1,C42)</f>
         <v>100</v>
       </c>
@@ -2415,10 +2424,10 @@
       <c r="C44" t="str">
         <v>web-app.servlet[0].init-param.maxUrlLength</v>
       </c>
-      <c r="D44" t="str">
+      <c r="D44">
         <v>500</v>
       </c>
-      <c r="E44" t="str">
+      <c r="E44">
         <f>_xll.JsonLookup($A$1,C44)</f>
         <v>500</v>
       </c>
@@ -2571,10 +2580,10 @@
       <c r="C56" t="str">
         <v>web-app.servlet[4].init-param.log</v>
       </c>
-      <c r="D56" t="str">
+      <c r="D56">
         <v>1</v>
       </c>
-      <c r="E56" t="str">
+      <c r="E56">
         <f>_xll.JsonLookup($A$1,C56)</f>
         <v>1</v>
       </c>
@@ -2610,10 +2619,10 @@
       <c r="C59" t="str">
         <v>web-app.servlet[4].init-param.dataLog</v>
       </c>
-      <c r="D59" t="str">
+      <c r="D59">
         <v>1</v>
       </c>
-      <c r="E59" t="str">
+      <c r="E59">
         <f>_xll.JsonLookup($A$1,C59)</f>
         <v>1</v>
       </c>
@@ -2688,10 +2697,10 @@
       <c r="C65" t="str">
         <v>web-app.servlet[4].init-param.lookInContext</v>
       </c>
-      <c r="D65" t="str">
+      <c r="D65">
         <v>1</v>
       </c>
-      <c r="E65" t="str">
+      <c r="E65">
         <f>_xll.JsonLookup($A$1,C65)</f>
         <v>1</v>
       </c>
@@ -2701,10 +2710,10 @@
       <c r="C66" t="str">
         <v>web-app.servlet[4].init-param.adminGroupID</v>
       </c>
-      <c r="D66" t="str">
+      <c r="D66">
         <v>4</v>
       </c>
-      <c r="E66" t="str">
+      <c r="E66">
         <f>_xll.JsonLookup($A$1,C66)</f>
         <v>4</v>
       </c>
@@ -2714,12 +2723,12 @@
       <c r="C67" t="str">
         <v>web-app.servlet[4].init-param.betaServer</v>
       </c>
-      <c r="D67" t="str">
-        <v>True</v>
-      </c>
-      <c r="E67" t="str">
+      <c r="D67" t="b">
+        <v>1</v>
+      </c>
+      <c r="E67" t="b">
         <f>_xll.JsonLookup($A$1,C67)</f>
-        <v>True</v>
+        <v>1</v>
       </c>
     </row>
     <row r="68" spans="1:5">
@@ -2889,25 +2898,26 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{54B4FA4A-253A-4DC7-B007-BD642767BFAD}">
-  <dimension ref="A1:D161"/>
+  <dimension ref="A1:G161"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="17.7109375" customWidth="1"/>
+    <col min="1" max="1" width="35" customWidth="1"/>
     <col min="2" max="2" width="22.28515625" customWidth="1"/>
     <col min="3" max="3" width="11.85546875" customWidth="1"/>
+    <col min="5" max="5" width="10.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:7">
       <c r="A1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:7">
       <c r="A5" t="str">
         <f t="array" ref="A5:B161">_xll.JsonToArray($A$1)</f>
         <v>Model</v>
@@ -2920,7 +2930,7 @@
         <v>SMA</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:7">
       <c r="A6" t="str">
         <v>Test.k</v>
       </c>
@@ -2931,15 +2941,12 @@
         <f>_xll.JsonLookup($A$1,A6)</f>
         <v>v</v>
       </c>
-      <c r="D6" t="str">
+      <c r="D6" t="e">
         <f>_xll.JsonLookup(A1,"Test")</f>
-        <v>{_x000D_
-  "k": "v",_x000D_
-  "k2": "v2"_x000D_
-}</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4">
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
       <c r="A7" t="str">
         <v>Test.k2</v>
       </c>
@@ -2951,7 +2958,7 @@
         <v>v2</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:7">
       <c r="A8" t="str">
         <v>TargetTime</v>
       </c>
@@ -2962,8 +2969,107 @@
         <f>_xll.JsonLookup($A$1,A8)</f>
         <v>43290.895138888889</v>
       </c>
-    </row>
-    <row r="9" spans="1:4">
+      <c r="E8" t="str">
+        <f>_xll.JsonLookup(A1,"Data")</f>
+        <v>{_x000D_
+  "2018-07-09T19:56:00Z": 6711.493,_x000D_
+  "2018-07-09T19:57:00Z": 6711.92,_x000D_
+  "2018-07-09T19:58:00Z": 6712.532,_x000D_
+  "2018-07-09T19:59:00Z": 6712.431,_x000D_
+  "2018-07-09T20:00:00Z": 6711.934,_x000D_
+  "2018-07-09T20:01:00Z": 6712.131,_x000D_
+  "2018-07-09T20:02:00Z": 6711.981,_x000D_
+  "2018-07-09T20:03:00Z": 6711.781,_x000D_
+  "2018-07-09T20:04:00Z": 6711.586,_x000D_
+  "2018-07-09T20:05:00Z": 6711.139,_x000D_
+  "2018-07-09T20:06:00Z": 6710.862,_x000D_
+  "2018-07-09T20:07:00Z": 6710.37,_x000D_
+  "2018-07-09T20:08:00Z": 6709.85,_x000D_
+  "2018-07-09T20:09:00Z": 6709.287,_x000D_
+  "2018-07-09T20:10:00Z": 6709.276,_x000D_
+  "2018-07-09T20:11:00Z": 6708.481,_x000D_
+  "2018-07-09T20:12:00Z": 6707.577,_x000D_
+  "2018-07-09T20:13:00Z": 6706.426,_x000D_
+  "2018-07-09T20:14:00Z": 6705.262,_x000D_
+  "2018-07-09T20:15:00Z": 6704.555,_x000D_
+  "2018-07-09T20:16:00Z": 6703.435,_x000D_
+  "2018-07-09T20:17:00Z": 6702.499,_x000D_
+  "2018-07-09T20:18:00Z": 6701.406,_x000D_
+  "2018-07-09T20:19:00Z": 6700.764,_x000D_
+  "2018-07-09T20:20:00Z": 6700.172,_x000D_
+  "2018-07-09T20:21:00Z": 6700.068,_x000D_
+  "2018-07-09T20:22:00Z": 6700.369,_x000D_
+  "2018-07-09T20:23:00Z": 6701.091,_x000D_
+  "2018-07-09T20:24:00Z": 6701.538,_x000D_
+  "2018-07-09T20:25:00Z": 6701.738,_x000D_
+  "2018-07-09T20:26:00Z": 6702.119,_x000D_
+  "2018-07-09T20:27:00Z": 6702.619,_x000D_
+  "2018-07-09T20:28:00Z": 6703.014,_x000D_
+  "2018-07-09T20:29:00Z": 6703.0,_x000D_
+  "2018-07-09T20:30:00Z": 6702.899,_x000D_
+  "2018-07-09T20:31:00Z": 6702.822,_x000D_
+  "2018-07-09T20:32:00Z": 6703.146,_x000D_
+  "2018-07-09T20:33:00Z": 6702.996,_x000D_
+  "2018-07-09T20:34:00Z": 6703.119,_x000D_
+  "2018-07-09T20:35:00Z": 6703.501,_x000D_
+  "2018-07-09T20:36:00Z": 6703.497,_x000D_
+  "2018-07-09T20:37:00Z": 6703.831,_x000D_
+  "2018-07-09T20:38:00Z": 6703.927,_x000D_
+  "2018-07-09T20:39:00Z": 6704.307,_x000D_
+  "2018-07-09T20:40:00Z": 6704.571,_x000D_
+  "2018-07-09T20:41:00Z": 6705.048,_x000D_
+  "2018-07-09T20:42:00Z": 6704.332,_x000D_
+  "2018-07-09T20:43:00Z": 6703.92,_x000D_
+  "2018-07-09T20:44:00Z": 6703.685,_x000D_
+  "2018-07-09T20:45:00Z": 6703.19,_x000D_
+  "2018-07-09T20:46:00Z": 6703.345,_x000D_
+  "2018-07-09T20:47:00Z": 6703.208,_x000D_
+  "2018-07-09T20:48:00Z": 6703.218,_x000D_
+  "2018-07-09T20:49:00Z": 6703.057,_x000D_
+  "2018-07-09T20:50:00Z": 6702.836,_x000D_
+  "2018-07-09T20:51:00Z": 6702.379,_x000D_
+  "2018-07-09T20:52:00Z": 6702.368,_x000D_
+  "2018-07-09T20:53:00Z": 6702.281,_x000D_
+  "2018-07-09T20:54:00Z": 6702.017,_x000D_
+  "2018-07-09T20:55:00Z": 6701.851,_x000D_
+  "2018-07-09T20:56:00Z": 6701.26,_x000D_
+  "2018-07-09T20:57:00Z": 6700.684,_x000D_
+  "2018-07-09T20:58:00Z": 6699.999,_x000D_
+  "2018-07-09T20:59:00Z": 6699.6,_x000D_
+  "2018-07-09T21:00:00Z": 6699.087,_x000D_
+  "2018-07-09T21:01:00Z": 6698.745,_x000D_
+  "2018-07-09T21:02:00Z": 6698.449,_x000D_
+  "2018-07-09T21:03:00Z": 6698.291,_x000D_
+  "2018-07-09T21:04:00Z": 6698.133,_x000D_
+  "2018-07-09T21:05:00Z": 6697.738,_x000D_
+  "2018-07-09T21:06:00Z": 6697.319,_x000D_
+  "2018-07-09T21:07:00Z": 6697.161,_x000D_
+  "2018-07-09T21:08:00Z": 6697.445,_x000D_
+  "2018-07-09T21:09:00Z": 6697.444,_x000D_
+  "2018-07-09T21:10:00Z": 6697.62,_x000D_
+  "2018-07-09T21:11:00Z": 6697.619,_x000D_
+  "2018-07-09T21:12:00Z": 6697.642,_x000D_
+  "2018-07-09T21:13:00Z": 6697.604,_x000D_
+  "2018-07-09T21:14:00Z": 6697.565,_x000D_
+  "2018-07-09T21:15:00Z": 6698.039,_x000D_
+  "2018-07-09T21:16:00Z": 6698.229,_x000D_
+  "2018-07-09T21:17:00Z": 6698.158,_x000D_
+  "2018-07-09T21:18:00Z": 6697.995,_x000D_
+  "2018-07-09T21:19:00Z": 6698.077,_x000D_
+  "2018-07-09T21:20:00Z": 6698.174,_x000D_
+  "2018-07-09T21:21:00Z": 6698.574,_x000D_
+  "2018-07-09T21:22:00Z": 6699.397,_x000D_
+  "2018-07-09T21:23:00Z": 6700.549,_x000D_
+  "2018-07-09T21:24:00Z": 6701.633,_x000D_
+  "2018-07-09T21:25:00Z": 6702.441,_x000D_
+  "2018-07-09T21:26:00Z": 6703.554,_x000D_
+  "2018-07-09T21:27:00Z": 6704.667,_x000D_
+  "2018-07-09T21:28:00Z": 6705.638,_x000D_
+  "2018-07-09T21:29:00Z": 6706.43_x000D_
+}</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
       <c r="A9" t="str">
         <v>Data.2018-07-09T19:56:00Z</v>
       </c>
@@ -2974,8 +3080,18 @@
         <f>_xll.JsonLookup($A$1,A9)</f>
         <v>6711.4930000000004</v>
       </c>
-    </row>
-    <row r="10" spans="1:4">
+      <c r="E9" t="str">
+        <f t="array" ref="E9:G102">_xll.JsonToArray(E8)</f>
+        <v>2018-07-09T19:56:00Z</v>
+      </c>
+      <c r="F9">
+        <v>6711.4930000000004</v>
+      </c>
+      <c r="G9" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
       <c r="A10" t="str">
         <v>Data.2018-07-09T19:57:00Z</v>
       </c>
@@ -2986,8 +3102,17 @@
         <f>_xll.JsonLookup($A$1,A10)</f>
         <v>6711.92</v>
       </c>
-    </row>
-    <row r="11" spans="1:4">
+      <c r="E10" t="str">
+        <v>2018-07-09T19:57:00Z</v>
+      </c>
+      <c r="F10">
+        <v>6711.92</v>
+      </c>
+      <c r="G10" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
       <c r="A11" t="str">
         <v>Data.2018-07-09T19:58:00Z</v>
       </c>
@@ -2998,8 +3123,17 @@
         <f>_xll.JsonLookup($A$1,A11)</f>
         <v>6712.5320000000002</v>
       </c>
-    </row>
-    <row r="12" spans="1:4">
+      <c r="E11" t="str">
+        <v>2018-07-09T19:58:00Z</v>
+      </c>
+      <c r="F11">
+        <v>6712.5320000000002</v>
+      </c>
+      <c r="G11" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
       <c r="A12" t="str">
         <v>Data.2018-07-09T19:59:00Z</v>
       </c>
@@ -3010,8 +3144,17 @@
         <f>_xll.JsonLookup($A$1,A12)</f>
         <v>6712.4309999999996</v>
       </c>
-    </row>
-    <row r="13" spans="1:4">
+      <c r="E12" t="str">
+        <v>2018-07-09T19:59:00Z</v>
+      </c>
+      <c r="F12">
+        <v>6712.4309999999996</v>
+      </c>
+      <c r="G12" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
       <c r="A13" t="str">
         <v>Data.2018-07-09T20:00:00Z</v>
       </c>
@@ -3022,8 +3165,17 @@
         <f>_xll.JsonLookup($A$1,A13)</f>
         <v>6711.9340000000002</v>
       </c>
-    </row>
-    <row r="14" spans="1:4">
+      <c r="E13" t="str">
+        <v>2018-07-09T20:00:00Z</v>
+      </c>
+      <c r="F13">
+        <v>6711.9340000000002</v>
+      </c>
+      <c r="G13" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7">
       <c r="A14" t="str">
         <v>Data.2018-07-09T20:01:00Z</v>
       </c>
@@ -3034,8 +3186,17 @@
         <f>_xll.JsonLookup($A$1,A14)</f>
         <v>6712.1310000000003</v>
       </c>
-    </row>
-    <row r="15" spans="1:4">
+      <c r="E14" t="str">
+        <v>2018-07-09T20:01:00Z</v>
+      </c>
+      <c r="F14">
+        <v>6712.1310000000003</v>
+      </c>
+      <c r="G14" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7">
       <c r="A15" t="str">
         <v>Data.2018-07-09T20:02:00Z</v>
       </c>
@@ -3046,8 +3207,17 @@
         <f>_xll.JsonLookup($A$1,A15)</f>
         <v>6711.9809999999998</v>
       </c>
-    </row>
-    <row r="16" spans="1:4">
+      <c r="E15" t="str">
+        <v>2018-07-09T20:02:00Z</v>
+      </c>
+      <c r="F15">
+        <v>6711.9809999999998</v>
+      </c>
+      <c r="G15" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7">
       <c r="A16" t="str">
         <v>Data.2018-07-09T20:03:00Z</v>
       </c>
@@ -3058,8 +3228,17 @@
         <f>_xll.JsonLookup($A$1,A16)</f>
         <v>6711.7809999999999</v>
       </c>
-    </row>
-    <row r="17" spans="1:3">
+      <c r="E16" t="str">
+        <v>2018-07-09T20:03:00Z</v>
+      </c>
+      <c r="F16">
+        <v>6711.7809999999999</v>
+      </c>
+      <c r="G16" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7">
       <c r="A17" t="str">
         <v>Data.2018-07-09T20:04:00Z</v>
       </c>
@@ -3070,8 +3249,17 @@
         <f>_xll.JsonLookup($A$1,A17)</f>
         <v>6711.5860000000002</v>
       </c>
-    </row>
-    <row r="18" spans="1:3">
+      <c r="E17" t="str">
+        <v>2018-07-09T20:04:00Z</v>
+      </c>
+      <c r="F17">
+        <v>6711.5860000000002</v>
+      </c>
+      <c r="G17" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7">
       <c r="A18" t="str">
         <v>Data.2018-07-09T20:05:00Z</v>
       </c>
@@ -3082,8 +3270,17 @@
         <f>_xll.JsonLookup($A$1,A18)</f>
         <v>6711.1390000000001</v>
       </c>
-    </row>
-    <row r="19" spans="1:3">
+      <c r="E18" t="str">
+        <v>2018-07-09T20:05:00Z</v>
+      </c>
+      <c r="F18">
+        <v>6711.1390000000001</v>
+      </c>
+      <c r="G18" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7">
       <c r="A19" t="str">
         <v>Data.2018-07-09T20:06:00Z</v>
       </c>
@@ -3094,8 +3291,17 @@
         <f>_xll.JsonLookup($A$1,A19)</f>
         <v>6710.8620000000001</v>
       </c>
-    </row>
-    <row r="20" spans="1:3">
+      <c r="E19" t="str">
+        <v>2018-07-09T20:06:00Z</v>
+      </c>
+      <c r="F19">
+        <v>6710.8620000000001</v>
+      </c>
+      <c r="G19" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7">
       <c r="A20" t="str">
         <v>Data.2018-07-09T20:07:00Z</v>
       </c>
@@ -3106,8 +3312,17 @@
         <f>_xll.JsonLookup($A$1,A20)</f>
         <v>6710.37</v>
       </c>
-    </row>
-    <row r="21" spans="1:3">
+      <c r="E20" t="str">
+        <v>2018-07-09T20:07:00Z</v>
+      </c>
+      <c r="F20">
+        <v>6710.37</v>
+      </c>
+      <c r="G20" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7">
       <c r="A21" t="str">
         <v>Data.2018-07-09T20:08:00Z</v>
       </c>
@@ -3118,8 +3333,17 @@
         <f>_xll.JsonLookup($A$1,A21)</f>
         <v>6709.85</v>
       </c>
-    </row>
-    <row r="22" spans="1:3">
+      <c r="E21" t="str">
+        <v>2018-07-09T20:08:00Z</v>
+      </c>
+      <c r="F21">
+        <v>6709.85</v>
+      </c>
+      <c r="G21" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7">
       <c r="A22" t="str">
         <v>Data.2018-07-09T20:09:00Z</v>
       </c>
@@ -3130,8 +3354,17 @@
         <f>_xll.JsonLookup($A$1,A22)</f>
         <v>6709.2870000000003</v>
       </c>
-    </row>
-    <row r="23" spans="1:3">
+      <c r="E22" t="str">
+        <v>2018-07-09T20:09:00Z</v>
+      </c>
+      <c r="F22">
+        <v>6709.2870000000003</v>
+      </c>
+      <c r="G22" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7">
       <c r="A23" t="str">
         <v>Data.2018-07-09T20:10:00Z</v>
       </c>
@@ -3142,8 +3375,17 @@
         <f>_xll.JsonLookup($A$1,A23)</f>
         <v>6709.2759999999998</v>
       </c>
-    </row>
-    <row r="24" spans="1:3">
+      <c r="E23" t="str">
+        <v>2018-07-09T20:10:00Z</v>
+      </c>
+      <c r="F23">
+        <v>6709.2759999999998</v>
+      </c>
+      <c r="G23" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7">
       <c r="A24" t="str">
         <v>Data.2018-07-09T20:11:00Z</v>
       </c>
@@ -3154,8 +3396,17 @@
         <f>_xll.JsonLookup($A$1,A24)</f>
         <v>6708.4809999999998</v>
       </c>
-    </row>
-    <row r="25" spans="1:3">
+      <c r="E24" t="str">
+        <v>2018-07-09T20:11:00Z</v>
+      </c>
+      <c r="F24">
+        <v>6708.4809999999998</v>
+      </c>
+      <c r="G24" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7">
       <c r="A25" t="str">
         <v>Data.2018-07-09T20:12:00Z</v>
       </c>
@@ -3166,8 +3417,17 @@
         <f>_xll.JsonLookup($A$1,A25)</f>
         <v>6707.5770000000002</v>
       </c>
-    </row>
-    <row r="26" spans="1:3">
+      <c r="E25" t="str">
+        <v>2018-07-09T20:12:00Z</v>
+      </c>
+      <c r="F25">
+        <v>6707.5770000000002</v>
+      </c>
+      <c r="G25" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7">
       <c r="A26" t="str">
         <v>Data.2018-07-09T20:13:00Z</v>
       </c>
@@ -3178,8 +3438,17 @@
         <f>_xll.JsonLookup($A$1,A26)</f>
         <v>6706.4260000000004</v>
       </c>
-    </row>
-    <row r="27" spans="1:3">
+      <c r="E26" t="str">
+        <v>2018-07-09T20:13:00Z</v>
+      </c>
+      <c r="F26">
+        <v>6706.4260000000004</v>
+      </c>
+      <c r="G26" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7">
       <c r="A27" t="str">
         <v>Data.2018-07-09T20:14:00Z</v>
       </c>
@@ -3190,8 +3459,17 @@
         <f>_xll.JsonLookup($A$1,A27)</f>
         <v>6705.2619999999997</v>
       </c>
-    </row>
-    <row r="28" spans="1:3">
+      <c r="E27" t="str">
+        <v>2018-07-09T20:14:00Z</v>
+      </c>
+      <c r="F27">
+        <v>6705.2619999999997</v>
+      </c>
+      <c r="G27" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7">
       <c r="A28" t="str">
         <v>Data.2018-07-09T20:15:00Z</v>
       </c>
@@ -3202,8 +3480,17 @@
         <f>_xll.JsonLookup($A$1,A28)</f>
         <v>6704.5550000000003</v>
       </c>
-    </row>
-    <row r="29" spans="1:3">
+      <c r="E28" t="str">
+        <v>2018-07-09T20:15:00Z</v>
+      </c>
+      <c r="F28">
+        <v>6704.5550000000003</v>
+      </c>
+      <c r="G28" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7">
       <c r="A29" t="str">
         <v>Data.2018-07-09T20:16:00Z</v>
       </c>
@@ -3214,8 +3501,17 @@
         <f>_xll.JsonLookup($A$1,A29)</f>
         <v>6703.4350000000004</v>
       </c>
-    </row>
-    <row r="30" spans="1:3">
+      <c r="E29" t="str">
+        <v>2018-07-09T20:16:00Z</v>
+      </c>
+      <c r="F29">
+        <v>6703.4350000000004</v>
+      </c>
+      <c r="G29" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7">
       <c r="A30" t="str">
         <v>Data.2018-07-09T20:17:00Z</v>
       </c>
@@ -3226,8 +3522,17 @@
         <f>_xll.JsonLookup($A$1,A30)</f>
         <v>6702.4989999999998</v>
       </c>
-    </row>
-    <row r="31" spans="1:3">
+      <c r="E30" t="str">
+        <v>2018-07-09T20:17:00Z</v>
+      </c>
+      <c r="F30">
+        <v>6702.4989999999998</v>
+      </c>
+      <c r="G30" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7">
       <c r="A31" t="str">
         <v>Data.2018-07-09T20:18:00Z</v>
       </c>
@@ -3238,8 +3543,17 @@
         <f>_xll.JsonLookup($A$1,A31)</f>
         <v>6701.4059999999999</v>
       </c>
-    </row>
-    <row r="32" spans="1:3">
+      <c r="E31" t="str">
+        <v>2018-07-09T20:18:00Z</v>
+      </c>
+      <c r="F31">
+        <v>6701.4059999999999</v>
+      </c>
+      <c r="G31" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7">
       <c r="A32" t="str">
         <v>Data.2018-07-09T20:19:00Z</v>
       </c>
@@ -3250,8 +3564,17 @@
         <f>_xll.JsonLookup($A$1,A32)</f>
         <v>6700.7640000000001</v>
       </c>
-    </row>
-    <row r="33" spans="1:3">
+      <c r="E32" t="str">
+        <v>2018-07-09T20:19:00Z</v>
+      </c>
+      <c r="F32">
+        <v>6700.7640000000001</v>
+      </c>
+      <c r="G32" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7">
       <c r="A33" t="str">
         <v>Data.2018-07-09T20:20:00Z</v>
       </c>
@@ -3262,8 +3585,17 @@
         <f>_xll.JsonLookup($A$1,A33)</f>
         <v>6700.1719999999996</v>
       </c>
-    </row>
-    <row r="34" spans="1:3">
+      <c r="E33" t="str">
+        <v>2018-07-09T20:20:00Z</v>
+      </c>
+      <c r="F33">
+        <v>6700.1719999999996</v>
+      </c>
+      <c r="G33" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7">
       <c r="A34" t="str">
         <v>Data.2018-07-09T20:21:00Z</v>
       </c>
@@ -3274,8 +3606,17 @@
         <f>_xll.JsonLookup($A$1,A34)</f>
         <v>6700.0680000000002</v>
       </c>
-    </row>
-    <row r="35" spans="1:3">
+      <c r="E34" t="str">
+        <v>2018-07-09T20:21:00Z</v>
+      </c>
+      <c r="F34">
+        <v>6700.0680000000002</v>
+      </c>
+      <c r="G34" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7">
       <c r="A35" t="str">
         <v>Data.2018-07-09T20:22:00Z</v>
       </c>
@@ -3286,8 +3627,17 @@
         <f>_xll.JsonLookup($A$1,A35)</f>
         <v>6700.3689999999997</v>
       </c>
-    </row>
-    <row r="36" spans="1:3">
+      <c r="E35" t="str">
+        <v>2018-07-09T20:22:00Z</v>
+      </c>
+      <c r="F35">
+        <v>6700.3689999999997</v>
+      </c>
+      <c r="G35" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7">
       <c r="A36" t="str">
         <v>Data.2018-07-09T20:23:00Z</v>
       </c>
@@ -3298,8 +3648,17 @@
         <f>_xll.JsonLookup($A$1,A36)</f>
         <v>6701.0910000000003</v>
       </c>
-    </row>
-    <row r="37" spans="1:3">
+      <c r="E36" t="str">
+        <v>2018-07-09T20:23:00Z</v>
+      </c>
+      <c r="F36">
+        <v>6701.0910000000003</v>
+      </c>
+      <c r="G36" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7">
       <c r="A37" t="str">
         <v>Data.2018-07-09T20:24:00Z</v>
       </c>
@@ -3310,8 +3669,17 @@
         <f>_xll.JsonLookup($A$1,A37)</f>
         <v>6701.5379999999996</v>
       </c>
-    </row>
-    <row r="38" spans="1:3">
+      <c r="E37" t="str">
+        <v>2018-07-09T20:24:00Z</v>
+      </c>
+      <c r="F37">
+        <v>6701.5379999999996</v>
+      </c>
+      <c r="G37" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7">
       <c r="A38" t="str">
         <v>Data.2018-07-09T20:25:00Z</v>
       </c>
@@ -3322,8 +3690,17 @@
         <f>_xll.JsonLookup($A$1,A38)</f>
         <v>6701.7380000000003</v>
       </c>
-    </row>
-    <row r="39" spans="1:3">
+      <c r="E38" t="str">
+        <v>2018-07-09T20:25:00Z</v>
+      </c>
+      <c r="F38">
+        <v>6701.7380000000003</v>
+      </c>
+      <c r="G38" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7">
       <c r="A39" t="str">
         <v>Data.2018-07-09T20:26:00Z</v>
       </c>
@@ -3334,8 +3711,17 @@
         <f>_xll.JsonLookup($A$1,A39)</f>
         <v>6702.1189999999997</v>
       </c>
-    </row>
-    <row r="40" spans="1:3">
+      <c r="E39" t="str">
+        <v>2018-07-09T20:26:00Z</v>
+      </c>
+      <c r="F39">
+        <v>6702.1189999999997</v>
+      </c>
+      <c r="G39" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7">
       <c r="A40" t="str">
         <v>Data.2018-07-09T20:27:00Z</v>
       </c>
@@ -3346,8 +3732,17 @@
         <f>_xll.JsonLookup($A$1,A40)</f>
         <v>6702.6189999999997</v>
       </c>
-    </row>
-    <row r="41" spans="1:3">
+      <c r="E40" t="str">
+        <v>2018-07-09T20:27:00Z</v>
+      </c>
+      <c r="F40">
+        <v>6702.6189999999997</v>
+      </c>
+      <c r="G40" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7">
       <c r="A41" t="str">
         <v>Data.2018-07-09T20:28:00Z</v>
       </c>
@@ -3358,8 +3753,17 @@
         <f>_xll.JsonLookup($A$1,A41)</f>
         <v>6703.0140000000001</v>
       </c>
-    </row>
-    <row r="42" spans="1:3">
+      <c r="E41" t="str">
+        <v>2018-07-09T20:28:00Z</v>
+      </c>
+      <c r="F41">
+        <v>6703.0140000000001</v>
+      </c>
+      <c r="G41" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7">
       <c r="A42" t="str">
         <v>Data.2018-07-09T20:29:00Z</v>
       </c>
@@ -3370,8 +3774,17 @@
         <f>_xll.JsonLookup($A$1,A42)</f>
         <v>6703</v>
       </c>
-    </row>
-    <row r="43" spans="1:3">
+      <c r="E42" t="str">
+        <v>2018-07-09T20:29:00Z</v>
+      </c>
+      <c r="F42">
+        <v>6703</v>
+      </c>
+      <c r="G42" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7">
       <c r="A43" t="str">
         <v>Data.2018-07-09T20:30:00Z</v>
       </c>
@@ -3382,8 +3795,17 @@
         <f>_xll.JsonLookup($A$1,A43)</f>
         <v>6702.8990000000003</v>
       </c>
-    </row>
-    <row r="44" spans="1:3">
+      <c r="E43" t="str">
+        <v>2018-07-09T20:30:00Z</v>
+      </c>
+      <c r="F43">
+        <v>6702.8990000000003</v>
+      </c>
+      <c r="G43" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7">
       <c r="A44" t="str">
         <v>Data.2018-07-09T20:31:00Z</v>
       </c>
@@ -3394,8 +3816,17 @@
         <f>_xll.JsonLookup($A$1,A44)</f>
         <v>6702.8220000000001</v>
       </c>
-    </row>
-    <row r="45" spans="1:3">
+      <c r="E44" t="str">
+        <v>2018-07-09T20:31:00Z</v>
+      </c>
+      <c r="F44">
+        <v>6702.8220000000001</v>
+      </c>
+      <c r="G44" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7">
       <c r="A45" t="str">
         <v>Data.2018-07-09T20:32:00Z</v>
       </c>
@@ -3406,8 +3837,17 @@
         <f>_xll.JsonLookup($A$1,A45)</f>
         <v>6703.1459999999997</v>
       </c>
-    </row>
-    <row r="46" spans="1:3">
+      <c r="E45" t="str">
+        <v>2018-07-09T20:32:00Z</v>
+      </c>
+      <c r="F45">
+        <v>6703.1459999999997</v>
+      </c>
+      <c r="G45" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7">
       <c r="A46" t="str">
         <v>Data.2018-07-09T20:33:00Z</v>
       </c>
@@ -3418,8 +3858,17 @@
         <f>_xll.JsonLookup($A$1,A46)</f>
         <v>6702.9960000000001</v>
       </c>
-    </row>
-    <row r="47" spans="1:3">
+      <c r="E46" t="str">
+        <v>2018-07-09T20:33:00Z</v>
+      </c>
+      <c r="F46">
+        <v>6702.9960000000001</v>
+      </c>
+      <c r="G46" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7">
       <c r="A47" t="str">
         <v>Data.2018-07-09T20:34:00Z</v>
       </c>
@@ -3430,8 +3879,17 @@
         <f>_xll.JsonLookup($A$1,A47)</f>
         <v>6703.1189999999997</v>
       </c>
-    </row>
-    <row r="48" spans="1:3">
+      <c r="E47" t="str">
+        <v>2018-07-09T20:34:00Z</v>
+      </c>
+      <c r="F47">
+        <v>6703.1189999999997</v>
+      </c>
+      <c r="G47" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7">
       <c r="A48" t="str">
         <v>Data.2018-07-09T20:35:00Z</v>
       </c>
@@ -3442,8 +3900,17 @@
         <f>_xll.JsonLookup($A$1,A48)</f>
         <v>6703.5010000000002</v>
       </c>
-    </row>
-    <row r="49" spans="1:3">
+      <c r="E48" t="str">
+        <v>2018-07-09T20:35:00Z</v>
+      </c>
+      <c r="F48">
+        <v>6703.5010000000002</v>
+      </c>
+      <c r="G48" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7">
       <c r="A49" t="str">
         <v>Data.2018-07-09T20:36:00Z</v>
       </c>
@@ -3454,8 +3921,17 @@
         <f>_xll.JsonLookup($A$1,A49)</f>
         <v>6703.4970000000003</v>
       </c>
-    </row>
-    <row r="50" spans="1:3">
+      <c r="E49" t="str">
+        <v>2018-07-09T20:36:00Z</v>
+      </c>
+      <c r="F49">
+        <v>6703.4970000000003</v>
+      </c>
+      <c r="G49" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7">
       <c r="A50" t="str">
         <v>Data.2018-07-09T20:37:00Z</v>
       </c>
@@ -3466,8 +3942,17 @@
         <f>_xll.JsonLookup($A$1,A50)</f>
         <v>6703.8310000000001</v>
       </c>
-    </row>
-    <row r="51" spans="1:3">
+      <c r="E50" t="str">
+        <v>2018-07-09T20:37:00Z</v>
+      </c>
+      <c r="F50">
+        <v>6703.8310000000001</v>
+      </c>
+      <c r="G50" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7">
       <c r="A51" t="str">
         <v>Data.2018-07-09T20:38:00Z</v>
       </c>
@@ -3478,8 +3963,17 @@
         <f>_xll.JsonLookup($A$1,A51)</f>
         <v>6703.9269999999997</v>
       </c>
-    </row>
-    <row r="52" spans="1:3">
+      <c r="E51" t="str">
+        <v>2018-07-09T20:38:00Z</v>
+      </c>
+      <c r="F51">
+        <v>6703.9269999999997</v>
+      </c>
+      <c r="G51" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7">
       <c r="A52" t="str">
         <v>Data.2018-07-09T20:39:00Z</v>
       </c>
@@ -3490,8 +3984,17 @@
         <f>_xll.JsonLookup($A$1,A52)</f>
         <v>6704.3069999999998</v>
       </c>
-    </row>
-    <row r="53" spans="1:3">
+      <c r="E52" t="str">
+        <v>2018-07-09T20:39:00Z</v>
+      </c>
+      <c r="F52">
+        <v>6704.3069999999998</v>
+      </c>
+      <c r="G52" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7">
       <c r="A53" t="str">
         <v>Data.2018-07-09T20:40:00Z</v>
       </c>
@@ -3502,8 +4005,17 @@
         <f>_xll.JsonLookup($A$1,A53)</f>
         <v>6704.5709999999999</v>
       </c>
-    </row>
-    <row r="54" spans="1:3">
+      <c r="E53" t="str">
+        <v>2018-07-09T20:40:00Z</v>
+      </c>
+      <c r="F53">
+        <v>6704.5709999999999</v>
+      </c>
+      <c r="G53" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7">
       <c r="A54" t="str">
         <v>Data.2018-07-09T20:41:00Z</v>
       </c>
@@ -3514,8 +4026,17 @@
         <f>_xll.JsonLookup($A$1,A54)</f>
         <v>6705.0479999999998</v>
       </c>
-    </row>
-    <row r="55" spans="1:3">
+      <c r="E54" t="str">
+        <v>2018-07-09T20:41:00Z</v>
+      </c>
+      <c r="F54">
+        <v>6705.0479999999998</v>
+      </c>
+      <c r="G54" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7">
       <c r="A55" t="str">
         <v>Data.2018-07-09T20:42:00Z</v>
       </c>
@@ -3526,8 +4047,17 @@
         <f>_xll.JsonLookup($A$1,A55)</f>
         <v>6704.3320000000003</v>
       </c>
-    </row>
-    <row r="56" spans="1:3">
+      <c r="E55" t="str">
+        <v>2018-07-09T20:42:00Z</v>
+      </c>
+      <c r="F55">
+        <v>6704.3320000000003</v>
+      </c>
+      <c r="G55" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7">
       <c r="A56" t="str">
         <v>Data.2018-07-09T20:43:00Z</v>
       </c>
@@ -3538,8 +4068,17 @@
         <f>_xll.JsonLookup($A$1,A56)</f>
         <v>6703.92</v>
       </c>
-    </row>
-    <row r="57" spans="1:3">
+      <c r="E56" t="str">
+        <v>2018-07-09T20:43:00Z</v>
+      </c>
+      <c r="F56">
+        <v>6703.92</v>
+      </c>
+      <c r="G56" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7">
       <c r="A57" t="str">
         <v>Data.2018-07-09T20:44:00Z</v>
       </c>
@@ -3550,8 +4089,17 @@
         <f>_xll.JsonLookup($A$1,A57)</f>
         <v>6703.6850000000004</v>
       </c>
-    </row>
-    <row r="58" spans="1:3">
+      <c r="E57" t="str">
+        <v>2018-07-09T20:44:00Z</v>
+      </c>
+      <c r="F57">
+        <v>6703.6850000000004</v>
+      </c>
+      <c r="G57" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7">
       <c r="A58" t="str">
         <v>Data.2018-07-09T20:45:00Z</v>
       </c>
@@ -3562,8 +4110,17 @@
         <f>_xll.JsonLookup($A$1,A58)</f>
         <v>6703.19</v>
       </c>
-    </row>
-    <row r="59" spans="1:3">
+      <c r="E58" t="str">
+        <v>2018-07-09T20:45:00Z</v>
+      </c>
+      <c r="F58">
+        <v>6703.19</v>
+      </c>
+      <c r="G58" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7">
       <c r="A59" t="str">
         <v>Data.2018-07-09T20:46:00Z</v>
       </c>
@@ -3574,8 +4131,17 @@
         <f>_xll.JsonLookup($A$1,A59)</f>
         <v>6703.3450000000003</v>
       </c>
-    </row>
-    <row r="60" spans="1:3">
+      <c r="E59" t="str">
+        <v>2018-07-09T20:46:00Z</v>
+      </c>
+      <c r="F59">
+        <v>6703.3450000000003</v>
+      </c>
+      <c r="G59" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7">
       <c r="A60" t="str">
         <v>Data.2018-07-09T20:47:00Z</v>
       </c>
@@ -3586,8 +4152,17 @@
         <f>_xll.JsonLookup($A$1,A60)</f>
         <v>6703.2079999999996</v>
       </c>
-    </row>
-    <row r="61" spans="1:3">
+      <c r="E60" t="str">
+        <v>2018-07-09T20:47:00Z</v>
+      </c>
+      <c r="F60">
+        <v>6703.2079999999996</v>
+      </c>
+      <c r="G60" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7">
       <c r="A61" t="str">
         <v>Data.2018-07-09T20:48:00Z</v>
       </c>
@@ -3598,8 +4173,17 @@
         <f>_xll.JsonLookup($A$1,A61)</f>
         <v>6703.2179999999998</v>
       </c>
-    </row>
-    <row r="62" spans="1:3">
+      <c r="E61" t="str">
+        <v>2018-07-09T20:48:00Z</v>
+      </c>
+      <c r="F61">
+        <v>6703.2179999999998</v>
+      </c>
+      <c r="G61" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7">
       <c r="A62" t="str">
         <v>Data.2018-07-09T20:49:00Z</v>
       </c>
@@ -3610,8 +4194,17 @@
         <f>_xll.JsonLookup($A$1,A62)</f>
         <v>6703.0569999999998</v>
       </c>
-    </row>
-    <row r="63" spans="1:3">
+      <c r="E62" t="str">
+        <v>2018-07-09T20:49:00Z</v>
+      </c>
+      <c r="F62">
+        <v>6703.0569999999998</v>
+      </c>
+      <c r="G62" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7">
       <c r="A63" t="str">
         <v>Data.2018-07-09T20:50:00Z</v>
       </c>
@@ -3622,8 +4215,17 @@
         <f>_xll.JsonLookup($A$1,A63)</f>
         <v>6702.8360000000002</v>
       </c>
-    </row>
-    <row r="64" spans="1:3">
+      <c r="E63" t="str">
+        <v>2018-07-09T20:50:00Z</v>
+      </c>
+      <c r="F63">
+        <v>6702.8360000000002</v>
+      </c>
+      <c r="G63" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7">
       <c r="A64" t="str">
         <v>Data.2018-07-09T20:51:00Z</v>
       </c>
@@ -3634,8 +4236,17 @@
         <f>_xll.JsonLookup($A$1,A64)</f>
         <v>6702.3789999999999</v>
       </c>
-    </row>
-    <row r="65" spans="1:3">
+      <c r="E64" t="str">
+        <v>2018-07-09T20:51:00Z</v>
+      </c>
+      <c r="F64">
+        <v>6702.3789999999999</v>
+      </c>
+      <c r="G64" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7">
       <c r="A65" t="str">
         <v>Data.2018-07-09T20:52:00Z</v>
       </c>
@@ -3646,8 +4257,17 @@
         <f>_xll.JsonLookup($A$1,A65)</f>
         <v>6702.3680000000004</v>
       </c>
-    </row>
-    <row r="66" spans="1:3">
+      <c r="E65" t="str">
+        <v>2018-07-09T20:52:00Z</v>
+      </c>
+      <c r="F65">
+        <v>6702.3680000000004</v>
+      </c>
+      <c r="G65" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7">
       <c r="A66" t="str">
         <v>Data.2018-07-09T20:53:00Z</v>
       </c>
@@ -3658,8 +4278,17 @@
         <f>_xll.JsonLookup($A$1,A66)</f>
         <v>6702.2809999999999</v>
       </c>
-    </row>
-    <row r="67" spans="1:3">
+      <c r="E66" t="str">
+        <v>2018-07-09T20:53:00Z</v>
+      </c>
+      <c r="F66">
+        <v>6702.2809999999999</v>
+      </c>
+      <c r="G66" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7">
       <c r="A67" t="str">
         <v>Data.2018-07-09T20:54:00Z</v>
       </c>
@@ -3670,8 +4299,17 @@
         <f>_xll.JsonLookup($A$1,A67)</f>
         <v>6702.0169999999998</v>
       </c>
-    </row>
-    <row r="68" spans="1:3">
+      <c r="E67" t="str">
+        <v>2018-07-09T20:54:00Z</v>
+      </c>
+      <c r="F67">
+        <v>6702.0169999999998</v>
+      </c>
+      <c r="G67" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7">
       <c r="A68" t="str">
         <v>Data.2018-07-09T20:55:00Z</v>
       </c>
@@ -3682,8 +4320,17 @@
         <f>_xll.JsonLookup($A$1,A68)</f>
         <v>6701.8509999999997</v>
       </c>
-    </row>
-    <row r="69" spans="1:3">
+      <c r="E68" t="str">
+        <v>2018-07-09T20:55:00Z</v>
+      </c>
+      <c r="F68">
+        <v>6701.8509999999997</v>
+      </c>
+      <c r="G68" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7">
       <c r="A69" t="str">
         <v>Data.2018-07-09T20:56:00Z</v>
       </c>
@@ -3694,8 +4341,17 @@
         <f>_xll.JsonLookup($A$1,A69)</f>
         <v>6701.26</v>
       </c>
-    </row>
-    <row r="70" spans="1:3">
+      <c r="E69" t="str">
+        <v>2018-07-09T20:56:00Z</v>
+      </c>
+      <c r="F69">
+        <v>6701.26</v>
+      </c>
+      <c r="G69" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7">
       <c r="A70" t="str">
         <v>Data.2018-07-09T20:57:00Z</v>
       </c>
@@ -3706,8 +4362,17 @@
         <f>_xll.JsonLookup($A$1,A70)</f>
         <v>6700.6840000000002</v>
       </c>
-    </row>
-    <row r="71" spans="1:3">
+      <c r="E70" t="str">
+        <v>2018-07-09T20:57:00Z</v>
+      </c>
+      <c r="F70">
+        <v>6700.6840000000002</v>
+      </c>
+      <c r="G70" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7">
       <c r="A71" t="str">
         <v>Data.2018-07-09T20:58:00Z</v>
       </c>
@@ -3718,8 +4383,17 @@
         <f>_xll.JsonLookup($A$1,A71)</f>
         <v>6699.9989999999998</v>
       </c>
-    </row>
-    <row r="72" spans="1:3">
+      <c r="E71" t="str">
+        <v>2018-07-09T20:58:00Z</v>
+      </c>
+      <c r="F71">
+        <v>6699.9989999999998</v>
+      </c>
+      <c r="G71" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7">
       <c r="A72" t="str">
         <v>Data.2018-07-09T20:59:00Z</v>
       </c>
@@ -3730,8 +4404,17 @@
         <f>_xll.JsonLookup($A$1,A72)</f>
         <v>6699.6</v>
       </c>
-    </row>
-    <row r="73" spans="1:3">
+      <c r="E72" t="str">
+        <v>2018-07-09T20:59:00Z</v>
+      </c>
+      <c r="F72">
+        <v>6699.6</v>
+      </c>
+      <c r="G72" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7">
       <c r="A73" t="str">
         <v>Data.2018-07-09T21:00:00Z</v>
       </c>
@@ -3742,8 +4425,17 @@
         <f>_xll.JsonLookup($A$1,A73)</f>
         <v>6699.0870000000004</v>
       </c>
-    </row>
-    <row r="74" spans="1:3">
+      <c r="E73" t="str">
+        <v>2018-07-09T21:00:00Z</v>
+      </c>
+      <c r="F73">
+        <v>6699.0870000000004</v>
+      </c>
+      <c r="G73" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7">
       <c r="A74" t="str">
         <v>Data.2018-07-09T21:01:00Z</v>
       </c>
@@ -3754,8 +4446,17 @@
         <f>_xll.JsonLookup($A$1,A74)</f>
         <v>6698.7449999999999</v>
       </c>
-    </row>
-    <row r="75" spans="1:3">
+      <c r="E74" t="str">
+        <v>2018-07-09T21:01:00Z</v>
+      </c>
+      <c r="F74">
+        <v>6698.7449999999999</v>
+      </c>
+      <c r="G74" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7">
       <c r="A75" t="str">
         <v>Data.2018-07-09T21:02:00Z</v>
       </c>
@@ -3766,8 +4467,17 @@
         <f>_xll.JsonLookup($A$1,A75)</f>
         <v>6698.4489999999996</v>
       </c>
-    </row>
-    <row r="76" spans="1:3">
+      <c r="E75" t="str">
+        <v>2018-07-09T21:02:00Z</v>
+      </c>
+      <c r="F75">
+        <v>6698.4489999999996</v>
+      </c>
+      <c r="G75" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7">
       <c r="A76" t="str">
         <v>Data.2018-07-09T21:03:00Z</v>
       </c>
@@ -3778,8 +4488,17 @@
         <f>_xll.JsonLookup($A$1,A76)</f>
         <v>6698.2910000000002</v>
       </c>
-    </row>
-    <row r="77" spans="1:3">
+      <c r="E76" t="str">
+        <v>2018-07-09T21:03:00Z</v>
+      </c>
+      <c r="F76">
+        <v>6698.2910000000002</v>
+      </c>
+      <c r="G76" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7">
       <c r="A77" t="str">
         <v>Data.2018-07-09T21:04:00Z</v>
       </c>
@@ -3790,8 +4509,17 @@
         <f>_xll.JsonLookup($A$1,A77)</f>
         <v>6698.1329999999998</v>
       </c>
-    </row>
-    <row r="78" spans="1:3">
+      <c r="E77" t="str">
+        <v>2018-07-09T21:04:00Z</v>
+      </c>
+      <c r="F77">
+        <v>6698.1329999999998</v>
+      </c>
+      <c r="G77" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7">
       <c r="A78" t="str">
         <v>Data.2018-07-09T21:05:00Z</v>
       </c>
@@ -3802,8 +4530,17 @@
         <f>_xll.JsonLookup($A$1,A78)</f>
         <v>6697.7380000000003</v>
       </c>
-    </row>
-    <row r="79" spans="1:3">
+      <c r="E78" t="str">
+        <v>2018-07-09T21:05:00Z</v>
+      </c>
+      <c r="F78">
+        <v>6697.7380000000003</v>
+      </c>
+      <c r="G78" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7">
       <c r="A79" t="str">
         <v>Data.2018-07-09T21:06:00Z</v>
       </c>
@@ -3814,8 +4551,17 @@
         <f>_xll.JsonLookup($A$1,A79)</f>
         <v>6697.3190000000004</v>
       </c>
-    </row>
-    <row r="80" spans="1:3">
+      <c r="E79" t="str">
+        <v>2018-07-09T21:06:00Z</v>
+      </c>
+      <c r="F79">
+        <v>6697.3190000000004</v>
+      </c>
+      <c r="G79" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7">
       <c r="A80" t="str">
         <v>Data.2018-07-09T21:07:00Z</v>
       </c>
@@ -3826,8 +4572,17 @@
         <f>_xll.JsonLookup($A$1,A80)</f>
         <v>6697.1610000000001</v>
       </c>
-    </row>
-    <row r="81" spans="1:3">
+      <c r="E80" t="str">
+        <v>2018-07-09T21:07:00Z</v>
+      </c>
+      <c r="F80">
+        <v>6697.1610000000001</v>
+      </c>
+      <c r="G80" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7">
       <c r="A81" t="str">
         <v>Data.2018-07-09T21:08:00Z</v>
       </c>
@@ -3838,8 +4593,17 @@
         <f>_xll.JsonLookup($A$1,A81)</f>
         <v>6697.4449999999997</v>
       </c>
-    </row>
-    <row r="82" spans="1:3">
+      <c r="E81" t="str">
+        <v>2018-07-09T21:08:00Z</v>
+      </c>
+      <c r="F81">
+        <v>6697.4449999999997</v>
+      </c>
+      <c r="G81" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="82" spans="1:7">
       <c r="A82" t="str">
         <v>Data.2018-07-09T21:09:00Z</v>
       </c>
@@ -3850,8 +4614,17 @@
         <f>_xll.JsonLookup($A$1,A82)</f>
         <v>6697.4440000000004</v>
       </c>
-    </row>
-    <row r="83" spans="1:3">
+      <c r="E82" t="str">
+        <v>2018-07-09T21:09:00Z</v>
+      </c>
+      <c r="F82">
+        <v>6697.4440000000004</v>
+      </c>
+      <c r="G82" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="83" spans="1:7">
       <c r="A83" t="str">
         <v>Data.2018-07-09T21:10:00Z</v>
       </c>
@@ -3862,8 +4635,17 @@
         <f>_xll.JsonLookup($A$1,A83)</f>
         <v>6697.62</v>
       </c>
-    </row>
-    <row r="84" spans="1:3">
+      <c r="E83" t="str">
+        <v>2018-07-09T21:10:00Z</v>
+      </c>
+      <c r="F83">
+        <v>6697.62</v>
+      </c>
+      <c r="G83" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="84" spans="1:7">
       <c r="A84" t="str">
         <v>Data.2018-07-09T21:11:00Z</v>
       </c>
@@ -3874,8 +4656,17 @@
         <f>_xll.JsonLookup($A$1,A84)</f>
         <v>6697.6189999999997</v>
       </c>
-    </row>
-    <row r="85" spans="1:3">
+      <c r="E84" t="str">
+        <v>2018-07-09T21:11:00Z</v>
+      </c>
+      <c r="F84">
+        <v>6697.6189999999997</v>
+      </c>
+      <c r="G84" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="85" spans="1:7">
       <c r="A85" t="str">
         <v>Data.2018-07-09T21:12:00Z</v>
       </c>
@@ -3886,8 +4677,17 @@
         <f>_xll.JsonLookup($A$1,A85)</f>
         <v>6697.6419999999998</v>
       </c>
-    </row>
-    <row r="86" spans="1:3">
+      <c r="E85" t="str">
+        <v>2018-07-09T21:12:00Z</v>
+      </c>
+      <c r="F85">
+        <v>6697.6419999999998</v>
+      </c>
+      <c r="G85" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="86" spans="1:7">
       <c r="A86" t="str">
         <v>Data.2018-07-09T21:13:00Z</v>
       </c>
@@ -3898,8 +4698,17 @@
         <f>_xll.JsonLookup($A$1,A86)</f>
         <v>6697.6040000000003</v>
       </c>
-    </row>
-    <row r="87" spans="1:3">
+      <c r="E86" t="str">
+        <v>2018-07-09T21:13:00Z</v>
+      </c>
+      <c r="F86">
+        <v>6697.6040000000003</v>
+      </c>
+      <c r="G86" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="87" spans="1:7">
       <c r="A87" t="str">
         <v>Data.2018-07-09T21:14:00Z</v>
       </c>
@@ -3910,8 +4719,17 @@
         <f>_xll.JsonLookup($A$1,A87)</f>
         <v>6697.5649999999996</v>
       </c>
-    </row>
-    <row r="88" spans="1:3">
+      <c r="E87" t="str">
+        <v>2018-07-09T21:14:00Z</v>
+      </c>
+      <c r="F87">
+        <v>6697.5649999999996</v>
+      </c>
+      <c r="G87" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="88" spans="1:7">
       <c r="A88" t="str">
         <v>Data.2018-07-09T21:15:00Z</v>
       </c>
@@ -3922,8 +4740,17 @@
         <f>_xll.JsonLookup($A$1,A88)</f>
         <v>6698.0389999999998</v>
       </c>
-    </row>
-    <row r="89" spans="1:3">
+      <c r="E88" t="str">
+        <v>2018-07-09T21:15:00Z</v>
+      </c>
+      <c r="F88">
+        <v>6698.0389999999998</v>
+      </c>
+      <c r="G88" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="89" spans="1:7">
       <c r="A89" t="str">
         <v>Data.2018-07-09T21:16:00Z</v>
       </c>
@@ -3934,8 +4761,17 @@
         <f>_xll.JsonLookup($A$1,A89)</f>
         <v>6698.2290000000003</v>
       </c>
-    </row>
-    <row r="90" spans="1:3">
+      <c r="E89" t="str">
+        <v>2018-07-09T21:16:00Z</v>
+      </c>
+      <c r="F89">
+        <v>6698.2290000000003</v>
+      </c>
+      <c r="G89" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="90" spans="1:7">
       <c r="A90" t="str">
         <v>Data.2018-07-09T21:17:00Z</v>
       </c>
@@ -3946,8 +4782,17 @@
         <f>_xll.JsonLookup($A$1,A90)</f>
         <v>6698.1580000000004</v>
       </c>
-    </row>
-    <row r="91" spans="1:3">
+      <c r="E90" t="str">
+        <v>2018-07-09T21:17:00Z</v>
+      </c>
+      <c r="F90">
+        <v>6698.1580000000004</v>
+      </c>
+      <c r="G90" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="91" spans="1:7">
       <c r="A91" t="str">
         <v>Data.2018-07-09T21:18:00Z</v>
       </c>
@@ -3958,8 +4803,17 @@
         <f>_xll.JsonLookup($A$1,A91)</f>
         <v>6697.9949999999999</v>
       </c>
-    </row>
-    <row r="92" spans="1:3">
+      <c r="E91" t="str">
+        <v>2018-07-09T21:18:00Z</v>
+      </c>
+      <c r="F91">
+        <v>6697.9949999999999</v>
+      </c>
+      <c r="G91" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="92" spans="1:7">
       <c r="A92" t="str">
         <v>Data.2018-07-09T21:19:00Z</v>
       </c>
@@ -3970,8 +4824,17 @@
         <f>_xll.JsonLookup($A$1,A92)</f>
         <v>6698.0770000000002</v>
       </c>
-    </row>
-    <row r="93" spans="1:3">
+      <c r="E92" t="str">
+        <v>2018-07-09T21:19:00Z</v>
+      </c>
+      <c r="F92">
+        <v>6698.0770000000002</v>
+      </c>
+      <c r="G92" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="93" spans="1:7">
       <c r="A93" t="str">
         <v>Data.2018-07-09T21:20:00Z</v>
       </c>
@@ -3982,8 +4845,17 @@
         <f>_xll.JsonLookup($A$1,A93)</f>
         <v>6698.174</v>
       </c>
-    </row>
-    <row r="94" spans="1:3">
+      <c r="E93" t="str">
+        <v>2018-07-09T21:20:00Z</v>
+      </c>
+      <c r="F93">
+        <v>6698.174</v>
+      </c>
+      <c r="G93" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="94" spans="1:7">
       <c r="A94" t="str">
         <v>Data.2018-07-09T21:21:00Z</v>
       </c>
@@ -3994,8 +4866,17 @@
         <f>_xll.JsonLookup($A$1,A94)</f>
         <v>6698.5739999999996</v>
       </c>
-    </row>
-    <row r="95" spans="1:3">
+      <c r="E94" t="str">
+        <v>2018-07-09T21:21:00Z</v>
+      </c>
+      <c r="F94">
+        <v>6698.5739999999996</v>
+      </c>
+      <c r="G94" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="95" spans="1:7">
       <c r="A95" t="str">
         <v>Data.2018-07-09T21:22:00Z</v>
       </c>
@@ -4006,8 +4887,17 @@
         <f>_xll.JsonLookup($A$1,A95)</f>
         <v>6699.3969999999999</v>
       </c>
-    </row>
-    <row r="96" spans="1:3">
+      <c r="E95" t="str">
+        <v>2018-07-09T21:22:00Z</v>
+      </c>
+      <c r="F95">
+        <v>6699.3969999999999</v>
+      </c>
+      <c r="G95" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="96" spans="1:7">
       <c r="A96" t="str">
         <v>Data.2018-07-09T21:23:00Z</v>
       </c>
@@ -4018,8 +4908,17 @@
         <f>_xll.JsonLookup($A$1,A96)</f>
         <v>6700.549</v>
       </c>
-    </row>
-    <row r="97" spans="1:3">
+      <c r="E96" t="str">
+        <v>2018-07-09T21:23:00Z</v>
+      </c>
+      <c r="F96">
+        <v>6700.549</v>
+      </c>
+      <c r="G96" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="97" spans="1:7">
       <c r="A97" t="str">
         <v>Data.2018-07-09T21:24:00Z</v>
       </c>
@@ -4030,8 +4929,17 @@
         <f>_xll.JsonLookup($A$1,A97)</f>
         <v>6701.6329999999998</v>
       </c>
-    </row>
-    <row r="98" spans="1:3">
+      <c r="E97" t="str">
+        <v>2018-07-09T21:24:00Z</v>
+      </c>
+      <c r="F97">
+        <v>6701.6329999999998</v>
+      </c>
+      <c r="G97" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="98" spans="1:7">
       <c r="A98" t="str">
         <v>Data.2018-07-09T21:25:00Z</v>
       </c>
@@ -4042,8 +4950,17 @@
         <f>_xll.JsonLookup($A$1,A98)</f>
         <v>6702.4409999999998</v>
       </c>
-    </row>
-    <row r="99" spans="1:3">
+      <c r="E98" t="str">
+        <v>2018-07-09T21:25:00Z</v>
+      </c>
+      <c r="F98">
+        <v>6702.4409999999998</v>
+      </c>
+      <c r="G98" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="99" spans="1:7">
       <c r="A99" t="str">
         <v>Data.2018-07-09T21:26:00Z</v>
       </c>
@@ -4054,8 +4971,17 @@
         <f>_xll.JsonLookup($A$1,A99)</f>
         <v>6703.5540000000001</v>
       </c>
-    </row>
-    <row r="100" spans="1:3">
+      <c r="E99" t="str">
+        <v>2018-07-09T21:26:00Z</v>
+      </c>
+      <c r="F99">
+        <v>6703.5540000000001</v>
+      </c>
+      <c r="G99" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="100" spans="1:7">
       <c r="A100" t="str">
         <v>Data.2018-07-09T21:27:00Z</v>
       </c>
@@ -4066,8 +4992,17 @@
         <f>_xll.JsonLookup($A$1,A100)</f>
         <v>6704.6670000000004</v>
       </c>
-    </row>
-    <row r="101" spans="1:3">
+      <c r="E100" t="str">
+        <v>2018-07-09T21:27:00Z</v>
+      </c>
+      <c r="F100">
+        <v>6704.6670000000004</v>
+      </c>
+      <c r="G100" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="101" spans="1:7">
       <c r="A101" t="str">
         <v>Data.2018-07-09T21:28:00Z</v>
       </c>
@@ -4078,8 +5013,17 @@
         <f>_xll.JsonLookup($A$1,A101)</f>
         <v>6705.6379999999999</v>
       </c>
-    </row>
-    <row r="102" spans="1:3">
+      <c r="E101" t="str">
+        <v>2018-07-09T21:28:00Z</v>
+      </c>
+      <c r="F101">
+        <v>6705.6379999999999</v>
+      </c>
+      <c r="G101" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="102" spans="1:7">
       <c r="A102" t="str">
         <v>Data.2018-07-09T21:29:00Z</v>
       </c>
@@ -4090,8 +5034,17 @@
         <f>_xll.JsonLookup($A$1,A102)</f>
         <v>6706.43</v>
       </c>
-    </row>
-    <row r="103" spans="1:3">
+      <c r="E102" t="str">
+        <v>2018-07-09T21:29:00Z</v>
+      </c>
+      <c r="F102">
+        <v>6706.43</v>
+      </c>
+      <c r="G102" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="103" spans="1:7">
       <c r="A103" t="str">
         <v>Inputs.PERIOD</v>
       </c>
@@ -4103,7 +5056,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="104" spans="1:3">
+    <row r="104" spans="1:7">
       <c r="A104" t="str">
         <v>ModelStartTime</v>
       </c>
@@ -4115,7 +5068,7 @@
         <v>1531157418480</v>
       </c>
     </row>
-    <row r="105" spans="1:3">
+    <row r="105" spans="1:7">
       <c r="A105" t="str">
         <v>ModelEndTime</v>
       </c>
@@ -4127,7 +5080,7 @@
         <v>1531157418480</v>
       </c>
     </row>
-    <row r="106" spans="1:3">
+    <row r="106" spans="1:7">
       <c r="A106" t="str">
         <v>Interval</v>
       </c>
@@ -4139,7 +5092,7 @@
         <v>OneMinute</v>
       </c>
     </row>
-    <row r="107" spans="1:3">
+    <row r="107" spans="1:7">
       <c r="A107" t="str">
         <v>Symbol</v>
       </c>
@@ -4151,7 +5104,7 @@
         <v>BTCUSDT</v>
       </c>
     </row>
-    <row r="108" spans="1:3">
+    <row r="108" spans="1:7">
       <c r="A108" t="str">
         <v>Source</v>
       </c>
@@ -4163,7 +5116,7 @@
         <v>BINANCE_KLINE.BTCUSDT.OneMinute</v>
       </c>
     </row>
-    <row r="109" spans="1:3">
+    <row r="109" spans="1:7">
       <c r="A109" t="e">
         <v>#N/A</v>
       </c>
@@ -4175,7 +5128,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="110" spans="1:3">
+    <row r="110" spans="1:7">
       <c r="A110" t="e">
         <v>#N/A</v>
       </c>
@@ -4187,7 +5140,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="111" spans="1:3">
+    <row r="111" spans="1:7">
       <c r="A111" t="e">
         <v>#N/A</v>
       </c>
@@ -4199,7 +5152,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="112" spans="1:3">
+    <row r="112" spans="1:7">
       <c r="A112" t="e">
         <v>#N/A</v>
       </c>
@@ -4804,4 +5757,86 @@
   <pageSetup orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E62A27CD-A10C-46B1-B527-B5F9DD6B5142}">
+  <dimension ref="A1:E7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" t="str">
+        <f t="array" ref="A3:B7">_xll.JsonToArray(A1)</f>
+        <v>[0]</v>
+      </c>
+      <c r="B3" t="str">
+        <v>aaa</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3" t="str">
+        <f>_xll.JsonLookup($A$1,$D3)</f>
+        <v>aaa</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" t="str">
+        <v>[1]</v>
+      </c>
+      <c r="B4" t="str">
+        <v>bbb</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4" t="str">
+        <f>_xll.JsonLookup($A$1,$D4)</f>
+        <v>bbb</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" t="str">
+        <v>[2]</v>
+      </c>
+      <c r="B5" t="str">
+        <v>cccc</v>
+      </c>
+      <c r="D5">
+        <v>2</v>
+      </c>
+      <c r="E5" t="str">
+        <f>_xll.JsonLookup($A$1,$D5)</f>
+        <v>cccc</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="B6" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="B7" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
added Sort2 and Unique array functions they need more work but its a start
</commit_message>
<xml_diff>
--- a/JsonExcel/doc/JsonExcel-test.xlsx
+++ b/JsonExcel/doc/JsonExcel-test.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20325"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="P:\OpenSource\JsonExcel\JsonExcel\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F86B41BD-385A-42A6-9943-DC9975470ED6}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0901D7D6-2A56-4525-B9C9-A454B946830C}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="18885" windowHeight="5910" activeTab="3" xr2:uid="{90F70DC4-6E6D-491C-88DA-FF972DBF519E}"/>
   </bookViews>
@@ -21,7 +21,7 @@
   <definedNames>
     <definedName name="JSON">'Simple Json'!$M$2</definedName>
   </definedNames>
-  <calcPr calcId="179017"/>
+  <calcPr calcId="179021"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -156,7 +156,7 @@
     <t>{"Model":"SMA", "Test": {"k":"v", "k2":"v2"},"TargetTime":"2018-07-09T21:29:00Z","Data":{"2018-07-09T19:56:00Z":6711.49300000,"2018-07-09T19:57:00Z":6711.92000000,"2018-07-09T19:58:00Z":6712.53200000,"2018-07-09T19:59:00Z":6712.43100000,"2018-07-09T20:00:00Z":6711.93400000,"2018-07-09T20:01:00Z":6712.13100000,"2018-07-09T20:02:00Z":6711.98100000,"2018-07-09T20:03:00Z":6711.78100000,"2018-07-09T20:04:00Z":6711.58600000,"2018-07-09T20:05:00Z":6711.13900000,"2018-07-09T20:06:00Z":6710.86200000,"2018-07-09T20:07:00Z":6710.37000000,"2018-07-09T20:08:00Z":6709.85000000,"2018-07-09T20:09:00Z":6709.28700000,"2018-07-09T20:10:00Z":6709.27600000,"2018-07-09T20:11:00Z":6708.48100000,"2018-07-09T20:12:00Z":6707.57700000,"2018-07-09T20:13:00Z":6706.42600000,"2018-07-09T20:14:00Z":6705.26200000,"2018-07-09T20:15:00Z":6704.55500000,"2018-07-09T20:16:00Z":6703.43500000,"2018-07-09T20:17:00Z":6702.49900000,"2018-07-09T20:18:00Z":6701.40600000,"2018-07-09T20:19:00Z":6700.76400000,"2018-07-09T20:20:00Z":6700.17200000,"2018-07-09T20:21:00Z":6700.06800000,"2018-07-09T20:22:00Z":6700.36900000,"2018-07-09T20:23:00Z":6701.09100000,"2018-07-09T20:24:00Z":6701.53800000,"2018-07-09T20:25:00Z":6701.73800000,"2018-07-09T20:26:00Z":6702.11900000,"2018-07-09T20:27:00Z":6702.61900000,"2018-07-09T20:28:00Z":6703.01400000,"2018-07-09T20:29:00Z":6703.00000000,"2018-07-09T20:30:00Z":6702.89900000,"2018-07-09T20:31:00Z":6702.82200000,"2018-07-09T20:32:00Z":6703.14600000,"2018-07-09T20:33:00Z":6702.99600000,"2018-07-09T20:34:00Z":6703.11900000,"2018-07-09T20:35:00Z":6703.50100000,"2018-07-09T20:36:00Z":6703.49700000,"2018-07-09T20:37:00Z":6703.83100000,"2018-07-09T20:38:00Z":6703.92700000,"2018-07-09T20:39:00Z":6704.30700000,"2018-07-09T20:40:00Z":6704.57100000,"2018-07-09T20:41:00Z":6705.04800000,"2018-07-09T20:42:00Z":6704.33200000,"2018-07-09T20:43:00Z":6703.92000000,"2018-07-09T20:44:00Z":6703.68500000,"2018-07-09T20:45:00Z":6703.19000000,"2018-07-09T20:46:00Z":6703.34500000,"2018-07-09T20:47:00Z":6703.20800000,"2018-07-09T20:48:00Z":6703.21800000,"2018-07-09T20:49:00Z":6703.05700000,"2018-07-09T20:50:00Z":6702.83600000,"2018-07-09T20:51:00Z":6702.37900000,"2018-07-09T20:52:00Z":6702.36800000,"2018-07-09T20:53:00Z":6702.28100000,"2018-07-09T20:54:00Z":6702.01700000,"2018-07-09T20:55:00Z":6701.85100000,"2018-07-09T20:56:00Z":6701.26000000,"2018-07-09T20:57:00Z":6700.68400000,"2018-07-09T20:58:00Z":6699.99900000,"2018-07-09T20:59:00Z":6699.60000000,"2018-07-09T21:00:00Z":6699.08700000,"2018-07-09T21:01:00Z":6698.74500000,"2018-07-09T21:02:00Z":6698.44900000,"2018-07-09T21:03:00Z":6698.29100000,"2018-07-09T21:04:00Z":6698.13300000,"2018-07-09T21:05:00Z":6697.73800000,"2018-07-09T21:06:00Z":6697.31900000,"2018-07-09T21:07:00Z":6697.16100000,"2018-07-09T21:08:00Z":6697.44500000,"2018-07-09T21:09:00Z":6697.44400000,"2018-07-09T21:10:00Z":6697.62000000,"2018-07-09T21:11:00Z":6697.61900000,"2018-07-09T21:12:00Z":6697.64200000,"2018-07-09T21:13:00Z":6697.60400000,"2018-07-09T21:14:00Z":6697.56500000,"2018-07-09T21:15:00Z":6698.03900000,"2018-07-09T21:16:00Z":6698.22900000,"2018-07-09T21:17:00Z":6698.15800000,"2018-07-09T21:18:00Z":6697.99500000,"2018-07-09T21:19:00Z":6698.07700000,"2018-07-09T21:20:00Z":6698.17400000,"2018-07-09T21:21:00Z":6698.57400000,"2018-07-09T21:22:00Z":6699.39700000,"2018-07-09T21:23:00Z":6700.54900000,"2018-07-09T21:24:00Z":6701.63300000,"2018-07-09T21:25:00Z":6702.44100000,"2018-07-09T21:26:00Z":6703.55400000,"2018-07-09T21:27:00Z":6704.66700000,"2018-07-09T21:28:00Z":6705.63800000,"2018-07-09T21:29:00Z":6706.43000000},"Inputs":{"PERIOD":10},"ModelStartTime":1531157418480.0,"ModelEndTime":1531157418480.0,"Interval":"OneMinute","Symbol":"BTCUSDT","Source":"BINANCE_KLINE.BTCUSDT.OneMinute"}</t>
   </si>
   <si>
-    <t>["aaa","bbb","cccc"]</t>
+    <t>["aaa","a","a","bbbb","ccc"]</t>
   </si>
 </sst>
 </file>
@@ -1684,7 +1684,7 @@
   <dimension ref="C1:M14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1740,7 +1740,7 @@
       </c>
       <c r="L5" t="str">
         <f>_xll.JsonFromCells(C5:E8)</f>
-        <v>{"aaaa":124.0,"bbb":456.0,"3":789.0}</v>
+        <v>{"aaaa":42,"bbb":42,"3":42,"ExcelErrorNA":42}</v>
       </c>
     </row>
     <row r="6" spans="3:13">
@@ -2941,9 +2941,12 @@
         <f>_xll.JsonLookup($A$1,A6)</f>
         <v>v</v>
       </c>
-      <c r="D6" t="e">
+      <c r="D6" t="str">
         <f>_xll.JsonLookup(A1,"Test")</f>
-        <v>#VALUE!</v>
+        <v>{_x000D_
+  "k": "v",_x000D_
+  "k2": "v2"_x000D_
+}</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -5761,20 +5764,20 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E62A27CD-A10C-46B1-B527-B5F9DD6B5142}">
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:8">
       <c r="A1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:8">
       <c r="A3" t="str">
         <f t="array" ref="A3:B7">_xll.JsonToArray(A1)</f>
         <v>[0]</v>
@@ -5789,51 +5792,83 @@
         <f>_xll.JsonLookup($A$1,$D3)</f>
         <v>aaa</v>
       </c>
-    </row>
-    <row r="4" spans="1:5">
+      <c r="G3" t="str">
+        <f t="array" ref="G3:H6">_xll.Unique(E3:E6)</f>
+        <v>aaa</v>
+      </c>
+      <c r="H3" t="str">
+        <v>aaa</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
       <c r="A4" t="str">
         <v>[1]</v>
       </c>
       <c r="B4" t="str">
-        <v>bbb</v>
+        <v>a</v>
       </c>
       <c r="D4">
         <v>1</v>
       </c>
       <c r="E4" t="str">
         <f>_xll.JsonLookup($A$1,$D4)</f>
-        <v>bbb</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
+        <v>a</v>
+      </c>
+      <c r="G4" t="str">
+        <v>a</v>
+      </c>
+      <c r="H4" t="str">
+        <v>a</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
       <c r="A5" t="str">
         <v>[2]</v>
       </c>
       <c r="B5" t="str">
-        <v>cccc</v>
+        <v>a</v>
       </c>
       <c r="D5">
         <v>2</v>
       </c>
       <c r="E5" t="str">
         <f>_xll.JsonLookup($A$1,$D5)</f>
-        <v>cccc</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5">
-      <c r="A6" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="B6" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5">
-      <c r="A7" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="B7" t="e">
-        <v>#N/A</v>
+        <v>a</v>
+      </c>
+      <c r="G5" t="str">
+        <v>bbbb</v>
+      </c>
+      <c r="H5" t="str">
+        <v>bbbb</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6" t="str">
+        <v>[3]</v>
+      </c>
+      <c r="B6" t="str">
+        <v>bbbb</v>
+      </c>
+      <c r="D6">
+        <v>3</v>
+      </c>
+      <c r="E6" t="str">
+        <f>_xll.JsonLookup($A$1,$D6)</f>
+        <v>bbbb</v>
+      </c>
+      <c r="G6" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="H6" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
+      <c r="A7" t="str">
+        <v>[4]</v>
+      </c>
+      <c r="B7" t="str">
+        <v>ccc</v>
       </c>
     </row>
   </sheetData>

</xml_diff>